<commit_message>
add info about adding some losed point of mesuring
</commit_message>
<xml_diff>
--- a/Documentation/База_данных_Арселор-Точки_измерения.xlsx
+++ b/Documentation/База_данных_Арселор-Точки_измерения.xlsx
@@ -2109,7 +2109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2172,11 +2172,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2186,19 +2184,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2482,7 +2479,7 @@
   <dimension ref="B2:I200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="E50" sqref="E50:E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2532,7 +2529,7 @@
       <c r="G3" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="28" t="s">
         <v>637</v>
       </c>
     </row>
@@ -3388,7 +3385,7 @@
       <c r="D50" s="11">
         <v>48</v>
       </c>
-      <c r="E50" s="32">
+      <c r="E50" s="29">
         <v>10053</v>
       </c>
       <c r="F50" s="11">
@@ -3408,7 +3405,7 @@
       <c r="D51" s="11">
         <v>49</v>
       </c>
-      <c r="E51" s="33"/>
+      <c r="E51" s="34"/>
       <c r="F51" s="11">
         <v>3</v>
       </c>
@@ -3426,7 +3423,7 @@
       <c r="D52" s="11">
         <v>50</v>
       </c>
-      <c r="E52" s="33"/>
+      <c r="E52" s="34"/>
       <c r="F52" s="11">
         <v>3</v>
       </c>
@@ -3444,7 +3441,7 @@
       <c r="D53" s="11">
         <v>51</v>
       </c>
-      <c r="E53" s="33"/>
+      <c r="E53" s="34"/>
       <c r="F53" s="11">
         <v>3</v>
       </c>
@@ -3462,7 +3459,7 @@
       <c r="D54" s="11">
         <v>52</v>
       </c>
-      <c r="E54" s="34"/>
+      <c r="E54" s="35"/>
       <c r="F54" s="11">
         <v>3</v>
       </c>
@@ -3590,7 +3587,7 @@
       <c r="D61" s="11">
         <v>59</v>
       </c>
-      <c r="E61" s="35">
+      <c r="E61" s="27">
         <v>10063</v>
       </c>
       <c r="F61" s="11">
@@ -3610,7 +3607,7 @@
       <c r="D62" s="11">
         <v>60</v>
       </c>
-      <c r="E62" s="35">
+      <c r="E62" s="27">
         <v>10064</v>
       </c>
       <c r="F62" s="11">
@@ -3630,7 +3627,7 @@
       <c r="D63" s="11">
         <v>61</v>
       </c>
-      <c r="E63" s="35">
+      <c r="E63" s="27">
         <v>10065</v>
       </c>
       <c r="F63" s="11">
@@ -3852,7 +3849,7 @@
       <c r="D75" s="11">
         <v>73</v>
       </c>
-      <c r="E75" s="32">
+      <c r="E75" s="29">
         <v>10078</v>
       </c>
       <c r="F75" s="11">
@@ -3872,7 +3869,7 @@
       <c r="D76" s="11">
         <v>74</v>
       </c>
-      <c r="E76" s="33"/>
+      <c r="E76" s="34"/>
       <c r="F76" s="11">
         <v>4</v>
       </c>
@@ -3890,7 +3887,7 @@
       <c r="D77" s="11">
         <v>75</v>
       </c>
-      <c r="E77" s="33"/>
+      <c r="E77" s="34"/>
       <c r="F77" s="11">
         <v>4</v>
       </c>
@@ -3908,7 +3905,7 @@
       <c r="D78" s="11">
         <v>76</v>
       </c>
-      <c r="E78" s="33"/>
+      <c r="E78" s="34"/>
       <c r="F78" s="11">
         <v>4</v>
       </c>
@@ -3926,7 +3923,7 @@
       <c r="D79" s="11">
         <v>77</v>
       </c>
-      <c r="E79" s="34"/>
+      <c r="E79" s="35"/>
       <c r="F79" s="11">
         <v>4</v>
       </c>
@@ -4036,7 +4033,7 @@
       <c r="D85" s="11">
         <v>83</v>
       </c>
-      <c r="E85" s="35">
+      <c r="E85" s="27">
         <v>10088</v>
       </c>
       <c r="F85" s="11">
@@ -4056,7 +4053,7 @@
       <c r="D86" s="11">
         <v>84</v>
       </c>
-      <c r="E86" s="35">
+      <c r="E86" s="27">
         <v>10089</v>
       </c>
       <c r="F86" s="11">
@@ -4076,7 +4073,7 @@
       <c r="D87" s="11">
         <v>85</v>
       </c>
-      <c r="E87" s="35">
+      <c r="E87" s="27">
         <v>10090</v>
       </c>
       <c r="F87" s="11">
@@ -5770,7 +5767,7 @@
       <c r="D179" s="11">
         <v>177</v>
       </c>
-      <c r="E179" s="32">
+      <c r="E179" s="29">
         <v>10181</v>
       </c>
       <c r="F179" s="11">
@@ -5790,7 +5787,7 @@
       <c r="D180" s="11">
         <v>178</v>
       </c>
-      <c r="E180" s="33"/>
+      <c r="E180" s="34"/>
       <c r="F180" s="11">
         <v>11</v>
       </c>
@@ -5808,7 +5805,7 @@
       <c r="D181" s="11">
         <v>179</v>
       </c>
-      <c r="E181" s="33"/>
+      <c r="E181" s="34"/>
       <c r="F181" s="11">
         <v>11</v>
       </c>
@@ -5826,7 +5823,7 @@
       <c r="D182" s="11">
         <v>180</v>
       </c>
-      <c r="E182" s="33"/>
+      <c r="E182" s="34"/>
       <c r="F182" s="11">
         <v>11</v>
       </c>
@@ -5844,7 +5841,7 @@
       <c r="D183" s="11">
         <v>181</v>
       </c>
-      <c r="E183" s="33"/>
+      <c r="E183" s="34"/>
       <c r="F183" s="11">
         <v>11</v>
       </c>
@@ -5862,7 +5859,7 @@
       <c r="D184" s="11">
         <v>182</v>
       </c>
-      <c r="E184" s="34"/>
+      <c r="E184" s="35"/>
       <c r="F184" s="11">
         <v>11</v>
       </c>
@@ -5880,7 +5877,7 @@
       <c r="D185" s="11">
         <v>183</v>
       </c>
-      <c r="E185" s="32">
+      <c r="E185" s="29">
         <v>10182</v>
       </c>
       <c r="F185" s="11">
@@ -5900,7 +5897,7 @@
       <c r="D186" s="11">
         <v>184</v>
       </c>
-      <c r="E186" s="33"/>
+      <c r="E186" s="34"/>
       <c r="F186" s="11">
         <v>11</v>
       </c>
@@ -5918,7 +5915,7 @@
       <c r="D187" s="11">
         <v>185</v>
       </c>
-      <c r="E187" s="33"/>
+      <c r="E187" s="34"/>
       <c r="F187" s="11">
         <v>11</v>
       </c>
@@ -5936,7 +5933,7 @@
       <c r="D188" s="11">
         <v>186</v>
       </c>
-      <c r="E188" s="33"/>
+      <c r="E188" s="34"/>
       <c r="F188" s="11">
         <v>11</v>
       </c>
@@ -5954,7 +5951,7 @@
       <c r="D189" s="11">
         <v>187</v>
       </c>
-      <c r="E189" s="34"/>
+      <c r="E189" s="35"/>
       <c r="F189" s="11">
         <v>11</v>
       </c>
@@ -6166,16 +6163,23 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="E173:E178"/>
-    <mergeCell ref="E179:E184"/>
-    <mergeCell ref="E185:E189"/>
-    <mergeCell ref="E190:E194"/>
-    <mergeCell ref="E195:E200"/>
-    <mergeCell ref="E136:E140"/>
-    <mergeCell ref="E143:E148"/>
-    <mergeCell ref="E149:E154"/>
-    <mergeCell ref="E155:E160"/>
-    <mergeCell ref="E161:E166"/>
+    <mergeCell ref="E3:E8"/>
+    <mergeCell ref="E9:E14"/>
+    <mergeCell ref="E15:E20"/>
+    <mergeCell ref="E21:E26"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="E99:E104"/>
+    <mergeCell ref="E33:E38"/>
+    <mergeCell ref="E39:E44"/>
+    <mergeCell ref="E45:E49"/>
+    <mergeCell ref="E50:E54"/>
+    <mergeCell ref="E55:E60"/>
+    <mergeCell ref="E64:E69"/>
+    <mergeCell ref="E70:E74"/>
+    <mergeCell ref="E75:E79"/>
+    <mergeCell ref="E80:E84"/>
+    <mergeCell ref="E88:E93"/>
+    <mergeCell ref="E94:E98"/>
     <mergeCell ref="E167:E172"/>
     <mergeCell ref="E105:E109"/>
     <mergeCell ref="E110:E113"/>
@@ -6183,23 +6187,16 @@
     <mergeCell ref="E118:E123"/>
     <mergeCell ref="E124:E129"/>
     <mergeCell ref="E130:E135"/>
-    <mergeCell ref="E70:E74"/>
-    <mergeCell ref="E75:E79"/>
-    <mergeCell ref="E80:E84"/>
-    <mergeCell ref="E88:E93"/>
-    <mergeCell ref="E94:E98"/>
-    <mergeCell ref="E99:E104"/>
-    <mergeCell ref="E33:E38"/>
-    <mergeCell ref="E39:E44"/>
-    <mergeCell ref="E45:E49"/>
-    <mergeCell ref="E50:E54"/>
-    <mergeCell ref="E55:E60"/>
-    <mergeCell ref="E64:E69"/>
-    <mergeCell ref="E3:E8"/>
-    <mergeCell ref="E9:E14"/>
-    <mergeCell ref="E15:E20"/>
-    <mergeCell ref="E21:E26"/>
-    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="E136:E140"/>
+    <mergeCell ref="E143:E148"/>
+    <mergeCell ref="E149:E154"/>
+    <mergeCell ref="E155:E160"/>
+    <mergeCell ref="E161:E166"/>
+    <mergeCell ref="E173:E178"/>
+    <mergeCell ref="E179:E184"/>
+    <mergeCell ref="E185:E189"/>
+    <mergeCell ref="E190:E194"/>
+    <mergeCell ref="E195:E200"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -6286,7 +6283,7 @@
       <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="33" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="6" t="s">
@@ -6309,7 +6306,7 @@
       <c r="C5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="28"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="6" t="s">
         <v>20</v>
       </c>
@@ -6330,7 +6327,7 @@
       <c r="C6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="28"/>
+      <c r="D6" s="33"/>
       <c r="E6" s="6" t="s">
         <v>25</v>
       </c>
@@ -6351,7 +6348,7 @@
       <c r="C7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="28"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="6" t="s">
         <v>30</v>
       </c>
@@ -6372,7 +6369,7 @@
       <c r="C8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="28"/>
+      <c r="D8" s="33"/>
       <c r="E8" s="6" t="s">
         <v>35</v>
       </c>
@@ -6393,7 +6390,7 @@
       <c r="C9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="33" t="s">
         <v>40</v>
       </c>
       <c r="E9" s="6" t="s">
@@ -6416,7 +6413,7 @@
       <c r="C10" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="28"/>
+      <c r="D10" s="33"/>
       <c r="E10" s="6" t="s">
         <v>46</v>
       </c>
@@ -6437,7 +6434,7 @@
       <c r="C11" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="28"/>
+      <c r="D11" s="33"/>
       <c r="E11" s="6" t="s">
         <v>51</v>
       </c>
@@ -6458,7 +6455,7 @@
       <c r="C12" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="28"/>
+      <c r="D12" s="33"/>
       <c r="E12" s="6" t="s">
         <v>55</v>
       </c>
@@ -6479,7 +6476,7 @@
       <c r="C13" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="28"/>
+      <c r="D13" s="33"/>
       <c r="E13" s="6" t="s">
         <v>48</v>
       </c>
@@ -6500,7 +6497,7 @@
       <c r="C14" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="28"/>
+      <c r="D14" s="33"/>
       <c r="E14" s="6" t="s">
         <v>48</v>
       </c>
@@ -6521,7 +6518,7 @@
       <c r="C15" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="28"/>
+      <c r="D15" s="33"/>
       <c r="E15" s="6" t="s">
         <v>48</v>
       </c>
@@ -6542,7 +6539,7 @@
       <c r="C16" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="33" t="s">
         <v>66</v>
       </c>
       <c r="E16" s="6" t="s">
@@ -6565,7 +6562,7 @@
       <c r="C17" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="28"/>
+      <c r="D17" s="33"/>
       <c r="E17" s="6" t="s">
         <v>72</v>
       </c>
@@ -6586,7 +6583,7 @@
       <c r="C18" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="28"/>
+      <c r="D18" s="33"/>
       <c r="E18" s="6" t="s">
         <v>76</v>
       </c>
@@ -6607,7 +6604,7 @@
       <c r="C19" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="28"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="6" t="s">
         <v>80</v>
       </c>
@@ -6628,7 +6625,7 @@
       <c r="C20" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="28"/>
+      <c r="D20" s="33"/>
       <c r="E20" s="6" t="s">
         <v>48</v>
       </c>
@@ -6649,7 +6646,7 @@
       <c r="C21" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="28"/>
+      <c r="D21" s="33"/>
       <c r="E21" s="6" t="s">
         <v>48</v>
       </c>
@@ -6670,7 +6667,7 @@
       <c r="C22" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="28"/>
+      <c r="D22" s="33"/>
       <c r="E22" s="6" t="s">
         <v>48</v>
       </c>
@@ -6691,7 +6688,7 @@
       <c r="C23" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="33" t="s">
         <v>90</v>
       </c>
       <c r="E23" s="6" t="s">
@@ -6714,7 +6711,7 @@
       <c r="C24" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="28"/>
+      <c r="D24" s="33"/>
       <c r="E24" s="6" t="s">
         <v>96</v>
       </c>
@@ -6735,7 +6732,7 @@
       <c r="C25" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="28"/>
+      <c r="D25" s="33"/>
       <c r="E25" s="6" t="s">
         <v>100</v>
       </c>
@@ -6756,7 +6753,7 @@
       <c r="C26" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="28"/>
+      <c r="D26" s="33"/>
       <c r="E26" s="6" t="s">
         <v>48</v>
       </c>
@@ -6777,7 +6774,7 @@
       <c r="C27" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="32" t="s">
         <v>107</v>
       </c>
       <c r="E27" s="6" t="s">
@@ -6800,7 +6797,7 @@
       <c r="C28" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D28" s="28"/>
+      <c r="D28" s="33"/>
       <c r="E28" s="6" t="s">
         <v>112</v>
       </c>
@@ -6821,7 +6818,7 @@
       <c r="C29" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="D29" s="28"/>
+      <c r="D29" s="33"/>
       <c r="E29" s="6" t="s">
         <v>116</v>
       </c>
@@ -6842,7 +6839,7 @@
       <c r="C30" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D30" s="28"/>
+      <c r="D30" s="33"/>
       <c r="E30" s="6" t="s">
         <v>120</v>
       </c>
@@ -6863,7 +6860,7 @@
       <c r="C31" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D31" s="28"/>
+      <c r="D31" s="33"/>
       <c r="E31" s="6" t="s">
         <v>125</v>
       </c>
@@ -6884,7 +6881,7 @@
       <c r="C32" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="D32" s="28"/>
+      <c r="D32" s="33"/>
       <c r="E32" s="6" t="s">
         <v>130</v>
       </c>
@@ -6905,7 +6902,7 @@
       <c r="C33" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="D33" s="28"/>
+      <c r="D33" s="33"/>
       <c r="E33" s="6" t="s">
         <v>135</v>
       </c>
@@ -6926,7 +6923,7 @@
       <c r="C34" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D34" s="28"/>
+      <c r="D34" s="33"/>
       <c r="E34" s="6" t="s">
         <v>140</v>
       </c>
@@ -6947,7 +6944,7 @@
       <c r="C35" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D35" s="28"/>
+      <c r="D35" s="33"/>
       <c r="E35" s="6" t="s">
         <v>145</v>
       </c>
@@ -6968,7 +6965,7 @@
       <c r="C36" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D36" s="28"/>
+      <c r="D36" s="33"/>
       <c r="E36" s="6" t="s">
         <v>150</v>
       </c>
@@ -6989,7 +6986,7 @@
       <c r="C37" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D37" s="28"/>
+      <c r="D37" s="33"/>
       <c r="E37" s="6" t="s">
         <v>151</v>
       </c>
@@ -7010,7 +7007,7 @@
       <c r="C38" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="D38" s="27" t="s">
+      <c r="D38" s="32" t="s">
         <v>153</v>
       </c>
       <c r="E38" s="6" t="s">
@@ -7033,7 +7030,7 @@
       <c r="C39" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D39" s="28"/>
+      <c r="D39" s="33"/>
       <c r="E39" s="6" t="s">
         <v>159</v>
       </c>
@@ -7054,7 +7051,7 @@
       <c r="C40" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="D40" s="28"/>
+      <c r="D40" s="33"/>
       <c r="E40" s="6" t="s">
         <v>164</v>
       </c>
@@ -7075,7 +7072,7 @@
       <c r="C41" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D41" s="28"/>
+      <c r="D41" s="33"/>
       <c r="E41" s="6" t="s">
         <v>168</v>
       </c>
@@ -7096,7 +7093,7 @@
       <c r="C42" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="D42" s="27" t="s">
+      <c r="D42" s="32" t="s">
         <v>172</v>
       </c>
       <c r="E42" s="6" t="s">
@@ -7119,7 +7116,7 @@
       <c r="C43" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D43" s="28"/>
+      <c r="D43" s="33"/>
       <c r="E43" s="6" t="s">
         <v>178</v>
       </c>
@@ -7140,7 +7137,7 @@
       <c r="C44" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D44" s="28"/>
+      <c r="D44" s="33"/>
       <c r="E44" s="6" t="s">
         <v>182</v>
       </c>
@@ -7161,7 +7158,7 @@
       <c r="C45" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D45" s="28"/>
+      <c r="D45" s="33"/>
       <c r="E45" s="7" t="s">
         <v>186</v>
       </c>

</xml_diff>

<commit_message>
add ID for aditional points of measurement
</commit_message>
<xml_diff>
--- a/Documentation/База_данных_Арселор-Точки_измерения.xlsx
+++ b/Documentation/База_данных_Арселор-Точки_измерения.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\prj_ASU\AMKP\git\gasCollectionPrj\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\AMKP\.git\gasCollectionPrj\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="665">
   <si>
     <t>№</t>
   </si>
@@ -1979,6 +1979,60 @@
   </si>
   <si>
     <t>Давление кислорода на газодувки цеха компрессии №1</t>
+  </si>
+  <si>
+    <t>PE_3_29</t>
+  </si>
+  <si>
+    <t>TE_3_27</t>
+  </si>
+  <si>
+    <t>FE_3_27</t>
+  </si>
+  <si>
+    <t>FE_3_27_norm</t>
+  </si>
+  <si>
+    <t>FE_3_27_normQ</t>
+  </si>
+  <si>
+    <t>Кислород на мартеновское поизводство</t>
+  </si>
+  <si>
+    <t>Кислород Сброс с Кар-30М1 №7</t>
+  </si>
+  <si>
+    <t>PE_3_26</t>
+  </si>
+  <si>
+    <t>TE_3_24</t>
+  </si>
+  <si>
+    <t>FE_3_24</t>
+  </si>
+  <si>
+    <t>FE_3_24_norm</t>
+  </si>
+  <si>
+    <t>FE_3_24_normQ</t>
+  </si>
+  <si>
+    <t>Кислород Сброс с АКАр-40/35 №2</t>
+  </si>
+  <si>
+    <t>PE_3_27</t>
+  </si>
+  <si>
+    <t>TE_3_25</t>
+  </si>
+  <si>
+    <t>FE_3_25</t>
+  </si>
+  <si>
+    <t>FE_3_25_norm</t>
+  </si>
+  <si>
+    <t>FE_3_25_normQ</t>
   </si>
 </sst>
 </file>
@@ -2252,16 +2306,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2556,10 +2610,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:G212"/>
+  <dimension ref="B2:G227"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B208" sqref="B208:B212"/>
+    <sheetView tabSelected="1" topLeftCell="A160" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G198" sqref="G198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2732,7 +2786,7 @@
       <c r="D10" s="10">
         <v>8</v>
       </c>
-      <c r="E10" s="41"/>
+      <c r="E10" s="43"/>
       <c r="F10" s="10">
         <v>2</v>
       </c>
@@ -2750,7 +2804,7 @@
       <c r="D11" s="10">
         <v>9</v>
       </c>
-      <c r="E11" s="41"/>
+      <c r="E11" s="43"/>
       <c r="F11" s="10">
         <v>2</v>
       </c>
@@ -2768,7 +2822,7 @@
       <c r="D12" s="10">
         <v>10</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="43"/>
       <c r="F12" s="10">
         <v>2</v>
       </c>
@@ -2786,7 +2840,7 @@
       <c r="D13" s="10">
         <v>11</v>
       </c>
-      <c r="E13" s="41"/>
+      <c r="E13" s="43"/>
       <c r="F13" s="10">
         <v>2</v>
       </c>
@@ -2804,7 +2858,7 @@
       <c r="D14" s="10">
         <v>12</v>
       </c>
-      <c r="E14" s="42"/>
+      <c r="E14" s="44"/>
       <c r="F14" s="10">
         <v>2</v>
       </c>
@@ -2842,7 +2896,7 @@
       <c r="D16" s="10">
         <v>14</v>
       </c>
-      <c r="E16" s="41"/>
+      <c r="E16" s="43"/>
       <c r="F16" s="10">
         <v>2</v>
       </c>
@@ -2860,7 +2914,7 @@
       <c r="D17" s="10">
         <v>15</v>
       </c>
-      <c r="E17" s="41"/>
+      <c r="E17" s="43"/>
       <c r="F17" s="10">
         <v>2</v>
       </c>
@@ -2878,7 +2932,7 @@
       <c r="D18" s="10">
         <v>16</v>
       </c>
-      <c r="E18" s="41"/>
+      <c r="E18" s="43"/>
       <c r="F18" s="10">
         <v>2</v>
       </c>
@@ -2896,7 +2950,7 @@
       <c r="D19" s="10">
         <v>17</v>
       </c>
-      <c r="E19" s="41"/>
+      <c r="E19" s="43"/>
       <c r="F19" s="10">
         <v>2</v>
       </c>
@@ -2914,7 +2968,7 @@
       <c r="D20" s="10">
         <v>18</v>
       </c>
-      <c r="E20" s="42"/>
+      <c r="E20" s="44"/>
       <c r="F20" s="10">
         <v>2</v>
       </c>
@@ -2952,7 +3006,7 @@
       <c r="D22" s="10">
         <v>20</v>
       </c>
-      <c r="E22" s="41"/>
+      <c r="E22" s="43"/>
       <c r="F22" s="10">
         <v>2</v>
       </c>
@@ -2970,7 +3024,7 @@
       <c r="D23" s="10">
         <v>21</v>
       </c>
-      <c r="E23" s="41"/>
+      <c r="E23" s="43"/>
       <c r="F23" s="10">
         <v>2</v>
       </c>
@@ -2988,7 +3042,7 @@
       <c r="D24" s="10">
         <v>22</v>
       </c>
-      <c r="E24" s="41"/>
+      <c r="E24" s="43"/>
       <c r="F24" s="10">
         <v>2</v>
       </c>
@@ -3006,7 +3060,7 @@
       <c r="D25" s="10">
         <v>23</v>
       </c>
-      <c r="E25" s="41"/>
+      <c r="E25" s="43"/>
       <c r="F25" s="10">
         <v>2</v>
       </c>
@@ -3024,7 +3078,7 @@
       <c r="D26" s="10">
         <v>24</v>
       </c>
-      <c r="E26" s="42"/>
+      <c r="E26" s="44"/>
       <c r="F26" s="10">
         <v>2</v>
       </c>
@@ -3062,7 +3116,7 @@
       <c r="D28" s="10">
         <v>26</v>
       </c>
-      <c r="E28" s="41"/>
+      <c r="E28" s="43"/>
       <c r="F28" s="10">
         <v>2</v>
       </c>
@@ -3080,7 +3134,7 @@
       <c r="D29" s="10">
         <v>27</v>
       </c>
-      <c r="E29" s="41"/>
+      <c r="E29" s="43"/>
       <c r="F29" s="10">
         <v>2</v>
       </c>
@@ -3098,7 +3152,7 @@
       <c r="D30" s="10">
         <v>28</v>
       </c>
-      <c r="E30" s="41"/>
+      <c r="E30" s="43"/>
       <c r="F30" s="10">
         <v>2</v>
       </c>
@@ -3116,7 +3170,7 @@
       <c r="D31" s="10">
         <v>29</v>
       </c>
-      <c r="E31" s="41"/>
+      <c r="E31" s="43"/>
       <c r="F31" s="10">
         <v>2</v>
       </c>
@@ -3134,7 +3188,7 @@
       <c r="D32" s="10">
         <v>30</v>
       </c>
-      <c r="E32" s="42"/>
+      <c r="E32" s="44"/>
       <c r="F32" s="10">
         <v>2</v>
       </c>
@@ -3172,7 +3226,7 @@
       <c r="D34" s="10">
         <v>32</v>
       </c>
-      <c r="E34" s="41"/>
+      <c r="E34" s="43"/>
       <c r="F34" s="10">
         <v>2</v>
       </c>
@@ -3190,7 +3244,7 @@
       <c r="D35" s="10">
         <v>33</v>
       </c>
-      <c r="E35" s="41"/>
+      <c r="E35" s="43"/>
       <c r="F35" s="10">
         <v>2</v>
       </c>
@@ -3208,7 +3262,7 @@
       <c r="D36" s="10">
         <v>34</v>
       </c>
-      <c r="E36" s="41"/>
+      <c r="E36" s="43"/>
       <c r="F36" s="10">
         <v>2</v>
       </c>
@@ -3226,7 +3280,7 @@
       <c r="D37" s="10">
         <v>35</v>
       </c>
-      <c r="E37" s="41"/>
+      <c r="E37" s="43"/>
       <c r="F37" s="10">
         <v>2</v>
       </c>
@@ -3244,7 +3298,7 @@
       <c r="D38" s="10">
         <v>36</v>
       </c>
-      <c r="E38" s="42"/>
+      <c r="E38" s="44"/>
       <c r="F38" s="10">
         <v>2</v>
       </c>
@@ -3282,7 +3336,7 @@
       <c r="D40" s="10">
         <v>38</v>
       </c>
-      <c r="E40" s="41"/>
+      <c r="E40" s="43"/>
       <c r="F40" s="10">
         <v>3</v>
       </c>
@@ -3300,7 +3354,7 @@
       <c r="D41" s="10">
         <v>39</v>
       </c>
-      <c r="E41" s="41"/>
+      <c r="E41" s="43"/>
       <c r="F41" s="10">
         <v>3</v>
       </c>
@@ -3318,7 +3372,7 @@
       <c r="D42" s="10">
         <v>40</v>
       </c>
-      <c r="E42" s="41"/>
+      <c r="E42" s="43"/>
       <c r="F42" s="10">
         <v>3</v>
       </c>
@@ -3336,7 +3390,7 @@
       <c r="D43" s="10">
         <v>41</v>
       </c>
-      <c r="E43" s="41"/>
+      <c r="E43" s="43"/>
       <c r="F43" s="10">
         <v>3</v>
       </c>
@@ -3354,7 +3408,7 @@
       <c r="D44" s="10">
         <v>42</v>
       </c>
-      <c r="E44" s="42"/>
+      <c r="E44" s="44"/>
       <c r="F44" s="10">
         <v>3</v>
       </c>
@@ -3392,7 +3446,7 @@
       <c r="D46" s="10">
         <v>44</v>
       </c>
-      <c r="E46" s="41"/>
+      <c r="E46" s="43"/>
       <c r="F46" s="10">
         <v>3</v>
       </c>
@@ -3410,7 +3464,7 @@
       <c r="D47" s="10">
         <v>45</v>
       </c>
-      <c r="E47" s="41"/>
+      <c r="E47" s="43"/>
       <c r="F47" s="10">
         <v>3</v>
       </c>
@@ -3428,7 +3482,7 @@
       <c r="D48" s="10">
         <v>46</v>
       </c>
-      <c r="E48" s="41"/>
+      <c r="E48" s="43"/>
       <c r="F48" s="10">
         <v>3</v>
       </c>
@@ -3446,7 +3500,7 @@
       <c r="D49" s="10">
         <v>47</v>
       </c>
-      <c r="E49" s="42"/>
+      <c r="E49" s="44"/>
       <c r="F49" s="10">
         <v>3</v>
       </c>
@@ -3484,7 +3538,7 @@
       <c r="D51" s="10">
         <v>49</v>
       </c>
-      <c r="E51" s="43"/>
+      <c r="E51" s="41"/>
       <c r="F51" s="10">
         <v>3</v>
       </c>
@@ -3502,7 +3556,7 @@
       <c r="D52" s="10">
         <v>50</v>
       </c>
-      <c r="E52" s="43"/>
+      <c r="E52" s="41"/>
       <c r="F52" s="10">
         <v>3</v>
       </c>
@@ -3520,7 +3574,7 @@
       <c r="D53" s="10">
         <v>51</v>
       </c>
-      <c r="E53" s="43"/>
+      <c r="E53" s="41"/>
       <c r="F53" s="10">
         <v>3</v>
       </c>
@@ -3538,7 +3592,7 @@
       <c r="D54" s="10">
         <v>52</v>
       </c>
-      <c r="E54" s="44"/>
+      <c r="E54" s="42"/>
       <c r="F54" s="10">
         <v>3</v>
       </c>
@@ -3576,7 +3630,7 @@
       <c r="D56" s="10">
         <v>54</v>
       </c>
-      <c r="E56" s="41"/>
+      <c r="E56" s="43"/>
       <c r="F56" s="10">
         <v>3</v>
       </c>
@@ -3594,7 +3648,7 @@
       <c r="D57" s="10">
         <v>55</v>
       </c>
-      <c r="E57" s="41"/>
+      <c r="E57" s="43"/>
       <c r="F57" s="10">
         <v>3</v>
       </c>
@@ -3612,7 +3666,7 @@
       <c r="D58" s="10">
         <v>56</v>
       </c>
-      <c r="E58" s="41"/>
+      <c r="E58" s="43"/>
       <c r="F58" s="10">
         <v>3</v>
       </c>
@@ -3630,7 +3684,7 @@
       <c r="D59" s="10">
         <v>57</v>
       </c>
-      <c r="E59" s="41"/>
+      <c r="E59" s="43"/>
       <c r="F59" s="10">
         <v>3</v>
       </c>
@@ -3648,7 +3702,7 @@
       <c r="D60" s="10">
         <v>58</v>
       </c>
-      <c r="E60" s="42"/>
+      <c r="E60" s="44"/>
       <c r="F60" s="10">
         <v>3</v>
       </c>
@@ -4192,7 +4246,7 @@
       <c r="D89" s="10">
         <v>87</v>
       </c>
-      <c r="E89" s="41"/>
+      <c r="E89" s="43"/>
       <c r="F89" s="10">
         <v>5</v>
       </c>
@@ -4210,7 +4264,7 @@
       <c r="D90" s="10">
         <v>88</v>
       </c>
-      <c r="E90" s="41"/>
+      <c r="E90" s="43"/>
       <c r="F90" s="10">
         <v>5</v>
       </c>
@@ -4228,7 +4282,7 @@
       <c r="D91" s="10">
         <v>89</v>
       </c>
-      <c r="E91" s="41"/>
+      <c r="E91" s="43"/>
       <c r="F91" s="10">
         <v>5</v>
       </c>
@@ -4246,7 +4300,7 @@
       <c r="D92" s="10">
         <v>90</v>
       </c>
-      <c r="E92" s="41"/>
+      <c r="E92" s="43"/>
       <c r="F92" s="10">
         <v>5</v>
       </c>
@@ -4264,7 +4318,7 @@
       <c r="D93" s="10">
         <v>91</v>
       </c>
-      <c r="E93" s="42"/>
+      <c r="E93" s="44"/>
       <c r="F93" s="10">
         <v>5</v>
       </c>
@@ -4302,7 +4356,7 @@
       <c r="D95" s="10">
         <v>93</v>
       </c>
-      <c r="E95" s="41"/>
+      <c r="E95" s="43"/>
       <c r="F95" s="10">
         <v>5</v>
       </c>
@@ -4320,7 +4374,7 @@
       <c r="D96" s="10">
         <v>94</v>
       </c>
-      <c r="E96" s="41"/>
+      <c r="E96" s="43"/>
       <c r="F96" s="10">
         <v>5</v>
       </c>
@@ -4338,7 +4392,7 @@
       <c r="D97" s="10">
         <v>95</v>
       </c>
-      <c r="E97" s="41"/>
+      <c r="E97" s="43"/>
       <c r="F97" s="10">
         <v>5</v>
       </c>
@@ -4356,7 +4410,7 @@
       <c r="D98" s="10">
         <v>96</v>
       </c>
-      <c r="E98" s="42"/>
+      <c r="E98" s="44"/>
       <c r="F98" s="10">
         <v>5</v>
       </c>
@@ -4394,7 +4448,7 @@
       <c r="D100" s="10">
         <v>98</v>
       </c>
-      <c r="E100" s="41"/>
+      <c r="E100" s="43"/>
       <c r="F100" s="10">
         <v>5</v>
       </c>
@@ -4412,7 +4466,7 @@
       <c r="D101" s="10">
         <v>99</v>
       </c>
-      <c r="E101" s="41"/>
+      <c r="E101" s="43"/>
       <c r="F101" s="10">
         <v>5</v>
       </c>
@@ -4430,7 +4484,7 @@
       <c r="D102" s="10">
         <v>100</v>
       </c>
-      <c r="E102" s="41"/>
+      <c r="E102" s="43"/>
       <c r="F102" s="10">
         <v>5</v>
       </c>
@@ -4448,7 +4502,7 @@
       <c r="D103" s="10">
         <v>101</v>
       </c>
-      <c r="E103" s="41"/>
+      <c r="E103" s="43"/>
       <c r="F103" s="10">
         <v>5</v>
       </c>
@@ -4466,7 +4520,7 @@
       <c r="D104" s="10">
         <v>102</v>
       </c>
-      <c r="E104" s="42"/>
+      <c r="E104" s="44"/>
       <c r="F104" s="10">
         <v>5</v>
       </c>
@@ -4746,7 +4800,7 @@
       <c r="D119" s="10">
         <v>117</v>
       </c>
-      <c r="E119" s="41"/>
+      <c r="E119" s="43"/>
       <c r="F119" s="10">
         <v>7</v>
       </c>
@@ -4764,7 +4818,7 @@
       <c r="D120" s="10">
         <v>118</v>
       </c>
-      <c r="E120" s="41"/>
+      <c r="E120" s="43"/>
       <c r="F120" s="10">
         <v>7</v>
       </c>
@@ -4782,7 +4836,7 @@
       <c r="D121" s="10">
         <v>119</v>
       </c>
-      <c r="E121" s="41"/>
+      <c r="E121" s="43"/>
       <c r="F121" s="10">
         <v>7</v>
       </c>
@@ -4800,7 +4854,7 @@
       <c r="D122" s="10">
         <v>120</v>
       </c>
-      <c r="E122" s="41"/>
+      <c r="E122" s="43"/>
       <c r="F122" s="10">
         <v>7</v>
       </c>
@@ -4818,7 +4872,7 @@
       <c r="D123" s="10">
         <v>121</v>
       </c>
-      <c r="E123" s="42"/>
+      <c r="E123" s="44"/>
       <c r="F123" s="10">
         <v>7</v>
       </c>
@@ -4856,7 +4910,7 @@
       <c r="D125" s="10">
         <v>123</v>
       </c>
-      <c r="E125" s="41"/>
+      <c r="E125" s="43"/>
       <c r="F125" s="10">
         <v>7</v>
       </c>
@@ -4874,7 +4928,7 @@
       <c r="D126" s="10">
         <v>124</v>
       </c>
-      <c r="E126" s="41"/>
+      <c r="E126" s="43"/>
       <c r="F126" s="10">
         <v>7</v>
       </c>
@@ -4892,7 +4946,7 @@
       <c r="D127" s="10">
         <v>125</v>
       </c>
-      <c r="E127" s="41"/>
+      <c r="E127" s="43"/>
       <c r="F127" s="10">
         <v>7</v>
       </c>
@@ -4910,7 +4964,7 @@
       <c r="D128" s="10">
         <v>126</v>
       </c>
-      <c r="E128" s="41"/>
+      <c r="E128" s="43"/>
       <c r="F128" s="10">
         <v>7</v>
       </c>
@@ -4928,7 +4982,7 @@
       <c r="D129" s="10">
         <v>127</v>
       </c>
-      <c r="E129" s="42"/>
+      <c r="E129" s="44"/>
       <c r="F129" s="10">
         <v>7</v>
       </c>
@@ -4966,7 +5020,7 @@
       <c r="D131" s="10">
         <v>129</v>
       </c>
-      <c r="E131" s="41"/>
+      <c r="E131" s="43"/>
       <c r="F131" s="10">
         <v>7</v>
       </c>
@@ -4984,7 +5038,7 @@
       <c r="D132" s="10">
         <v>130</v>
       </c>
-      <c r="E132" s="41"/>
+      <c r="E132" s="43"/>
       <c r="F132" s="10">
         <v>7</v>
       </c>
@@ -5002,7 +5056,7 @@
       <c r="D133" s="10">
         <v>131</v>
       </c>
-      <c r="E133" s="41"/>
+      <c r="E133" s="43"/>
       <c r="F133" s="10">
         <v>7</v>
       </c>
@@ -5020,7 +5074,7 @@
       <c r="D134" s="10">
         <v>132</v>
       </c>
-      <c r="E134" s="41"/>
+      <c r="E134" s="43"/>
       <c r="F134" s="10">
         <v>7</v>
       </c>
@@ -5038,7 +5092,7 @@
       <c r="D135" s="10">
         <v>133</v>
       </c>
-      <c r="E135" s="42"/>
+      <c r="E135" s="44"/>
       <c r="F135" s="10">
         <v>7</v>
       </c>
@@ -5076,7 +5130,7 @@
       <c r="D137" s="10">
         <v>135</v>
       </c>
-      <c r="E137" s="41"/>
+      <c r="E137" s="43"/>
       <c r="F137" s="10">
         <v>7</v>
       </c>
@@ -5094,7 +5148,7 @@
       <c r="D138" s="10">
         <v>136</v>
       </c>
-      <c r="E138" s="41"/>
+      <c r="E138" s="43"/>
       <c r="F138" s="10">
         <v>7</v>
       </c>
@@ -5112,7 +5166,7 @@
       <c r="D139" s="10">
         <v>137</v>
       </c>
-      <c r="E139" s="41"/>
+      <c r="E139" s="43"/>
       <c r="F139" s="10">
         <v>7</v>
       </c>
@@ -5130,7 +5184,7 @@
       <c r="D140" s="10">
         <v>138</v>
       </c>
-      <c r="E140" s="42"/>
+      <c r="E140" s="44"/>
       <c r="F140" s="10">
         <v>7</v>
       </c>
@@ -5164,7 +5218,7 @@
       <c r="D142" s="25">
         <v>200</v>
       </c>
-      <c r="E142" s="41"/>
+      <c r="E142" s="43"/>
       <c r="F142" s="25">
         <v>7</v>
       </c>
@@ -5180,7 +5234,7 @@
       <c r="D143" s="25">
         <v>201</v>
       </c>
-      <c r="E143" s="41"/>
+      <c r="E143" s="43"/>
       <c r="F143" s="25">
         <v>7</v>
       </c>
@@ -5196,7 +5250,7 @@
       <c r="D144" s="25">
         <v>202</v>
       </c>
-      <c r="E144" s="41"/>
+      <c r="E144" s="43"/>
       <c r="F144" s="25">
         <v>7</v>
       </c>
@@ -5212,7 +5266,7 @@
       <c r="D145" s="25">
         <v>203</v>
       </c>
-      <c r="E145" s="42"/>
+      <c r="E145" s="44"/>
       <c r="F145" s="25">
         <v>7</v>
       </c>
@@ -5290,7 +5344,7 @@
       <c r="D149" s="10">
         <v>142</v>
       </c>
-      <c r="E149" s="41"/>
+      <c r="E149" s="43"/>
       <c r="F149" s="10">
         <v>8</v>
       </c>
@@ -5308,7 +5362,7 @@
       <c r="D150" s="10">
         <v>143</v>
       </c>
-      <c r="E150" s="41"/>
+      <c r="E150" s="43"/>
       <c r="F150" s="10">
         <v>8</v>
       </c>
@@ -5326,7 +5380,7 @@
       <c r="D151" s="10">
         <v>144</v>
       </c>
-      <c r="E151" s="41"/>
+      <c r="E151" s="43"/>
       <c r="F151" s="10">
         <v>8</v>
       </c>
@@ -5344,7 +5398,7 @@
       <c r="D152" s="10">
         <v>145</v>
       </c>
-      <c r="E152" s="41"/>
+      <c r="E152" s="43"/>
       <c r="F152" s="10">
         <v>8</v>
       </c>
@@ -5362,7 +5416,7 @@
       <c r="D153" s="10">
         <v>146</v>
       </c>
-      <c r="E153" s="42"/>
+      <c r="E153" s="44"/>
       <c r="F153" s="10">
         <v>8</v>
       </c>
@@ -5400,7 +5454,7 @@
       <c r="D155" s="10">
         <v>148</v>
       </c>
-      <c r="E155" s="41"/>
+      <c r="E155" s="43"/>
       <c r="F155" s="10">
         <v>8</v>
       </c>
@@ -5418,7 +5472,7 @@
       <c r="D156" s="10">
         <v>149</v>
       </c>
-      <c r="E156" s="41"/>
+      <c r="E156" s="43"/>
       <c r="F156" s="10">
         <v>8</v>
       </c>
@@ -5436,7 +5490,7 @@
       <c r="D157" s="10">
         <v>150</v>
       </c>
-      <c r="E157" s="41"/>
+      <c r="E157" s="43"/>
       <c r="F157" s="10">
         <v>8</v>
       </c>
@@ -5454,7 +5508,7 @@
       <c r="D158" s="10">
         <v>151</v>
       </c>
-      <c r="E158" s="41"/>
+      <c r="E158" s="43"/>
       <c r="F158" s="10">
         <v>8</v>
       </c>
@@ -5472,7 +5526,7 @@
       <c r="D159" s="10">
         <v>152</v>
       </c>
-      <c r="E159" s="42"/>
+      <c r="E159" s="44"/>
       <c r="F159" s="10">
         <v>8</v>
       </c>
@@ -5481,890 +5535,1126 @@
       </c>
     </row>
     <row r="160" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B160" s="10" t="s">
-        <v>356</v>
-      </c>
-      <c r="C160" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="D160" s="10">
-        <v>153</v>
-      </c>
-      <c r="E160" s="40">
-        <v>10162</v>
-      </c>
-      <c r="F160" s="10">
-        <v>9</v>
-      </c>
-      <c r="G160" s="10" t="s">
-        <v>611</v>
+      <c r="B160" s="23" t="s">
+        <v>652</v>
+      </c>
+      <c r="C160" s="24"/>
+      <c r="D160" s="25">
+        <v>204</v>
+      </c>
+      <c r="E160" s="45">
+        <v>10157</v>
+      </c>
+      <c r="F160" s="25">
+        <v>8</v>
+      </c>
+      <c r="G160" s="25" t="s">
+        <v>647</v>
       </c>
     </row>
     <row r="161" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B161" s="10" t="s">
-        <v>357</v>
-      </c>
-      <c r="C161" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="D161" s="10">
-        <v>154</v>
-      </c>
-      <c r="E161" s="41"/>
-      <c r="F161" s="10">
-        <v>9</v>
-      </c>
-      <c r="G161" s="10" t="s">
-        <v>612</v>
+      <c r="B161" s="23" t="s">
+        <v>652</v>
+      </c>
+      <c r="C161" s="24"/>
+      <c r="D161" s="25">
+        <v>205</v>
+      </c>
+      <c r="E161" s="43"/>
+      <c r="F161" s="25">
+        <v>8</v>
+      </c>
+      <c r="G161" s="25" t="s">
+        <v>648</v>
       </c>
     </row>
     <row r="162" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B162" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="C162" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="D162" s="10">
-        <v>155</v>
-      </c>
-      <c r="E162" s="41"/>
-      <c r="F162" s="10">
-        <v>9</v>
-      </c>
-      <c r="G162" s="10" t="s">
-        <v>613</v>
+      <c r="B162" s="23" t="s">
+        <v>652</v>
+      </c>
+      <c r="C162" s="24"/>
+      <c r="D162" s="25">
+        <v>206</v>
+      </c>
+      <c r="E162" s="43"/>
+      <c r="F162" s="25">
+        <v>8</v>
+      </c>
+      <c r="G162" s="25" t="s">
+        <v>649</v>
       </c>
     </row>
     <row r="163" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B163" s="10" t="s">
-        <v>359</v>
-      </c>
-      <c r="C163" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="D163" s="10">
-        <v>156</v>
-      </c>
-      <c r="E163" s="41"/>
-      <c r="F163" s="10">
-        <v>9</v>
-      </c>
-      <c r="G163" s="10" t="s">
-        <v>614</v>
+      <c r="B163" s="23" t="s">
+        <v>652</v>
+      </c>
+      <c r="C163" s="24"/>
+      <c r="D163" s="25">
+        <v>207</v>
+      </c>
+      <c r="E163" s="43"/>
+      <c r="F163" s="25">
+        <v>8</v>
+      </c>
+      <c r="G163" s="25" t="s">
+        <v>650</v>
       </c>
     </row>
     <row r="164" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B164" s="10" t="s">
-        <v>360</v>
-      </c>
-      <c r="C164" s="31" t="s">
-        <v>434</v>
-      </c>
-      <c r="D164" s="10">
-        <v>157</v>
-      </c>
-      <c r="E164" s="41"/>
-      <c r="F164" s="10">
-        <v>9</v>
-      </c>
-      <c r="G164" s="10" t="s">
-        <v>615</v>
+      <c r="B164" s="23" t="s">
+        <v>652</v>
+      </c>
+      <c r="C164" s="24"/>
+      <c r="D164" s="25">
+        <v>208</v>
+      </c>
+      <c r="E164" s="44"/>
+      <c r="F164" s="25">
+        <v>8</v>
+      </c>
+      <c r="G164" s="25" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="165" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B165" s="10" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="C165" s="31" t="s">
-        <v>435</v>
+        <v>154</v>
       </c>
       <c r="D165" s="10">
-        <v>158</v>
-      </c>
-      <c r="E165" s="42"/>
+        <v>153</v>
+      </c>
+      <c r="E165" s="40">
+        <v>10162</v>
+      </c>
       <c r="F165" s="10">
         <v>9</v>
       </c>
       <c r="G165" s="10" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
     </row>
     <row r="166" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B166" s="10" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="C166" s="31" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D166" s="10">
-        <v>159</v>
-      </c>
-      <c r="E166" s="40">
-        <v>10168</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="E166" s="43"/>
       <c r="F166" s="10">
         <v>9</v>
       </c>
       <c r="G166" s="10" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
     <row r="167" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B167" s="10" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C167" s="31" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D167" s="10">
-        <v>160</v>
-      </c>
-      <c r="E167" s="41"/>
+        <v>155</v>
+      </c>
+      <c r="E167" s="43"/>
       <c r="F167" s="10">
         <v>9</v>
       </c>
       <c r="G167" s="10" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
     <row r="168" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B168" s="10" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="C168" s="31" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D168" s="10">
-        <v>161</v>
-      </c>
-      <c r="E168" s="41"/>
+        <v>156</v>
+      </c>
+      <c r="E168" s="43"/>
       <c r="F168" s="10">
         <v>9</v>
       </c>
       <c r="G168" s="10" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
     <row r="169" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B169" s="10" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="C169" s="31" t="s">
-        <v>161</v>
+        <v>434</v>
       </c>
       <c r="D169" s="10">
-        <v>162</v>
-      </c>
-      <c r="E169" s="41"/>
+        <v>157</v>
+      </c>
+      <c r="E169" s="43"/>
       <c r="F169" s="10">
         <v>9</v>
       </c>
       <c r="G169" s="10" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
     </row>
     <row r="170" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B170" s="10" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C170" s="31" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D170" s="10">
-        <v>163</v>
-      </c>
-      <c r="E170" s="41"/>
+        <v>158</v>
+      </c>
+      <c r="E170" s="44"/>
       <c r="F170" s="10">
         <v>9</v>
       </c>
       <c r="G170" s="10" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
     </row>
     <row r="171" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B171" s="10" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="C171" s="31" t="s">
-        <v>437</v>
+        <v>159</v>
       </c>
       <c r="D171" s="10">
-        <v>164</v>
-      </c>
-      <c r="E171" s="42"/>
+        <v>159</v>
+      </c>
+      <c r="E171" s="40">
+        <v>10168</v>
+      </c>
       <c r="F171" s="10">
         <v>9</v>
       </c>
       <c r="G171" s="10" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
     </row>
     <row r="172" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B172" s="10" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="C172" s="31" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D172" s="10">
-        <v>165</v>
-      </c>
-      <c r="E172" s="40">
-        <v>10174</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="E172" s="43"/>
       <c r="F172" s="10">
         <v>9</v>
       </c>
       <c r="G172" s="10" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
     </row>
     <row r="173" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B173" s="10" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="C173" s="31" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D173" s="10">
-        <v>166</v>
-      </c>
-      <c r="E173" s="41"/>
+        <v>161</v>
+      </c>
+      <c r="E173" s="43"/>
       <c r="F173" s="10">
         <v>9</v>
       </c>
       <c r="G173" s="10" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
     </row>
     <row r="174" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B174" s="10" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="C174" s="31" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D174" s="10">
-        <v>167</v>
-      </c>
-      <c r="E174" s="41"/>
+        <v>162</v>
+      </c>
+      <c r="E174" s="43"/>
       <c r="F174" s="10">
         <v>9</v>
       </c>
       <c r="G174" s="10" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
     </row>
     <row r="175" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B175" s="10" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C175" s="31" t="s">
-        <v>142</v>
+        <v>436</v>
       </c>
       <c r="D175" s="10">
-        <v>168</v>
-      </c>
-      <c r="E175" s="41"/>
+        <v>163</v>
+      </c>
+      <c r="E175" s="43"/>
       <c r="F175" s="10">
         <v>9</v>
       </c>
       <c r="G175" s="10" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
     </row>
     <row r="176" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B176" s="10" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C176" s="31" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D176" s="10">
-        <v>169</v>
-      </c>
-      <c r="E176" s="41"/>
+        <v>164</v>
+      </c>
+      <c r="E176" s="44"/>
       <c r="F176" s="10">
         <v>9</v>
       </c>
       <c r="G176" s="10" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
     </row>
     <row r="177" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B177" s="10" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="C177" s="31" t="s">
-        <v>439</v>
+        <v>164</v>
       </c>
       <c r="D177" s="10">
-        <v>170</v>
-      </c>
-      <c r="E177" s="42"/>
+        <v>165</v>
+      </c>
+      <c r="E177" s="40">
+        <v>10174</v>
+      </c>
       <c r="F177" s="10">
         <v>9</v>
       </c>
       <c r="G177" s="10" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
     </row>
     <row r="178" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B178" s="10" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="C178" s="31" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D178" s="10">
-        <v>171</v>
-      </c>
-      <c r="E178" s="37">
-        <v>10180</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="E178" s="43"/>
       <c r="F178" s="10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G178" s="10" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
     </row>
     <row r="179" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B179" s="10" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C179" s="31" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D179" s="10">
-        <v>172</v>
-      </c>
-      <c r="E179" s="38"/>
+        <v>167</v>
+      </c>
+      <c r="E179" s="43"/>
       <c r="F179" s="10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G179" s="10" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
     </row>
     <row r="180" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B180" s="10" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C180" s="31" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="D180" s="10">
-        <v>173</v>
-      </c>
-      <c r="E180" s="38"/>
+        <v>168</v>
+      </c>
+      <c r="E180" s="43"/>
       <c r="F180" s="10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G180" s="10" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
     </row>
     <row r="181" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B181" s="10" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="C181" s="31" t="s">
-        <v>147</v>
+        <v>438</v>
       </c>
       <c r="D181" s="10">
-        <v>174</v>
-      </c>
-      <c r="E181" s="38"/>
+        <v>169</v>
+      </c>
+      <c r="E181" s="43"/>
       <c r="F181" s="10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G181" s="10" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
     </row>
     <row r="182" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B182" s="10" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="C182" s="31" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D182" s="10">
-        <v>175</v>
-      </c>
-      <c r="E182" s="38"/>
+        <v>170</v>
+      </c>
+      <c r="E182" s="44"/>
       <c r="F182" s="10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G182" s="10" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
     </row>
     <row r="183" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B183" s="14" t="s">
-        <v>379</v>
-      </c>
-      <c r="C183" s="33" t="s">
-        <v>441</v>
-      </c>
-      <c r="D183" s="10">
-        <v>176</v>
-      </c>
-      <c r="E183" s="39"/>
-      <c r="F183" s="10">
-        <v>10</v>
-      </c>
-      <c r="G183" s="10" t="s">
-        <v>634</v>
+      <c r="B183" s="23" t="s">
+        <v>653</v>
+      </c>
+      <c r="C183" s="24"/>
+      <c r="D183" s="25">
+        <v>209</v>
+      </c>
+      <c r="E183" s="45">
+        <v>10175</v>
+      </c>
+      <c r="F183" s="25">
+        <v>9</v>
+      </c>
+      <c r="G183" s="25" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="184" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B184" s="10" t="s">
-        <v>388</v>
-      </c>
-      <c r="C184" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="D184" s="10">
-        <v>177</v>
-      </c>
-      <c r="E184" s="40">
-        <v>10181</v>
-      </c>
-      <c r="F184" s="10">
-        <v>11</v>
-      </c>
-      <c r="G184" s="10" t="s">
-        <v>173</v>
+      <c r="B184" s="23" t="s">
+        <v>653</v>
+      </c>
+      <c r="C184" s="24"/>
+      <c r="D184" s="25">
+        <v>210</v>
+      </c>
+      <c r="E184" s="43"/>
+      <c r="F184" s="25">
+        <v>9</v>
+      </c>
+      <c r="G184" s="25" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="185" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B185" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="C185" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="D185" s="10">
-        <v>178</v>
+      <c r="B185" s="23" t="s">
+        <v>653</v>
+      </c>
+      <c r="C185" s="24"/>
+      <c r="D185" s="25">
+        <v>211</v>
       </c>
       <c r="E185" s="43"/>
-      <c r="F185" s="10">
-        <v>11</v>
-      </c>
-      <c r="G185" s="10" t="s">
-        <v>174</v>
+      <c r="F185" s="25">
+        <v>9</v>
+      </c>
+      <c r="G185" s="25" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="186" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B186" s="10" t="s">
-        <v>390</v>
-      </c>
-      <c r="C186" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="D186" s="10">
-        <v>179</v>
+      <c r="B186" s="23" t="s">
+        <v>653</v>
+      </c>
+      <c r="C186" s="24"/>
+      <c r="D186" s="25">
+        <v>212</v>
       </c>
       <c r="E186" s="43"/>
-      <c r="F186" s="10">
-        <v>11</v>
-      </c>
-      <c r="G186" s="10" t="s">
-        <v>176</v>
+      <c r="F186" s="25">
+        <v>9</v>
+      </c>
+      <c r="G186" s="25" t="s">
+        <v>657</v>
       </c>
     </row>
     <row r="187" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B187" s="10" t="s">
-        <v>391</v>
-      </c>
-      <c r="C187" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="D187" s="10">
-        <v>180</v>
-      </c>
-      <c r="E187" s="43"/>
-      <c r="F187" s="10">
-        <v>11</v>
-      </c>
-      <c r="G187" s="10" t="s">
-        <v>175</v>
+      <c r="B187" s="23" t="s">
+        <v>653</v>
+      </c>
+      <c r="C187" s="24"/>
+      <c r="D187" s="25">
+        <v>213</v>
+      </c>
+      <c r="E187" s="44"/>
+      <c r="F187" s="25">
+        <v>9</v>
+      </c>
+      <c r="G187" s="25" t="s">
+        <v>658</v>
       </c>
     </row>
     <row r="188" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B188" s="10" t="s">
-        <v>392</v>
-      </c>
-      <c r="C188" s="12" t="s">
-        <v>380</v>
+        <v>374</v>
+      </c>
+      <c r="C188" s="31" t="s">
+        <v>168</v>
       </c>
       <c r="D188" s="10">
-        <v>181</v>
-      </c>
-      <c r="E188" s="43"/>
+        <v>171</v>
+      </c>
+      <c r="E188" s="37">
+        <v>10180</v>
+      </c>
       <c r="F188" s="10">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G188" s="10" t="s">
-        <v>380</v>
+        <v>629</v>
       </c>
     </row>
     <row r="189" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B189" s="10" t="s">
-        <v>393</v>
-      </c>
-      <c r="C189" s="12" t="s">
-        <v>381</v>
+        <v>375</v>
+      </c>
+      <c r="C189" s="31" t="s">
+        <v>169</v>
       </c>
       <c r="D189" s="10">
-        <v>182</v>
-      </c>
-      <c r="E189" s="44"/>
+        <v>172</v>
+      </c>
+      <c r="E189" s="38"/>
       <c r="F189" s="10">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G189" s="10" t="s">
-        <v>381</v>
+        <v>630</v>
       </c>
     </row>
     <row r="190" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B190" s="10" t="s">
-        <v>394</v>
-      </c>
-      <c r="C190" s="12" t="s">
-        <v>178</v>
+        <v>376</v>
+      </c>
+      <c r="C190" s="31" t="s">
+        <v>170</v>
       </c>
       <c r="D190" s="10">
-        <v>183</v>
-      </c>
-      <c r="E190" s="40">
-        <v>10182</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="E190" s="38"/>
       <c r="F190" s="10">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G190" s="10" t="s">
-        <v>178</v>
+        <v>631</v>
       </c>
     </row>
     <row r="191" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B191" s="10" t="s">
-        <v>395</v>
-      </c>
-      <c r="C191" s="12" t="s">
-        <v>179</v>
+        <v>377</v>
+      </c>
+      <c r="C191" s="31" t="s">
+        <v>147</v>
       </c>
       <c r="D191" s="10">
-        <v>184</v>
-      </c>
-      <c r="E191" s="43"/>
+        <v>174</v>
+      </c>
+      <c r="E191" s="38"/>
       <c r="F191" s="10">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G191" s="10" t="s">
-        <v>179</v>
+        <v>632</v>
       </c>
     </row>
     <row r="192" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B192" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="C192" s="12" t="s">
-        <v>180</v>
+        <v>378</v>
+      </c>
+      <c r="C192" s="31" t="s">
+        <v>440</v>
       </c>
       <c r="D192" s="10">
-        <v>185</v>
-      </c>
-      <c r="E192" s="43"/>
+        <v>175</v>
+      </c>
+      <c r="E192" s="38"/>
       <c r="F192" s="10">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G192" s="10" t="s">
-        <v>180</v>
+        <v>633</v>
       </c>
     </row>
     <row r="193" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B193" s="10" t="s">
-        <v>397</v>
-      </c>
-      <c r="C193" s="12" t="s">
-        <v>382</v>
+      <c r="B193" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="C193" s="33" t="s">
+        <v>441</v>
       </c>
       <c r="D193" s="10">
-        <v>186</v>
-      </c>
-      <c r="E193" s="43"/>
+        <v>176</v>
+      </c>
+      <c r="E193" s="39"/>
       <c r="F193" s="10">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G193" s="10" t="s">
-        <v>382</v>
+        <v>634</v>
       </c>
     </row>
     <row r="194" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B194" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="C194" s="12" t="s">
-        <v>383</v>
-      </c>
-      <c r="D194" s="10">
-        <v>187</v>
-      </c>
-      <c r="E194" s="44"/>
-      <c r="F194" s="10">
-        <v>11</v>
-      </c>
-      <c r="G194" s="10" t="s">
-        <v>383</v>
+      <c r="B194" s="23" t="s">
+        <v>659</v>
+      </c>
+      <c r="C194" s="24"/>
+      <c r="D194" s="25">
+        <v>214</v>
+      </c>
+      <c r="E194" s="45">
+        <v>101181</v>
+      </c>
+      <c r="F194" s="25">
+        <v>10</v>
+      </c>
+      <c r="G194" s="25" t="s">
+        <v>660</v>
       </c>
     </row>
     <row r="195" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B195" s="10" t="s">
-        <v>399</v>
-      </c>
-      <c r="C195" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="D195" s="10">
-        <v>188</v>
-      </c>
-      <c r="E195" s="40">
-        <v>10197</v>
-      </c>
-      <c r="F195" s="10">
-        <v>11</v>
-      </c>
-      <c r="G195" s="10" t="s">
-        <v>182</v>
+      <c r="B195" s="23" t="s">
+        <v>659</v>
+      </c>
+      <c r="C195" s="24"/>
+      <c r="D195" s="25">
+        <v>215</v>
+      </c>
+      <c r="E195" s="43"/>
+      <c r="F195" s="25">
+        <v>10</v>
+      </c>
+      <c r="G195" s="25" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="196" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B196" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="C196" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="D196" s="10">
-        <v>189</v>
-      </c>
-      <c r="E196" s="41"/>
-      <c r="F196" s="10">
-        <v>11</v>
-      </c>
-      <c r="G196" s="10" t="s">
-        <v>183</v>
+      <c r="B196" s="23" t="s">
+        <v>659</v>
+      </c>
+      <c r="C196" s="24"/>
+      <c r="D196" s="25">
+        <v>216</v>
+      </c>
+      <c r="E196" s="43"/>
+      <c r="F196" s="25">
+        <v>10</v>
+      </c>
+      <c r="G196" s="25" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="197" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B197" s="10" t="s">
-        <v>401</v>
-      </c>
-      <c r="C197" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="D197" s="10">
-        <v>190</v>
-      </c>
-      <c r="E197" s="41"/>
-      <c r="F197" s="10">
-        <v>11</v>
-      </c>
-      <c r="G197" s="10" t="s">
-        <v>184</v>
+      <c r="B197" s="23" t="s">
+        <v>659</v>
+      </c>
+      <c r="C197" s="24"/>
+      <c r="D197" s="25">
+        <v>217</v>
+      </c>
+      <c r="E197" s="43"/>
+      <c r="F197" s="25">
+        <v>10</v>
+      </c>
+      <c r="G197" s="25" t="s">
+        <v>663</v>
       </c>
     </row>
     <row r="198" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B198" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="C198" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="D198" s="10">
-        <v>191</v>
-      </c>
-      <c r="E198" s="41"/>
-      <c r="F198" s="10">
-        <v>11</v>
-      </c>
-      <c r="G198" s="10" t="s">
-        <v>384</v>
+      <c r="B198" s="23" t="s">
+        <v>659</v>
+      </c>
+      <c r="C198" s="24"/>
+      <c r="D198" s="25">
+        <v>218</v>
+      </c>
+      <c r="E198" s="44"/>
+      <c r="F198" s="25">
+        <v>10</v>
+      </c>
+      <c r="G198" s="25" t="s">
+        <v>664</v>
       </c>
     </row>
     <row r="199" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B199" s="10" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="C199" s="12" t="s">
-        <v>385</v>
+        <v>173</v>
       </c>
       <c r="D199" s="10">
-        <v>192</v>
-      </c>
-      <c r="E199" s="42"/>
+        <v>177</v>
+      </c>
+      <c r="E199" s="40">
+        <v>10181</v>
+      </c>
       <c r="F199" s="10">
         <v>11</v>
       </c>
       <c r="G199" s="10" t="s">
-        <v>385</v>
+        <v>173</v>
       </c>
     </row>
     <row r="200" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B200" s="10" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="C200" s="12" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="D200" s="10">
-        <v>193</v>
-      </c>
-      <c r="E200" s="40">
-        <v>10202</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="E200" s="41"/>
       <c r="F200" s="10">
         <v>11</v>
       </c>
       <c r="G200" s="10" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
     </row>
     <row r="201" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B201" s="10" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="C201" s="12" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="D201" s="10">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="E201" s="41"/>
       <c r="F201" s="10">
         <v>11</v>
       </c>
       <c r="G201" s="10" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="202" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B202" s="10" t="s">
-        <v>406</v>
+        <v>391</v>
       </c>
       <c r="C202" s="12" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="D202" s="10">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="E202" s="41"/>
       <c r="F202" s="10">
         <v>11</v>
       </c>
       <c r="G202" s="10" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
     </row>
     <row r="203" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B203" s="10" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
       <c r="C203" s="12" t="s">
-        <v>188</v>
+        <v>380</v>
       </c>
       <c r="D203" s="10">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="E203" s="41"/>
       <c r="F203" s="10">
         <v>11</v>
       </c>
       <c r="G203" s="10" t="s">
-        <v>188</v>
+        <v>380</v>
       </c>
     </row>
     <row r="204" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B204" s="10" t="s">
-        <v>408</v>
+        <v>393</v>
       </c>
       <c r="C204" s="12" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="D204" s="10">
-        <v>197</v>
-      </c>
-      <c r="E204" s="41"/>
+        <v>182</v>
+      </c>
+      <c r="E204" s="42"/>
       <c r="F204" s="10">
         <v>11</v>
       </c>
       <c r="G204" s="10" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
     </row>
     <row r="205" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B205" s="10" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
       <c r="C205" s="12" t="s">
-        <v>387</v>
+        <v>178</v>
       </c>
       <c r="D205" s="10">
-        <v>198</v>
-      </c>
-      <c r="E205" s="42"/>
+        <v>183</v>
+      </c>
+      <c r="E205" s="40">
+        <v>10182</v>
+      </c>
       <c r="F205" s="10">
         <v>11</v>
       </c>
       <c r="G205" s="10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="206" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B206" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="C206" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="D206" s="10">
+        <v>184</v>
+      </c>
+      <c r="E206" s="41"/>
+      <c r="F206" s="10">
+        <v>11</v>
+      </c>
+      <c r="G206" s="10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="207" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B207" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="C207" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D207" s="10">
+        <v>185</v>
+      </c>
+      <c r="E207" s="41"/>
+      <c r="F207" s="10">
+        <v>11</v>
+      </c>
+      <c r="G207" s="10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="208" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B208" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="C208" s="12" t="s">
+        <v>382</v>
+      </c>
+      <c r="D208" s="10">
+        <v>186</v>
+      </c>
+      <c r="E208" s="41"/>
+      <c r="F208" s="10">
+        <v>11</v>
+      </c>
+      <c r="G208" s="10" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="209" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B209" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="C209" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="D209" s="10">
+        <v>187</v>
+      </c>
+      <c r="E209" s="42"/>
+      <c r="F209" s="10">
+        <v>11</v>
+      </c>
+      <c r="G209" s="10" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="210" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B210" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="C210" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="D210" s="10">
+        <v>188</v>
+      </c>
+      <c r="E210" s="40">
+        <v>10197</v>
+      </c>
+      <c r="F210" s="10">
+        <v>11</v>
+      </c>
+      <c r="G210" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="211" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B211" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="C211" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="D211" s="10">
+        <v>189</v>
+      </c>
+      <c r="E211" s="43"/>
+      <c r="F211" s="10">
+        <v>11</v>
+      </c>
+      <c r="G211" s="10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="212" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B212" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="C212" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="D212" s="10">
+        <v>190</v>
+      </c>
+      <c r="E212" s="43"/>
+      <c r="F212" s="10">
+        <v>11</v>
+      </c>
+      <c r="G212" s="10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="213" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B213" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="C213" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="D213" s="10">
+        <v>191</v>
+      </c>
+      <c r="E213" s="43"/>
+      <c r="F213" s="10">
+        <v>11</v>
+      </c>
+      <c r="G213" s="10" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="214" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B214" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="C214" s="12" t="s">
+        <v>385</v>
+      </c>
+      <c r="D214" s="10">
+        <v>192</v>
+      </c>
+      <c r="E214" s="44"/>
+      <c r="F214" s="10">
+        <v>11</v>
+      </c>
+      <c r="G214" s="10" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="215" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B215" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="C215" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D215" s="10">
+        <v>193</v>
+      </c>
+      <c r="E215" s="40">
+        <v>10202</v>
+      </c>
+      <c r="F215" s="10">
+        <v>11</v>
+      </c>
+      <c r="G215" s="10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="216" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B216" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="C216" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D216" s="10">
+        <v>194</v>
+      </c>
+      <c r="E216" s="43"/>
+      <c r="F216" s="10">
+        <v>11</v>
+      </c>
+      <c r="G216" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="217" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B217" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="C217" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="D217" s="10">
+        <v>195</v>
+      </c>
+      <c r="E217" s="43"/>
+      <c r="F217" s="10">
+        <v>11</v>
+      </c>
+      <c r="G217" s="10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="218" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B218" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="C218" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="D218" s="10">
+        <v>196</v>
+      </c>
+      <c r="E218" s="43"/>
+      <c r="F218" s="10">
+        <v>11</v>
+      </c>
+      <c r="G218" s="10" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="219" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B219" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="C219" s="12" t="s">
+        <v>386</v>
+      </c>
+      <c r="D219" s="10">
+        <v>197</v>
+      </c>
+      <c r="E219" s="43"/>
+      <c r="F219" s="10">
+        <v>11</v>
+      </c>
+      <c r="G219" s="10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="220" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B220" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="C220" s="12" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="207" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="208" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B208" s="22" t="s">
+      <c r="D220" s="10">
+        <v>198</v>
+      </c>
+      <c r="E220" s="44"/>
+      <c r="F220" s="10">
+        <v>11</v>
+      </c>
+      <c r="G220" s="10" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="222" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="223" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B223" s="22" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="209" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B209" s="2"/>
-    </row>
-    <row r="210" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B210" s="26" t="s">
+    <row r="224" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B224" s="2"/>
+    </row>
+    <row r="225" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B225" s="26" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="211" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B211" s="2"/>
-    </row>
-    <row r="212" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B212" s="28" t="s">
+    <row r="226" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B226" s="2"/>
+    </row>
+    <row r="227" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B227" s="28" t="s">
         <v>644</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="E178:E183"/>
-    <mergeCell ref="E184:E189"/>
-    <mergeCell ref="E190:E194"/>
-    <mergeCell ref="E195:E199"/>
-    <mergeCell ref="E200:E205"/>
-    <mergeCell ref="E172:E177"/>
-    <mergeCell ref="E110:E113"/>
-    <mergeCell ref="E114:E117"/>
-    <mergeCell ref="E118:E123"/>
-    <mergeCell ref="E124:E129"/>
-    <mergeCell ref="E130:E135"/>
-    <mergeCell ref="E136:E140"/>
-    <mergeCell ref="E148:E153"/>
-    <mergeCell ref="E154:E159"/>
-    <mergeCell ref="E160:E165"/>
-    <mergeCell ref="E166:E171"/>
-    <mergeCell ref="E141:E145"/>
+  <mergeCells count="38">
+    <mergeCell ref="E183:E187"/>
+    <mergeCell ref="E194:E198"/>
+    <mergeCell ref="E3:E8"/>
+    <mergeCell ref="E9:E14"/>
+    <mergeCell ref="E15:E20"/>
+    <mergeCell ref="E21:E26"/>
+    <mergeCell ref="E27:E32"/>
     <mergeCell ref="E106:E109"/>
     <mergeCell ref="E99:E104"/>
     <mergeCell ref="E33:E38"/>
@@ -6378,11 +6668,24 @@
     <mergeCell ref="E80:E84"/>
     <mergeCell ref="E88:E93"/>
     <mergeCell ref="E94:E98"/>
-    <mergeCell ref="E3:E8"/>
-    <mergeCell ref="E9:E14"/>
-    <mergeCell ref="E15:E20"/>
-    <mergeCell ref="E21:E26"/>
-    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="E177:E182"/>
+    <mergeCell ref="E110:E113"/>
+    <mergeCell ref="E114:E117"/>
+    <mergeCell ref="E118:E123"/>
+    <mergeCell ref="E124:E129"/>
+    <mergeCell ref="E130:E135"/>
+    <mergeCell ref="E136:E140"/>
+    <mergeCell ref="E148:E153"/>
+    <mergeCell ref="E154:E159"/>
+    <mergeCell ref="E165:E170"/>
+    <mergeCell ref="E171:E176"/>
+    <mergeCell ref="E141:E145"/>
+    <mergeCell ref="E160:E164"/>
+    <mergeCell ref="E188:E193"/>
+    <mergeCell ref="E199:E204"/>
+    <mergeCell ref="E205:E209"/>
+    <mergeCell ref="E210:E214"/>
+    <mergeCell ref="E215:E220"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
add data for Olvia
</commit_message>
<xml_diff>
--- a/Documentation/База_данных_Арселор-Точки_измерения.xlsx
+++ b/Documentation/База_данных_Арселор-Точки_измерения.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="691">
   <si>
     <t>№</t>
   </si>
@@ -2033,6 +2033,84 @@
   </si>
   <si>
     <t>FE_3_25_normQ</t>
+  </si>
+  <si>
+    <t>Данные от Olvia</t>
+  </si>
+  <si>
+    <t>Ольвия, давление кислорода на входе в коллектор, линия 1</t>
+  </si>
+  <si>
+    <t>Ольвия, давление кислорода на входе в коллектор, линия 2</t>
+  </si>
+  <si>
+    <t>Ольвия, температура кислорода на входе в коллектор, линия 1</t>
+  </si>
+  <si>
+    <t>Ольвия, концентрация кислорода на входе в коллектор, линия 1</t>
+  </si>
+  <si>
+    <t>Ольвия, объёмный расход кислорода на входе в коллектор, линия 1</t>
+  </si>
+  <si>
+    <t>Ольвия, приведённый объёмный расход кислорода на входе в коллектор, линия 1</t>
+  </si>
+  <si>
+    <t>TE_1a2</t>
+  </si>
+  <si>
+    <t>PE_4a2</t>
+  </si>
+  <si>
+    <t>Ольвия, температура кислорода на входе в коллектор, линия 2</t>
+  </si>
+  <si>
+    <t>Ольвия, концентрация кислорода на входе в коллектор, линия 2</t>
+  </si>
+  <si>
+    <t>Ольвия, объёмный расход кислорода на входе в коллектор, линия 2</t>
+  </si>
+  <si>
+    <t>Ольвия, приведённый объёмный расход кислорода на входе в коллектор, линия 2</t>
+  </si>
+  <si>
+    <t>QE_1a2</t>
+  </si>
+  <si>
+    <t>FE_1a2_norm</t>
+  </si>
+  <si>
+    <t>FE_1a2_normQ</t>
+  </si>
+  <si>
+    <t>PE_4a1</t>
+  </si>
+  <si>
+    <t>TE_1a1</t>
+  </si>
+  <si>
+    <t>QE_1a1</t>
+  </si>
+  <si>
+    <t>FE_1a1_norm</t>
+  </si>
+  <si>
+    <t>FE_1a1_normQ</t>
+  </si>
+  <si>
+    <t>PE_5a2</t>
+  </si>
+  <si>
+    <t>Ольвия, давление кислорода на выходе из коллектора, №1</t>
+  </si>
+  <si>
+    <t>Ольвия, давление кислорода на выходе из коллектора, №2</t>
+  </si>
+  <si>
+    <t>PE_6a2</t>
+  </si>
+  <si>
+    <t>olvia</t>
   </si>
 </sst>
 </file>
@@ -2073,7 +2151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2107,6 +2185,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2214,7 +2298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2294,6 +2378,15 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2312,19 +2405,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2610,10 +2712,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:G227"/>
+  <dimension ref="B2:G241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G198" sqref="G198"/>
+    <sheetView tabSelected="1" topLeftCell="A205" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G238" sqref="G238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2656,7 +2758,7 @@
       <c r="D3" s="10">
         <v>1</v>
       </c>
-      <c r="E3" s="37">
+      <c r="E3" s="40">
         <v>10010</v>
       </c>
       <c r="F3" s="10">
@@ -2676,7 +2778,7 @@
       <c r="D4" s="10">
         <v>2</v>
       </c>
-      <c r="E4" s="38"/>
+      <c r="E4" s="41"/>
       <c r="F4" s="10">
         <v>1</v>
       </c>
@@ -2694,7 +2796,7 @@
       <c r="D5" s="10">
         <v>3</v>
       </c>
-      <c r="E5" s="38"/>
+      <c r="E5" s="41"/>
       <c r="F5" s="10">
         <v>1</v>
       </c>
@@ -2712,7 +2814,7 @@
       <c r="D6" s="10">
         <v>4</v>
       </c>
-      <c r="E6" s="38"/>
+      <c r="E6" s="41"/>
       <c r="F6" s="10">
         <v>1</v>
       </c>
@@ -2730,7 +2832,7 @@
       <c r="D7" s="10">
         <v>5</v>
       </c>
-      <c r="E7" s="38"/>
+      <c r="E7" s="41"/>
       <c r="F7" s="10">
         <v>1</v>
       </c>
@@ -2748,7 +2850,7 @@
       <c r="D8" s="10">
         <v>6</v>
       </c>
-      <c r="E8" s="39"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="10">
         <v>1</v>
       </c>
@@ -2766,7 +2868,7 @@
       <c r="D9" s="10">
         <v>7</v>
       </c>
-      <c r="E9" s="40">
+      <c r="E9" s="43">
         <v>10016</v>
       </c>
       <c r="F9" s="10">
@@ -2786,7 +2888,7 @@
       <c r="D10" s="10">
         <v>8</v>
       </c>
-      <c r="E10" s="43"/>
+      <c r="E10" s="38"/>
       <c r="F10" s="10">
         <v>2</v>
       </c>
@@ -2804,7 +2906,7 @@
       <c r="D11" s="10">
         <v>9</v>
       </c>
-      <c r="E11" s="43"/>
+      <c r="E11" s="38"/>
       <c r="F11" s="10">
         <v>2</v>
       </c>
@@ -2822,7 +2924,7 @@
       <c r="D12" s="10">
         <v>10</v>
       </c>
-      <c r="E12" s="43"/>
+      <c r="E12" s="38"/>
       <c r="F12" s="10">
         <v>2</v>
       </c>
@@ -2840,7 +2942,7 @@
       <c r="D13" s="10">
         <v>11</v>
       </c>
-      <c r="E13" s="43"/>
+      <c r="E13" s="38"/>
       <c r="F13" s="10">
         <v>2</v>
       </c>
@@ -2858,7 +2960,7 @@
       <c r="D14" s="10">
         <v>12</v>
       </c>
-      <c r="E14" s="44"/>
+      <c r="E14" s="39"/>
       <c r="F14" s="10">
         <v>2</v>
       </c>
@@ -2876,7 +2978,7 @@
       <c r="D15" s="10">
         <v>13</v>
       </c>
-      <c r="E15" s="40">
+      <c r="E15" s="43">
         <v>10022</v>
       </c>
       <c r="F15" s="10">
@@ -2896,7 +2998,7 @@
       <c r="D16" s="10">
         <v>14</v>
       </c>
-      <c r="E16" s="43"/>
+      <c r="E16" s="38"/>
       <c r="F16" s="10">
         <v>2</v>
       </c>
@@ -2914,7 +3016,7 @@
       <c r="D17" s="10">
         <v>15</v>
       </c>
-      <c r="E17" s="43"/>
+      <c r="E17" s="38"/>
       <c r="F17" s="10">
         <v>2</v>
       </c>
@@ -2932,7 +3034,7 @@
       <c r="D18" s="10">
         <v>16</v>
       </c>
-      <c r="E18" s="43"/>
+      <c r="E18" s="38"/>
       <c r="F18" s="10">
         <v>2</v>
       </c>
@@ -2950,7 +3052,7 @@
       <c r="D19" s="10">
         <v>17</v>
       </c>
-      <c r="E19" s="43"/>
+      <c r="E19" s="38"/>
       <c r="F19" s="10">
         <v>2</v>
       </c>
@@ -2968,7 +3070,7 @@
       <c r="D20" s="10">
         <v>18</v>
       </c>
-      <c r="E20" s="44"/>
+      <c r="E20" s="39"/>
       <c r="F20" s="10">
         <v>2</v>
       </c>
@@ -2986,7 +3088,7 @@
       <c r="D21" s="10">
         <v>19</v>
       </c>
-      <c r="E21" s="40">
+      <c r="E21" s="43">
         <v>10028</v>
       </c>
       <c r="F21" s="10">
@@ -3006,7 +3108,7 @@
       <c r="D22" s="10">
         <v>20</v>
       </c>
-      <c r="E22" s="43"/>
+      <c r="E22" s="38"/>
       <c r="F22" s="10">
         <v>2</v>
       </c>
@@ -3024,7 +3126,7 @@
       <c r="D23" s="10">
         <v>21</v>
       </c>
-      <c r="E23" s="43"/>
+      <c r="E23" s="38"/>
       <c r="F23" s="10">
         <v>2</v>
       </c>
@@ -3042,7 +3144,7 @@
       <c r="D24" s="10">
         <v>22</v>
       </c>
-      <c r="E24" s="43"/>
+      <c r="E24" s="38"/>
       <c r="F24" s="10">
         <v>2</v>
       </c>
@@ -3060,7 +3162,7 @@
       <c r="D25" s="10">
         <v>23</v>
       </c>
-      <c r="E25" s="43"/>
+      <c r="E25" s="38"/>
       <c r="F25" s="10">
         <v>2</v>
       </c>
@@ -3078,7 +3180,7 @@
       <c r="D26" s="10">
         <v>24</v>
       </c>
-      <c r="E26" s="44"/>
+      <c r="E26" s="39"/>
       <c r="F26" s="10">
         <v>2</v>
       </c>
@@ -3096,7 +3198,7 @@
       <c r="D27" s="10">
         <v>25</v>
       </c>
-      <c r="E27" s="40">
+      <c r="E27" s="43">
         <v>10034</v>
       </c>
       <c r="F27" s="10">
@@ -3116,7 +3218,7 @@
       <c r="D28" s="10">
         <v>26</v>
       </c>
-      <c r="E28" s="43"/>
+      <c r="E28" s="38"/>
       <c r="F28" s="10">
         <v>2</v>
       </c>
@@ -3134,7 +3236,7 @@
       <c r="D29" s="10">
         <v>27</v>
       </c>
-      <c r="E29" s="43"/>
+      <c r="E29" s="38"/>
       <c r="F29" s="10">
         <v>2</v>
       </c>
@@ -3152,7 +3254,7 @@
       <c r="D30" s="10">
         <v>28</v>
       </c>
-      <c r="E30" s="43"/>
+      <c r="E30" s="38"/>
       <c r="F30" s="10">
         <v>2</v>
       </c>
@@ -3170,7 +3272,7 @@
       <c r="D31" s="10">
         <v>29</v>
       </c>
-      <c r="E31" s="43"/>
+      <c r="E31" s="38"/>
       <c r="F31" s="10">
         <v>2</v>
       </c>
@@ -3188,7 +3290,7 @@
       <c r="D32" s="10">
         <v>30</v>
       </c>
-      <c r="E32" s="44"/>
+      <c r="E32" s="39"/>
       <c r="F32" s="10">
         <v>2</v>
       </c>
@@ -3206,7 +3308,7 @@
       <c r="D33" s="10">
         <v>31</v>
       </c>
-      <c r="E33" s="40">
+      <c r="E33" s="43">
         <v>10040</v>
       </c>
       <c r="F33" s="10">
@@ -3226,7 +3328,7 @@
       <c r="D34" s="10">
         <v>32</v>
       </c>
-      <c r="E34" s="43"/>
+      <c r="E34" s="38"/>
       <c r="F34" s="10">
         <v>2</v>
       </c>
@@ -3244,7 +3346,7 @@
       <c r="D35" s="10">
         <v>33</v>
       </c>
-      <c r="E35" s="43"/>
+      <c r="E35" s="38"/>
       <c r="F35" s="10">
         <v>2</v>
       </c>
@@ -3262,7 +3364,7 @@
       <c r="D36" s="10">
         <v>34</v>
       </c>
-      <c r="E36" s="43"/>
+      <c r="E36" s="38"/>
       <c r="F36" s="10">
         <v>2</v>
       </c>
@@ -3280,7 +3382,7 @@
       <c r="D37" s="10">
         <v>35</v>
       </c>
-      <c r="E37" s="43"/>
+      <c r="E37" s="38"/>
       <c r="F37" s="10">
         <v>2</v>
       </c>
@@ -3298,7 +3400,7 @@
       <c r="D38" s="10">
         <v>36</v>
       </c>
-      <c r="E38" s="44"/>
+      <c r="E38" s="39"/>
       <c r="F38" s="10">
         <v>2</v>
       </c>
@@ -3316,7 +3418,7 @@
       <c r="D39" s="10">
         <v>37</v>
       </c>
-      <c r="E39" s="40">
+      <c r="E39" s="43">
         <v>10046</v>
       </c>
       <c r="F39" s="10">
@@ -3336,7 +3438,7 @@
       <c r="D40" s="10">
         <v>38</v>
       </c>
-      <c r="E40" s="43"/>
+      <c r="E40" s="38"/>
       <c r="F40" s="10">
         <v>3</v>
       </c>
@@ -3354,7 +3456,7 @@
       <c r="D41" s="10">
         <v>39</v>
       </c>
-      <c r="E41" s="43"/>
+      <c r="E41" s="38"/>
       <c r="F41" s="10">
         <v>3</v>
       </c>
@@ -3372,7 +3474,7 @@
       <c r="D42" s="10">
         <v>40</v>
       </c>
-      <c r="E42" s="43"/>
+      <c r="E42" s="38"/>
       <c r="F42" s="10">
         <v>3</v>
       </c>
@@ -3390,7 +3492,7 @@
       <c r="D43" s="10">
         <v>41</v>
       </c>
-      <c r="E43" s="43"/>
+      <c r="E43" s="38"/>
       <c r="F43" s="10">
         <v>3</v>
       </c>
@@ -3408,7 +3510,7 @@
       <c r="D44" s="10">
         <v>42</v>
       </c>
-      <c r="E44" s="44"/>
+      <c r="E44" s="39"/>
       <c r="F44" s="10">
         <v>3</v>
       </c>
@@ -3426,7 +3528,7 @@
       <c r="D45" s="10">
         <v>43</v>
       </c>
-      <c r="E45" s="40">
+      <c r="E45" s="43">
         <v>10052</v>
       </c>
       <c r="F45" s="10">
@@ -3446,7 +3548,7 @@
       <c r="D46" s="10">
         <v>44</v>
       </c>
-      <c r="E46" s="43"/>
+      <c r="E46" s="38"/>
       <c r="F46" s="10">
         <v>3</v>
       </c>
@@ -3464,7 +3566,7 @@
       <c r="D47" s="10">
         <v>45</v>
       </c>
-      <c r="E47" s="43"/>
+      <c r="E47" s="38"/>
       <c r="F47" s="10">
         <v>3</v>
       </c>
@@ -3482,7 +3584,7 @@
       <c r="D48" s="10">
         <v>46</v>
       </c>
-      <c r="E48" s="43"/>
+      <c r="E48" s="38"/>
       <c r="F48" s="10">
         <v>3</v>
       </c>
@@ -3500,7 +3602,7 @@
       <c r="D49" s="10">
         <v>47</v>
       </c>
-      <c r="E49" s="44"/>
+      <c r="E49" s="39"/>
       <c r="F49" s="10">
         <v>3</v>
       </c>
@@ -3518,7 +3620,7 @@
       <c r="D50" s="10">
         <v>48</v>
       </c>
-      <c r="E50" s="40">
+      <c r="E50" s="43">
         <v>10053</v>
       </c>
       <c r="F50" s="10">
@@ -3538,7 +3640,7 @@
       <c r="D51" s="10">
         <v>49</v>
       </c>
-      <c r="E51" s="41"/>
+      <c r="E51" s="44"/>
       <c r="F51" s="10">
         <v>3</v>
       </c>
@@ -3556,7 +3658,7 @@
       <c r="D52" s="10">
         <v>50</v>
       </c>
-      <c r="E52" s="41"/>
+      <c r="E52" s="44"/>
       <c r="F52" s="10">
         <v>3</v>
       </c>
@@ -3574,7 +3676,7 @@
       <c r="D53" s="10">
         <v>51</v>
       </c>
-      <c r="E53" s="41"/>
+      <c r="E53" s="44"/>
       <c r="F53" s="10">
         <v>3</v>
       </c>
@@ -3592,7 +3694,7 @@
       <c r="D54" s="10">
         <v>52</v>
       </c>
-      <c r="E54" s="42"/>
+      <c r="E54" s="45"/>
       <c r="F54" s="10">
         <v>3</v>
       </c>
@@ -3610,7 +3712,7 @@
       <c r="D55" s="10">
         <v>53</v>
       </c>
-      <c r="E55" s="40">
+      <c r="E55" s="43">
         <v>10062</v>
       </c>
       <c r="F55" s="10">
@@ -3630,7 +3732,7 @@
       <c r="D56" s="10">
         <v>54</v>
       </c>
-      <c r="E56" s="43"/>
+      <c r="E56" s="38"/>
       <c r="F56" s="10">
         <v>3</v>
       </c>
@@ -3648,7 +3750,7 @@
       <c r="D57" s="10">
         <v>55</v>
       </c>
-      <c r="E57" s="43"/>
+      <c r="E57" s="38"/>
       <c r="F57" s="10">
         <v>3</v>
       </c>
@@ -3666,7 +3768,7 @@
       <c r="D58" s="10">
         <v>56</v>
       </c>
-      <c r="E58" s="43"/>
+      <c r="E58" s="38"/>
       <c r="F58" s="10">
         <v>3</v>
       </c>
@@ -3684,7 +3786,7 @@
       <c r="D59" s="10">
         <v>57</v>
       </c>
-      <c r="E59" s="43"/>
+      <c r="E59" s="38"/>
       <c r="F59" s="10">
         <v>3</v>
       </c>
@@ -3702,7 +3804,7 @@
       <c r="D60" s="10">
         <v>58</v>
       </c>
-      <c r="E60" s="44"/>
+      <c r="E60" s="39"/>
       <c r="F60" s="10">
         <v>3</v>
       </c>
@@ -3780,7 +3882,7 @@
       <c r="D64" s="10">
         <v>62</v>
       </c>
-      <c r="E64" s="37">
+      <c r="E64" s="40">
         <v>10071</v>
       </c>
       <c r="F64" s="10">
@@ -3800,7 +3902,7 @@
       <c r="D65" s="10">
         <v>63</v>
       </c>
-      <c r="E65" s="38"/>
+      <c r="E65" s="41"/>
       <c r="F65" s="10">
         <v>4</v>
       </c>
@@ -3818,7 +3920,7 @@
       <c r="D66" s="10">
         <v>64</v>
       </c>
-      <c r="E66" s="38"/>
+      <c r="E66" s="41"/>
       <c r="F66" s="10">
         <v>4</v>
       </c>
@@ -3836,7 +3938,7 @@
       <c r="D67" s="10">
         <v>65</v>
       </c>
-      <c r="E67" s="38"/>
+      <c r="E67" s="41"/>
       <c r="F67" s="10">
         <v>4</v>
       </c>
@@ -3854,7 +3956,7 @@
       <c r="D68" s="10">
         <v>66</v>
       </c>
-      <c r="E68" s="38"/>
+      <c r="E68" s="41"/>
       <c r="F68" s="10">
         <v>4</v>
       </c>
@@ -3872,7 +3974,7 @@
       <c r="D69" s="10">
         <v>67</v>
       </c>
-      <c r="E69" s="39"/>
+      <c r="E69" s="42"/>
       <c r="F69" s="10">
         <v>4</v>
       </c>
@@ -3890,7 +3992,7 @@
       <c r="D70" s="10">
         <v>68</v>
       </c>
-      <c r="E70" s="37">
+      <c r="E70" s="40">
         <v>10077</v>
       </c>
       <c r="F70" s="10">
@@ -3910,7 +4012,7 @@
       <c r="D71" s="10">
         <v>69</v>
       </c>
-      <c r="E71" s="38"/>
+      <c r="E71" s="41"/>
       <c r="F71" s="10">
         <v>4</v>
       </c>
@@ -3928,7 +4030,7 @@
       <c r="D72" s="10">
         <v>70</v>
       </c>
-      <c r="E72" s="38"/>
+      <c r="E72" s="41"/>
       <c r="F72" s="10">
         <v>4</v>
       </c>
@@ -3946,7 +4048,7 @@
       <c r="D73" s="10">
         <v>71</v>
       </c>
-      <c r="E73" s="38"/>
+      <c r="E73" s="41"/>
       <c r="F73" s="10">
         <v>4</v>
       </c>
@@ -3964,7 +4066,7 @@
       <c r="D74" s="10">
         <v>72</v>
       </c>
-      <c r="E74" s="39"/>
+      <c r="E74" s="42"/>
       <c r="F74" s="10">
         <v>4</v>
       </c>
@@ -3982,7 +4084,7 @@
       <c r="D75" s="10">
         <v>73</v>
       </c>
-      <c r="E75" s="37">
+      <c r="E75" s="40">
         <v>10078</v>
       </c>
       <c r="F75" s="10">
@@ -4002,7 +4104,7 @@
       <c r="D76" s="10">
         <v>74</v>
       </c>
-      <c r="E76" s="38"/>
+      <c r="E76" s="41"/>
       <c r="F76" s="10">
         <v>4</v>
       </c>
@@ -4020,7 +4122,7 @@
       <c r="D77" s="10">
         <v>75</v>
       </c>
-      <c r="E77" s="38"/>
+      <c r="E77" s="41"/>
       <c r="F77" s="10">
         <v>4</v>
       </c>
@@ -4038,7 +4140,7 @@
       <c r="D78" s="10">
         <v>76</v>
       </c>
-      <c r="E78" s="38"/>
+      <c r="E78" s="41"/>
       <c r="F78" s="10">
         <v>4</v>
       </c>
@@ -4056,7 +4158,7 @@
       <c r="D79" s="10">
         <v>77</v>
       </c>
-      <c r="E79" s="39"/>
+      <c r="E79" s="42"/>
       <c r="F79" s="10">
         <v>4</v>
       </c>
@@ -4074,7 +4176,7 @@
       <c r="D80" s="10">
         <v>78</v>
       </c>
-      <c r="E80" s="37">
+      <c r="E80" s="40">
         <v>10087</v>
       </c>
       <c r="F80" s="10">
@@ -4094,7 +4196,7 @@
       <c r="D81" s="10">
         <v>79</v>
       </c>
-      <c r="E81" s="38"/>
+      <c r="E81" s="41"/>
       <c r="F81" s="10">
         <v>4</v>
       </c>
@@ -4112,7 +4214,7 @@
       <c r="D82" s="10">
         <v>80</v>
       </c>
-      <c r="E82" s="38"/>
+      <c r="E82" s="41"/>
       <c r="F82" s="10">
         <v>4</v>
       </c>
@@ -4130,7 +4232,7 @@
       <c r="D83" s="10">
         <v>81</v>
       </c>
-      <c r="E83" s="38"/>
+      <c r="E83" s="41"/>
       <c r="F83" s="10">
         <v>4</v>
       </c>
@@ -4148,7 +4250,7 @@
       <c r="D84" s="10">
         <v>82</v>
       </c>
-      <c r="E84" s="39"/>
+      <c r="E84" s="42"/>
       <c r="F84" s="10">
         <v>4</v>
       </c>
@@ -4226,7 +4328,7 @@
       <c r="D88" s="10">
         <v>86</v>
       </c>
-      <c r="E88" s="40">
+      <c r="E88" s="43">
         <v>10095</v>
       </c>
       <c r="F88" s="10">
@@ -4246,7 +4348,7 @@
       <c r="D89" s="10">
         <v>87</v>
       </c>
-      <c r="E89" s="43"/>
+      <c r="E89" s="38"/>
       <c r="F89" s="10">
         <v>5</v>
       </c>
@@ -4264,7 +4366,7 @@
       <c r="D90" s="10">
         <v>88</v>
       </c>
-      <c r="E90" s="43"/>
+      <c r="E90" s="38"/>
       <c r="F90" s="10">
         <v>5</v>
       </c>
@@ -4282,7 +4384,7 @@
       <c r="D91" s="10">
         <v>89</v>
       </c>
-      <c r="E91" s="43"/>
+      <c r="E91" s="38"/>
       <c r="F91" s="10">
         <v>5</v>
       </c>
@@ -4300,7 +4402,7 @@
       <c r="D92" s="10">
         <v>90</v>
       </c>
-      <c r="E92" s="43"/>
+      <c r="E92" s="38"/>
       <c r="F92" s="10">
         <v>5</v>
       </c>
@@ -4318,7 +4420,7 @@
       <c r="D93" s="10">
         <v>91</v>
       </c>
-      <c r="E93" s="44"/>
+      <c r="E93" s="39"/>
       <c r="F93" s="10">
         <v>5</v>
       </c>
@@ -4336,7 +4438,7 @@
       <c r="D94" s="10">
         <v>92</v>
       </c>
-      <c r="E94" s="40">
+      <c r="E94" s="43">
         <v>10101</v>
       </c>
       <c r="F94" s="10">
@@ -4356,7 +4458,7 @@
       <c r="D95" s="10">
         <v>93</v>
       </c>
-      <c r="E95" s="43"/>
+      <c r="E95" s="38"/>
       <c r="F95" s="10">
         <v>5</v>
       </c>
@@ -4374,7 +4476,7 @@
       <c r="D96" s="10">
         <v>94</v>
       </c>
-      <c r="E96" s="43"/>
+      <c r="E96" s="38"/>
       <c r="F96" s="10">
         <v>5</v>
       </c>
@@ -4392,7 +4494,7 @@
       <c r="D97" s="10">
         <v>95</v>
       </c>
-      <c r="E97" s="43"/>
+      <c r="E97" s="38"/>
       <c r="F97" s="10">
         <v>5</v>
       </c>
@@ -4410,7 +4512,7 @@
       <c r="D98" s="10">
         <v>96</v>
       </c>
-      <c r="E98" s="44"/>
+      <c r="E98" s="39"/>
       <c r="F98" s="10">
         <v>5</v>
       </c>
@@ -4428,7 +4530,7 @@
       <c r="D99" s="10">
         <v>97</v>
       </c>
-      <c r="E99" s="40">
+      <c r="E99" s="43">
         <v>10107</v>
       </c>
       <c r="F99" s="10">
@@ -4448,7 +4550,7 @@
       <c r="D100" s="10">
         <v>98</v>
       </c>
-      <c r="E100" s="43"/>
+      <c r="E100" s="38"/>
       <c r="F100" s="10">
         <v>5</v>
       </c>
@@ -4466,7 +4568,7 @@
       <c r="D101" s="10">
         <v>99</v>
       </c>
-      <c r="E101" s="43"/>
+      <c r="E101" s="38"/>
       <c r="F101" s="10">
         <v>5</v>
       </c>
@@ -4484,7 +4586,7 @@
       <c r="D102" s="10">
         <v>100</v>
       </c>
-      <c r="E102" s="43"/>
+      <c r="E102" s="38"/>
       <c r="F102" s="10">
         <v>5</v>
       </c>
@@ -4502,7 +4604,7 @@
       <c r="D103" s="10">
         <v>101</v>
       </c>
-      <c r="E103" s="43"/>
+      <c r="E103" s="38"/>
       <c r="F103" s="10">
         <v>5</v>
       </c>
@@ -4520,7 +4622,7 @@
       <c r="D104" s="10">
         <v>102</v>
       </c>
-      <c r="E104" s="44"/>
+      <c r="E104" s="39"/>
       <c r="F104" s="10">
         <v>5</v>
       </c>
@@ -4558,7 +4660,7 @@
       <c r="D106" s="10">
         <v>104</v>
       </c>
-      <c r="E106" s="38">
+      <c r="E106" s="41">
         <v>10113</v>
       </c>
       <c r="F106" s="10">
@@ -4578,7 +4680,7 @@
       <c r="D107" s="10">
         <v>105</v>
       </c>
-      <c r="E107" s="38"/>
+      <c r="E107" s="41"/>
       <c r="F107" s="10">
         <v>7</v>
       </c>
@@ -4596,7 +4698,7 @@
       <c r="D108" s="10">
         <v>106</v>
       </c>
-      <c r="E108" s="38"/>
+      <c r="E108" s="41"/>
       <c r="F108" s="10">
         <v>7</v>
       </c>
@@ -4614,7 +4716,7 @@
       <c r="D109" s="10">
         <v>107</v>
       </c>
-      <c r="E109" s="39"/>
+      <c r="E109" s="42"/>
       <c r="F109" s="10">
         <v>7</v>
       </c>
@@ -4632,7 +4734,7 @@
       <c r="D110" s="10">
         <v>108</v>
       </c>
-      <c r="E110" s="37">
+      <c r="E110" s="40">
         <v>10117</v>
       </c>
       <c r="F110" s="10">
@@ -4652,7 +4754,7 @@
       <c r="D111" s="10">
         <v>109</v>
       </c>
-      <c r="E111" s="38"/>
+      <c r="E111" s="41"/>
       <c r="F111" s="10">
         <v>7</v>
       </c>
@@ -4670,7 +4772,7 @@
       <c r="D112" s="10">
         <v>110</v>
       </c>
-      <c r="E112" s="38"/>
+      <c r="E112" s="41"/>
       <c r="F112" s="10">
         <v>7</v>
       </c>
@@ -4688,7 +4790,7 @@
       <c r="D113" s="10">
         <v>111</v>
       </c>
-      <c r="E113" s="39"/>
+      <c r="E113" s="42"/>
       <c r="F113" s="10">
         <v>7</v>
       </c>
@@ -4706,7 +4808,7 @@
       <c r="D114" s="10">
         <v>112</v>
       </c>
-      <c r="E114" s="37">
+      <c r="E114" s="40">
         <v>10121</v>
       </c>
       <c r="F114" s="10">
@@ -4726,7 +4828,7 @@
       <c r="D115" s="10">
         <v>113</v>
       </c>
-      <c r="E115" s="38"/>
+      <c r="E115" s="41"/>
       <c r="F115" s="10">
         <v>7</v>
       </c>
@@ -4744,7 +4846,7 @@
       <c r="D116" s="10">
         <v>114</v>
       </c>
-      <c r="E116" s="38"/>
+      <c r="E116" s="41"/>
       <c r="F116" s="10">
         <v>7</v>
       </c>
@@ -4762,7 +4864,7 @@
       <c r="D117" s="10">
         <v>115</v>
       </c>
-      <c r="E117" s="39"/>
+      <c r="E117" s="42"/>
       <c r="F117" s="10">
         <v>7</v>
       </c>
@@ -4780,7 +4882,7 @@
       <c r="D118" s="10">
         <v>116</v>
       </c>
-      <c r="E118" s="40">
+      <c r="E118" s="43">
         <v>10125</v>
       </c>
       <c r="F118" s="10">
@@ -4800,7 +4902,7 @@
       <c r="D119" s="10">
         <v>117</v>
       </c>
-      <c r="E119" s="43"/>
+      <c r="E119" s="38"/>
       <c r="F119" s="10">
         <v>7</v>
       </c>
@@ -4818,7 +4920,7 @@
       <c r="D120" s="10">
         <v>118</v>
       </c>
-      <c r="E120" s="43"/>
+      <c r="E120" s="38"/>
       <c r="F120" s="10">
         <v>7</v>
       </c>
@@ -4836,7 +4938,7 @@
       <c r="D121" s="10">
         <v>119</v>
       </c>
-      <c r="E121" s="43"/>
+      <c r="E121" s="38"/>
       <c r="F121" s="10">
         <v>7</v>
       </c>
@@ -4854,7 +4956,7 @@
       <c r="D122" s="10">
         <v>120</v>
       </c>
-      <c r="E122" s="43"/>
+      <c r="E122" s="38"/>
       <c r="F122" s="10">
         <v>7</v>
       </c>
@@ -4872,7 +4974,7 @@
       <c r="D123" s="10">
         <v>121</v>
       </c>
-      <c r="E123" s="44"/>
+      <c r="E123" s="39"/>
       <c r="F123" s="10">
         <v>7</v>
       </c>
@@ -4890,7 +4992,7 @@
       <c r="D124" s="10">
         <v>122</v>
       </c>
-      <c r="E124" s="40">
+      <c r="E124" s="43">
         <v>10131</v>
       </c>
       <c r="F124" s="10">
@@ -4910,7 +5012,7 @@
       <c r="D125" s="10">
         <v>123</v>
       </c>
-      <c r="E125" s="43"/>
+      <c r="E125" s="38"/>
       <c r="F125" s="10">
         <v>7</v>
       </c>
@@ -4928,7 +5030,7 @@
       <c r="D126" s="10">
         <v>124</v>
       </c>
-      <c r="E126" s="43"/>
+      <c r="E126" s="38"/>
       <c r="F126" s="10">
         <v>7</v>
       </c>
@@ -4946,7 +5048,7 @@
       <c r="D127" s="10">
         <v>125</v>
       </c>
-      <c r="E127" s="43"/>
+      <c r="E127" s="38"/>
       <c r="F127" s="10">
         <v>7</v>
       </c>
@@ -4964,7 +5066,7 @@
       <c r="D128" s="10">
         <v>126</v>
       </c>
-      <c r="E128" s="43"/>
+      <c r="E128" s="38"/>
       <c r="F128" s="10">
         <v>7</v>
       </c>
@@ -4982,7 +5084,7 @@
       <c r="D129" s="10">
         <v>127</v>
       </c>
-      <c r="E129" s="44"/>
+      <c r="E129" s="39"/>
       <c r="F129" s="10">
         <v>7</v>
       </c>
@@ -5000,7 +5102,7 @@
       <c r="D130" s="10">
         <v>128</v>
       </c>
-      <c r="E130" s="40">
+      <c r="E130" s="43">
         <v>10137</v>
       </c>
       <c r="F130" s="10">
@@ -5020,7 +5122,7 @@
       <c r="D131" s="10">
         <v>129</v>
       </c>
-      <c r="E131" s="43"/>
+      <c r="E131" s="38"/>
       <c r="F131" s="10">
         <v>7</v>
       </c>
@@ -5038,7 +5140,7 @@
       <c r="D132" s="10">
         <v>130</v>
       </c>
-      <c r="E132" s="43"/>
+      <c r="E132" s="38"/>
       <c r="F132" s="10">
         <v>7</v>
       </c>
@@ -5056,7 +5158,7 @@
       <c r="D133" s="10">
         <v>131</v>
       </c>
-      <c r="E133" s="43"/>
+      <c r="E133" s="38"/>
       <c r="F133" s="10">
         <v>7</v>
       </c>
@@ -5074,7 +5176,7 @@
       <c r="D134" s="10">
         <v>132</v>
       </c>
-      <c r="E134" s="43"/>
+      <c r="E134" s="38"/>
       <c r="F134" s="10">
         <v>7</v>
       </c>
@@ -5092,7 +5194,7 @@
       <c r="D135" s="10">
         <v>133</v>
       </c>
-      <c r="E135" s="44"/>
+      <c r="E135" s="39"/>
       <c r="F135" s="10">
         <v>7</v>
       </c>
@@ -5110,7 +5212,7 @@
       <c r="D136" s="10">
         <v>134</v>
       </c>
-      <c r="E136" s="40">
+      <c r="E136" s="43">
         <v>10143</v>
       </c>
       <c r="F136" s="10">
@@ -5130,7 +5232,7 @@
       <c r="D137" s="10">
         <v>135</v>
       </c>
-      <c r="E137" s="43"/>
+      <c r="E137" s="38"/>
       <c r="F137" s="10">
         <v>7</v>
       </c>
@@ -5148,7 +5250,7 @@
       <c r="D138" s="10">
         <v>136</v>
       </c>
-      <c r="E138" s="43"/>
+      <c r="E138" s="38"/>
       <c r="F138" s="10">
         <v>7</v>
       </c>
@@ -5166,7 +5268,7 @@
       <c r="D139" s="10">
         <v>137</v>
       </c>
-      <c r="E139" s="43"/>
+      <c r="E139" s="38"/>
       <c r="F139" s="10">
         <v>7</v>
       </c>
@@ -5184,7 +5286,7 @@
       <c r="D140" s="10">
         <v>138</v>
       </c>
-      <c r="E140" s="44"/>
+      <c r="E140" s="39"/>
       <c r="F140" s="10">
         <v>7</v>
       </c>
@@ -5200,7 +5302,7 @@
       <c r="D141" s="25">
         <v>199</v>
       </c>
-      <c r="E141" s="45">
+      <c r="E141" s="37">
         <v>10144</v>
       </c>
       <c r="F141" s="25">
@@ -5218,7 +5320,7 @@
       <c r="D142" s="25">
         <v>200</v>
       </c>
-      <c r="E142" s="43"/>
+      <c r="E142" s="38"/>
       <c r="F142" s="25">
         <v>7</v>
       </c>
@@ -5234,7 +5336,7 @@
       <c r="D143" s="25">
         <v>201</v>
       </c>
-      <c r="E143" s="43"/>
+      <c r="E143" s="38"/>
       <c r="F143" s="25">
         <v>7</v>
       </c>
@@ -5250,7 +5352,7 @@
       <c r="D144" s="25">
         <v>202</v>
       </c>
-      <c r="E144" s="43"/>
+      <c r="E144" s="38"/>
       <c r="F144" s="25">
         <v>7</v>
       </c>
@@ -5266,7 +5368,7 @@
       <c r="D145" s="25">
         <v>203</v>
       </c>
-      <c r="E145" s="44"/>
+      <c r="E145" s="39"/>
       <c r="F145" s="25">
         <v>7</v>
       </c>
@@ -5324,7 +5426,7 @@
       <c r="D148" s="10">
         <v>141</v>
       </c>
-      <c r="E148" s="40">
+      <c r="E148" s="43">
         <v>10150</v>
       </c>
       <c r="F148" s="10">
@@ -5344,7 +5446,7 @@
       <c r="D149" s="10">
         <v>142</v>
       </c>
-      <c r="E149" s="43"/>
+      <c r="E149" s="38"/>
       <c r="F149" s="10">
         <v>8</v>
       </c>
@@ -5362,7 +5464,7 @@
       <c r="D150" s="10">
         <v>143</v>
       </c>
-      <c r="E150" s="43"/>
+      <c r="E150" s="38"/>
       <c r="F150" s="10">
         <v>8</v>
       </c>
@@ -5380,7 +5482,7 @@
       <c r="D151" s="10">
         <v>144</v>
       </c>
-      <c r="E151" s="43"/>
+      <c r="E151" s="38"/>
       <c r="F151" s="10">
         <v>8</v>
       </c>
@@ -5398,7 +5500,7 @@
       <c r="D152" s="10">
         <v>145</v>
       </c>
-      <c r="E152" s="43"/>
+      <c r="E152" s="38"/>
       <c r="F152" s="10">
         <v>8</v>
       </c>
@@ -5416,7 +5518,7 @@
       <c r="D153" s="10">
         <v>146</v>
       </c>
-      <c r="E153" s="44"/>
+      <c r="E153" s="39"/>
       <c r="F153" s="10">
         <v>8</v>
       </c>
@@ -5434,7 +5536,7 @@
       <c r="D154" s="10">
         <v>147</v>
       </c>
-      <c r="E154" s="40">
+      <c r="E154" s="43">
         <v>10156</v>
       </c>
       <c r="F154" s="10">
@@ -5454,7 +5556,7 @@
       <c r="D155" s="10">
         <v>148</v>
       </c>
-      <c r="E155" s="43"/>
+      <c r="E155" s="38"/>
       <c r="F155" s="10">
         <v>8</v>
       </c>
@@ -5472,7 +5574,7 @@
       <c r="D156" s="10">
         <v>149</v>
       </c>
-      <c r="E156" s="43"/>
+      <c r="E156" s="38"/>
       <c r="F156" s="10">
         <v>8</v>
       </c>
@@ -5490,7 +5592,7 @@
       <c r="D157" s="10">
         <v>150</v>
       </c>
-      <c r="E157" s="43"/>
+      <c r="E157" s="38"/>
       <c r="F157" s="10">
         <v>8</v>
       </c>
@@ -5508,7 +5610,7 @@
       <c r="D158" s="10">
         <v>151</v>
       </c>
-      <c r="E158" s="43"/>
+      <c r="E158" s="38"/>
       <c r="F158" s="10">
         <v>8</v>
       </c>
@@ -5526,7 +5628,7 @@
       <c r="D159" s="10">
         <v>152</v>
       </c>
-      <c r="E159" s="44"/>
+      <c r="E159" s="39"/>
       <c r="F159" s="10">
         <v>8</v>
       </c>
@@ -5542,7 +5644,7 @@
       <c r="D160" s="25">
         <v>204</v>
       </c>
-      <c r="E160" s="45">
+      <c r="E160" s="37">
         <v>10157</v>
       </c>
       <c r="F160" s="25">
@@ -5560,7 +5662,7 @@
       <c r="D161" s="25">
         <v>205</v>
       </c>
-      <c r="E161" s="43"/>
+      <c r="E161" s="38"/>
       <c r="F161" s="25">
         <v>8</v>
       </c>
@@ -5576,7 +5678,7 @@
       <c r="D162" s="25">
         <v>206</v>
       </c>
-      <c r="E162" s="43"/>
+      <c r="E162" s="38"/>
       <c r="F162" s="25">
         <v>8</v>
       </c>
@@ -5592,7 +5694,7 @@
       <c r="D163" s="25">
         <v>207</v>
       </c>
-      <c r="E163" s="43"/>
+      <c r="E163" s="38"/>
       <c r="F163" s="25">
         <v>8</v>
       </c>
@@ -5608,7 +5710,7 @@
       <c r="D164" s="25">
         <v>208</v>
       </c>
-      <c r="E164" s="44"/>
+      <c r="E164" s="39"/>
       <c r="F164" s="25">
         <v>8</v>
       </c>
@@ -5626,7 +5728,7 @@
       <c r="D165" s="10">
         <v>153</v>
       </c>
-      <c r="E165" s="40">
+      <c r="E165" s="43">
         <v>10162</v>
       </c>
       <c r="F165" s="10">
@@ -5646,7 +5748,7 @@
       <c r="D166" s="10">
         <v>154</v>
       </c>
-      <c r="E166" s="43"/>
+      <c r="E166" s="38"/>
       <c r="F166" s="10">
         <v>9</v>
       </c>
@@ -5664,7 +5766,7 @@
       <c r="D167" s="10">
         <v>155</v>
       </c>
-      <c r="E167" s="43"/>
+      <c r="E167" s="38"/>
       <c r="F167" s="10">
         <v>9</v>
       </c>
@@ -5682,7 +5784,7 @@
       <c r="D168" s="10">
         <v>156</v>
       </c>
-      <c r="E168" s="43"/>
+      <c r="E168" s="38"/>
       <c r="F168" s="10">
         <v>9</v>
       </c>
@@ -5700,7 +5802,7 @@
       <c r="D169" s="10">
         <v>157</v>
       </c>
-      <c r="E169" s="43"/>
+      <c r="E169" s="38"/>
       <c r="F169" s="10">
         <v>9</v>
       </c>
@@ -5718,7 +5820,7 @@
       <c r="D170" s="10">
         <v>158</v>
       </c>
-      <c r="E170" s="44"/>
+      <c r="E170" s="39"/>
       <c r="F170" s="10">
         <v>9</v>
       </c>
@@ -5736,7 +5838,7 @@
       <c r="D171" s="10">
         <v>159</v>
       </c>
-      <c r="E171" s="40">
+      <c r="E171" s="43">
         <v>10168</v>
       </c>
       <c r="F171" s="10">
@@ -5756,7 +5858,7 @@
       <c r="D172" s="10">
         <v>160</v>
       </c>
-      <c r="E172" s="43"/>
+      <c r="E172" s="38"/>
       <c r="F172" s="10">
         <v>9</v>
       </c>
@@ -5774,7 +5876,7 @@
       <c r="D173" s="10">
         <v>161</v>
       </c>
-      <c r="E173" s="43"/>
+      <c r="E173" s="38"/>
       <c r="F173" s="10">
         <v>9</v>
       </c>
@@ -5792,7 +5894,7 @@
       <c r="D174" s="10">
         <v>162</v>
       </c>
-      <c r="E174" s="43"/>
+      <c r="E174" s="38"/>
       <c r="F174" s="10">
         <v>9</v>
       </c>
@@ -5810,7 +5912,7 @@
       <c r="D175" s="10">
         <v>163</v>
       </c>
-      <c r="E175" s="43"/>
+      <c r="E175" s="38"/>
       <c r="F175" s="10">
         <v>9</v>
       </c>
@@ -5828,7 +5930,7 @@
       <c r="D176" s="10">
         <v>164</v>
       </c>
-      <c r="E176" s="44"/>
+      <c r="E176" s="39"/>
       <c r="F176" s="10">
         <v>9</v>
       </c>
@@ -5846,7 +5948,7 @@
       <c r="D177" s="10">
         <v>165</v>
       </c>
-      <c r="E177" s="40">
+      <c r="E177" s="43">
         <v>10174</v>
       </c>
       <c r="F177" s="10">
@@ -5866,7 +5968,7 @@
       <c r="D178" s="10">
         <v>166</v>
       </c>
-      <c r="E178" s="43"/>
+      <c r="E178" s="38"/>
       <c r="F178" s="10">
         <v>9</v>
       </c>
@@ -5884,7 +5986,7 @@
       <c r="D179" s="10">
         <v>167</v>
       </c>
-      <c r="E179" s="43"/>
+      <c r="E179" s="38"/>
       <c r="F179" s="10">
         <v>9</v>
       </c>
@@ -5902,7 +6004,7 @@
       <c r="D180" s="10">
         <v>168</v>
       </c>
-      <c r="E180" s="43"/>
+      <c r="E180" s="38"/>
       <c r="F180" s="10">
         <v>9</v>
       </c>
@@ -5920,7 +6022,7 @@
       <c r="D181" s="10">
         <v>169</v>
       </c>
-      <c r="E181" s="43"/>
+      <c r="E181" s="38"/>
       <c r="F181" s="10">
         <v>9</v>
       </c>
@@ -5938,7 +6040,7 @@
       <c r="D182" s="10">
         <v>170</v>
       </c>
-      <c r="E182" s="44"/>
+      <c r="E182" s="39"/>
       <c r="F182" s="10">
         <v>9</v>
       </c>
@@ -5954,7 +6056,7 @@
       <c r="D183" s="25">
         <v>209</v>
       </c>
-      <c r="E183" s="45">
+      <c r="E183" s="37">
         <v>10175</v>
       </c>
       <c r="F183" s="25">
@@ -5972,7 +6074,7 @@
       <c r="D184" s="25">
         <v>210</v>
       </c>
-      <c r="E184" s="43"/>
+      <c r="E184" s="38"/>
       <c r="F184" s="25">
         <v>9</v>
       </c>
@@ -5988,7 +6090,7 @@
       <c r="D185" s="25">
         <v>211</v>
       </c>
-      <c r="E185" s="43"/>
+      <c r="E185" s="38"/>
       <c r="F185" s="25">
         <v>9</v>
       </c>
@@ -6004,7 +6106,7 @@
       <c r="D186" s="25">
         <v>212</v>
       </c>
-      <c r="E186" s="43"/>
+      <c r="E186" s="38"/>
       <c r="F186" s="25">
         <v>9</v>
       </c>
@@ -6020,7 +6122,7 @@
       <c r="D187" s="25">
         <v>213</v>
       </c>
-      <c r="E187" s="44"/>
+      <c r="E187" s="39"/>
       <c r="F187" s="25">
         <v>9</v>
       </c>
@@ -6038,7 +6140,7 @@
       <c r="D188" s="10">
         <v>171</v>
       </c>
-      <c r="E188" s="37">
+      <c r="E188" s="40">
         <v>10180</v>
       </c>
       <c r="F188" s="10">
@@ -6058,7 +6160,7 @@
       <c r="D189" s="10">
         <v>172</v>
       </c>
-      <c r="E189" s="38"/>
+      <c r="E189" s="41"/>
       <c r="F189" s="10">
         <v>10</v>
       </c>
@@ -6076,7 +6178,7 @@
       <c r="D190" s="10">
         <v>173</v>
       </c>
-      <c r="E190" s="38"/>
+      <c r="E190" s="41"/>
       <c r="F190" s="10">
         <v>10</v>
       </c>
@@ -6094,7 +6196,7 @@
       <c r="D191" s="10">
         <v>174</v>
       </c>
-      <c r="E191" s="38"/>
+      <c r="E191" s="41"/>
       <c r="F191" s="10">
         <v>10</v>
       </c>
@@ -6112,7 +6214,7 @@
       <c r="D192" s="10">
         <v>175</v>
       </c>
-      <c r="E192" s="38"/>
+      <c r="E192" s="41"/>
       <c r="F192" s="10">
         <v>10</v>
       </c>
@@ -6130,7 +6232,7 @@
       <c r="D193" s="10">
         <v>176</v>
       </c>
-      <c r="E193" s="39"/>
+      <c r="E193" s="42"/>
       <c r="F193" s="10">
         <v>10</v>
       </c>
@@ -6146,8 +6248,8 @@
       <c r="D194" s="25">
         <v>214</v>
       </c>
-      <c r="E194" s="45">
-        <v>101181</v>
+      <c r="E194" s="37">
+        <v>10179</v>
       </c>
       <c r="F194" s="25">
         <v>10</v>
@@ -6164,7 +6266,7 @@
       <c r="D195" s="25">
         <v>215</v>
       </c>
-      <c r="E195" s="43"/>
+      <c r="E195" s="38"/>
       <c r="F195" s="25">
         <v>10</v>
       </c>
@@ -6180,7 +6282,7 @@
       <c r="D196" s="25">
         <v>216</v>
       </c>
-      <c r="E196" s="43"/>
+      <c r="E196" s="38"/>
       <c r="F196" s="25">
         <v>10</v>
       </c>
@@ -6196,7 +6298,7 @@
       <c r="D197" s="25">
         <v>217</v>
       </c>
-      <c r="E197" s="43"/>
+      <c r="E197" s="38"/>
       <c r="F197" s="25">
         <v>10</v>
       </c>
@@ -6212,7 +6314,7 @@
       <c r="D198" s="25">
         <v>218</v>
       </c>
-      <c r="E198" s="44"/>
+      <c r="E198" s="39"/>
       <c r="F198" s="25">
         <v>10</v>
       </c>
@@ -6230,7 +6332,7 @@
       <c r="D199" s="10">
         <v>177</v>
       </c>
-      <c r="E199" s="40">
+      <c r="E199" s="43">
         <v>10181</v>
       </c>
       <c r="F199" s="10">
@@ -6250,7 +6352,7 @@
       <c r="D200" s="10">
         <v>178</v>
       </c>
-      <c r="E200" s="41"/>
+      <c r="E200" s="44"/>
       <c r="F200" s="10">
         <v>11</v>
       </c>
@@ -6268,7 +6370,7 @@
       <c r="D201" s="10">
         <v>179</v>
       </c>
-      <c r="E201" s="41"/>
+      <c r="E201" s="44"/>
       <c r="F201" s="10">
         <v>11</v>
       </c>
@@ -6286,7 +6388,7 @@
       <c r="D202" s="10">
         <v>180</v>
       </c>
-      <c r="E202" s="41"/>
+      <c r="E202" s="44"/>
       <c r="F202" s="10">
         <v>11</v>
       </c>
@@ -6304,7 +6406,7 @@
       <c r="D203" s="10">
         <v>181</v>
       </c>
-      <c r="E203" s="41"/>
+      <c r="E203" s="44"/>
       <c r="F203" s="10">
         <v>11</v>
       </c>
@@ -6322,7 +6424,7 @@
       <c r="D204" s="10">
         <v>182</v>
       </c>
-      <c r="E204" s="42"/>
+      <c r="E204" s="45"/>
       <c r="F204" s="10">
         <v>11</v>
       </c>
@@ -6340,7 +6442,7 @@
       <c r="D205" s="10">
         <v>183</v>
       </c>
-      <c r="E205" s="40">
+      <c r="E205" s="43">
         <v>10182</v>
       </c>
       <c r="F205" s="10">
@@ -6360,7 +6462,7 @@
       <c r="D206" s="10">
         <v>184</v>
       </c>
-      <c r="E206" s="41"/>
+      <c r="E206" s="44"/>
       <c r="F206" s="10">
         <v>11</v>
       </c>
@@ -6378,7 +6480,7 @@
       <c r="D207" s="10">
         <v>185</v>
       </c>
-      <c r="E207" s="41"/>
+      <c r="E207" s="44"/>
       <c r="F207" s="10">
         <v>11</v>
       </c>
@@ -6396,7 +6498,7 @@
       <c r="D208" s="10">
         <v>186</v>
       </c>
-      <c r="E208" s="41"/>
+      <c r="E208" s="44"/>
       <c r="F208" s="10">
         <v>11</v>
       </c>
@@ -6414,7 +6516,7 @@
       <c r="D209" s="10">
         <v>187</v>
       </c>
-      <c r="E209" s="42"/>
+      <c r="E209" s="45"/>
       <c r="F209" s="10">
         <v>11</v>
       </c>
@@ -6432,7 +6534,7 @@
       <c r="D210" s="10">
         <v>188</v>
       </c>
-      <c r="E210" s="40">
+      <c r="E210" s="43">
         <v>10197</v>
       </c>
       <c r="F210" s="10">
@@ -6452,7 +6554,7 @@
       <c r="D211" s="10">
         <v>189</v>
       </c>
-      <c r="E211" s="43"/>
+      <c r="E211" s="38"/>
       <c r="F211" s="10">
         <v>11</v>
       </c>
@@ -6470,7 +6572,7 @@
       <c r="D212" s="10">
         <v>190</v>
       </c>
-      <c r="E212" s="43"/>
+      <c r="E212" s="38"/>
       <c r="F212" s="10">
         <v>11</v>
       </c>
@@ -6488,7 +6590,7 @@
       <c r="D213" s="10">
         <v>191</v>
       </c>
-      <c r="E213" s="43"/>
+      <c r="E213" s="38"/>
       <c r="F213" s="10">
         <v>11</v>
       </c>
@@ -6506,7 +6608,7 @@
       <c r="D214" s="10">
         <v>192</v>
       </c>
-      <c r="E214" s="44"/>
+      <c r="E214" s="39"/>
       <c r="F214" s="10">
         <v>11</v>
       </c>
@@ -6524,7 +6626,7 @@
       <c r="D215" s="10">
         <v>193</v>
       </c>
-      <c r="E215" s="40">
+      <c r="E215" s="43">
         <v>10202</v>
       </c>
       <c r="F215" s="10">
@@ -6544,7 +6646,7 @@
       <c r="D216" s="10">
         <v>194</v>
       </c>
-      <c r="E216" s="43"/>
+      <c r="E216" s="38"/>
       <c r="F216" s="10">
         <v>11</v>
       </c>
@@ -6562,7 +6664,7 @@
       <c r="D217" s="10">
         <v>195</v>
       </c>
-      <c r="E217" s="43"/>
+      <c r="E217" s="38"/>
       <c r="F217" s="10">
         <v>11</v>
       </c>
@@ -6580,7 +6682,7 @@
       <c r="D218" s="10">
         <v>196</v>
       </c>
-      <c r="E218" s="43"/>
+      <c r="E218" s="38"/>
       <c r="F218" s="10">
         <v>11</v>
       </c>
@@ -6598,7 +6700,7 @@
       <c r="D219" s="10">
         <v>197</v>
       </c>
-      <c r="E219" s="43"/>
+      <c r="E219" s="38"/>
       <c r="F219" s="10">
         <v>11</v>
       </c>
@@ -6616,7 +6718,7 @@
       <c r="D220" s="10">
         <v>198</v>
       </c>
-      <c r="E220" s="44"/>
+      <c r="E220" s="39"/>
       <c r="F220" s="10">
         <v>11</v>
       </c>
@@ -6624,30 +6726,260 @@
         <v>387</v>
       </c>
     </row>
-    <row r="222" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="223" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B223" s="22" t="s">
+    <row r="221" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B221" s="48" t="s">
+        <v>666</v>
+      </c>
+      <c r="C221" s="49"/>
+      <c r="D221" s="50">
+        <v>219</v>
+      </c>
+      <c r="E221" s="51">
+        <v>10210</v>
+      </c>
+      <c r="F221" s="50" t="s">
+        <v>690</v>
+      </c>
+      <c r="G221" s="50" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="222" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B222" s="48" t="s">
+        <v>668</v>
+      </c>
+      <c r="C222" s="49"/>
+      <c r="D222" s="50">
+        <v>220</v>
+      </c>
+      <c r="E222" s="52"/>
+      <c r="F222" s="50" t="s">
+        <v>690</v>
+      </c>
+      <c r="G222" s="50" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="223" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B223" s="48" t="s">
+        <v>669</v>
+      </c>
+      <c r="C223" s="49"/>
+      <c r="D223" s="50">
+        <v>221</v>
+      </c>
+      <c r="E223" s="52"/>
+      <c r="F223" s="50" t="s">
+        <v>690</v>
+      </c>
+      <c r="G223" s="50" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="224" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B224" s="48" t="s">
+        <v>670</v>
+      </c>
+      <c r="C224" s="49"/>
+      <c r="D224" s="50">
+        <v>222</v>
+      </c>
+      <c r="E224" s="52"/>
+      <c r="F224" s="50" t="s">
+        <v>690</v>
+      </c>
+      <c r="G224" s="50" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="225" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B225" s="48" t="s">
+        <v>671</v>
+      </c>
+      <c r="C225" s="49"/>
+      <c r="D225" s="50">
+        <v>223</v>
+      </c>
+      <c r="E225" s="53"/>
+      <c r="F225" s="50" t="s">
+        <v>690</v>
+      </c>
+      <c r="G225" s="50" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="226" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B226" s="48" t="s">
+        <v>667</v>
+      </c>
+      <c r="C226" s="49"/>
+      <c r="D226" s="50">
+        <v>224</v>
+      </c>
+      <c r="E226" s="51">
+        <v>10211</v>
+      </c>
+      <c r="F226" s="50" t="s">
+        <v>690</v>
+      </c>
+      <c r="G226" s="50" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="227" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B227" s="48" t="s">
+        <v>674</v>
+      </c>
+      <c r="C227" s="49"/>
+      <c r="D227" s="50">
+        <v>225</v>
+      </c>
+      <c r="E227" s="52"/>
+      <c r="F227" s="50" t="s">
+        <v>690</v>
+      </c>
+      <c r="G227" s="50" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="228" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B228" s="48" t="s">
+        <v>675</v>
+      </c>
+      <c r="C228" s="49"/>
+      <c r="D228" s="50">
+        <v>226</v>
+      </c>
+      <c r="E228" s="52"/>
+      <c r="F228" s="50" t="s">
+        <v>690</v>
+      </c>
+      <c r="G228" s="50" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="229" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B229" s="48" t="s">
+        <v>676</v>
+      </c>
+      <c r="C229" s="49"/>
+      <c r="D229" s="50">
+        <v>227</v>
+      </c>
+      <c r="E229" s="52"/>
+      <c r="F229" s="50" t="s">
+        <v>690</v>
+      </c>
+      <c r="G229" s="50" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="230" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B230" s="48" t="s">
+        <v>677</v>
+      </c>
+      <c r="C230" s="49"/>
+      <c r="D230" s="50">
+        <v>228</v>
+      </c>
+      <c r="E230" s="53"/>
+      <c r="F230" s="50" t="s">
+        <v>690</v>
+      </c>
+      <c r="G230" s="50" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="231" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B231" s="48" t="s">
+        <v>687</v>
+      </c>
+      <c r="C231" s="49"/>
+      <c r="D231" s="50">
+        <v>219</v>
+      </c>
+      <c r="E231" s="55">
+        <v>10212</v>
+      </c>
+      <c r="F231" s="50" t="s">
+        <v>690</v>
+      </c>
+      <c r="G231" s="50" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="232" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B232" s="48" t="s">
+        <v>688</v>
+      </c>
+      <c r="C232" s="49"/>
+      <c r="D232" s="50">
+        <v>219</v>
+      </c>
+      <c r="E232" s="55">
+        <v>10213</v>
+      </c>
+      <c r="F232" s="50" t="s">
+        <v>690</v>
+      </c>
+      <c r="G232" s="50" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="234" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="235" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B235" s="22" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="224" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B224" s="2"/>
-    </row>
-    <row r="225" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B225" s="26" t="s">
+    <row r="236" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B236" s="2"/>
+    </row>
+    <row r="237" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B237" s="26" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="226" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B226" s="2"/>
-    </row>
-    <row r="227" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B227" s="28" t="s">
+    <row r="238" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B238" s="2"/>
+    </row>
+    <row r="239" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B239" s="28" t="s">
         <v>644</v>
       </c>
     </row>
+    <row r="240" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="241" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B241" s="54" t="s">
+        <v>665</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="40">
+    <mergeCell ref="E215:E220"/>
+    <mergeCell ref="E221:E225"/>
+    <mergeCell ref="E226:E230"/>
+    <mergeCell ref="E160:E164"/>
+    <mergeCell ref="E188:E193"/>
+    <mergeCell ref="E199:E204"/>
+    <mergeCell ref="E205:E209"/>
+    <mergeCell ref="E210:E214"/>
+    <mergeCell ref="E75:E79"/>
+    <mergeCell ref="E80:E84"/>
+    <mergeCell ref="E88:E93"/>
+    <mergeCell ref="E94:E98"/>
+    <mergeCell ref="E177:E182"/>
+    <mergeCell ref="E110:E113"/>
+    <mergeCell ref="E114:E117"/>
+    <mergeCell ref="E118:E123"/>
+    <mergeCell ref="E124:E129"/>
+    <mergeCell ref="E130:E135"/>
+    <mergeCell ref="E136:E140"/>
+    <mergeCell ref="E148:E153"/>
+    <mergeCell ref="E154:E159"/>
+    <mergeCell ref="E165:E170"/>
+    <mergeCell ref="E171:E176"/>
+    <mergeCell ref="E141:E145"/>
     <mergeCell ref="E183:E187"/>
     <mergeCell ref="E194:E198"/>
     <mergeCell ref="E3:E8"/>
@@ -6664,28 +6996,6 @@
     <mergeCell ref="E55:E60"/>
     <mergeCell ref="E64:E69"/>
     <mergeCell ref="E70:E74"/>
-    <mergeCell ref="E75:E79"/>
-    <mergeCell ref="E80:E84"/>
-    <mergeCell ref="E88:E93"/>
-    <mergeCell ref="E94:E98"/>
-    <mergeCell ref="E177:E182"/>
-    <mergeCell ref="E110:E113"/>
-    <mergeCell ref="E114:E117"/>
-    <mergeCell ref="E118:E123"/>
-    <mergeCell ref="E124:E129"/>
-    <mergeCell ref="E130:E135"/>
-    <mergeCell ref="E136:E140"/>
-    <mergeCell ref="E148:E153"/>
-    <mergeCell ref="E154:E159"/>
-    <mergeCell ref="E165:E170"/>
-    <mergeCell ref="E171:E176"/>
-    <mergeCell ref="E141:E145"/>
-    <mergeCell ref="E160:E164"/>
-    <mergeCell ref="E188:E193"/>
-    <mergeCell ref="E199:E204"/>
-    <mergeCell ref="E205:E209"/>
-    <mergeCell ref="E210:E214"/>
-    <mergeCell ref="E215:E220"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
fix data for Olvia
</commit_message>
<xml_diff>
--- a/Documentation/База_данных_Арселор-Точки_измерения.xlsx
+++ b/Documentation/База_данных_Арселор-Точки_измерения.xlsx
@@ -2378,13 +2378,34 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2394,9 +2415,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2409,24 +2427,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2714,8 +2714,8 @@
   </sheetPr>
   <dimension ref="B2:G241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G238" sqref="G238"/>
+    <sheetView tabSelected="1" topLeftCell="A193" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B231" sqref="B231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2758,7 +2758,7 @@
       <c r="D3" s="10">
         <v>1</v>
       </c>
-      <c r="E3" s="40">
+      <c r="E3" s="49">
         <v>10010</v>
       </c>
       <c r="F3" s="10">
@@ -2778,7 +2778,7 @@
       <c r="D4" s="10">
         <v>2</v>
       </c>
-      <c r="E4" s="41"/>
+      <c r="E4" s="50"/>
       <c r="F4" s="10">
         <v>1</v>
       </c>
@@ -2796,7 +2796,7 @@
       <c r="D5" s="10">
         <v>3</v>
       </c>
-      <c r="E5" s="41"/>
+      <c r="E5" s="50"/>
       <c r="F5" s="10">
         <v>1</v>
       </c>
@@ -2814,7 +2814,7 @@
       <c r="D6" s="10">
         <v>4</v>
       </c>
-      <c r="E6" s="41"/>
+      <c r="E6" s="50"/>
       <c r="F6" s="10">
         <v>1</v>
       </c>
@@ -2832,7 +2832,7 @@
       <c r="D7" s="10">
         <v>5</v>
       </c>
-      <c r="E7" s="41"/>
+      <c r="E7" s="50"/>
       <c r="F7" s="10">
         <v>1</v>
       </c>
@@ -2850,7 +2850,7 @@
       <c r="D8" s="10">
         <v>6</v>
       </c>
-      <c r="E8" s="42"/>
+      <c r="E8" s="51"/>
       <c r="F8" s="10">
         <v>1</v>
       </c>
@@ -2868,7 +2868,7 @@
       <c r="D9" s="10">
         <v>7</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="42">
         <v>10016</v>
       </c>
       <c r="F9" s="10">
@@ -2888,7 +2888,7 @@
       <c r="D10" s="10">
         <v>8</v>
       </c>
-      <c r="E10" s="38"/>
+      <c r="E10" s="43"/>
       <c r="F10" s="10">
         <v>2</v>
       </c>
@@ -2906,7 +2906,7 @@
       <c r="D11" s="10">
         <v>9</v>
       </c>
-      <c r="E11" s="38"/>
+      <c r="E11" s="43"/>
       <c r="F11" s="10">
         <v>2</v>
       </c>
@@ -2924,7 +2924,7 @@
       <c r="D12" s="10">
         <v>10</v>
       </c>
-      <c r="E12" s="38"/>
+      <c r="E12" s="43"/>
       <c r="F12" s="10">
         <v>2</v>
       </c>
@@ -2942,7 +2942,7 @@
       <c r="D13" s="10">
         <v>11</v>
       </c>
-      <c r="E13" s="38"/>
+      <c r="E13" s="43"/>
       <c r="F13" s="10">
         <v>2</v>
       </c>
@@ -2960,7 +2960,7 @@
       <c r="D14" s="10">
         <v>12</v>
       </c>
-      <c r="E14" s="39"/>
+      <c r="E14" s="44"/>
       <c r="F14" s="10">
         <v>2</v>
       </c>
@@ -2978,7 +2978,7 @@
       <c r="D15" s="10">
         <v>13</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E15" s="42">
         <v>10022</v>
       </c>
       <c r="F15" s="10">
@@ -2998,7 +2998,7 @@
       <c r="D16" s="10">
         <v>14</v>
       </c>
-      <c r="E16" s="38"/>
+      <c r="E16" s="43"/>
       <c r="F16" s="10">
         <v>2</v>
       </c>
@@ -3016,7 +3016,7 @@
       <c r="D17" s="10">
         <v>15</v>
       </c>
-      <c r="E17" s="38"/>
+      <c r="E17" s="43"/>
       <c r="F17" s="10">
         <v>2</v>
       </c>
@@ -3034,7 +3034,7 @@
       <c r="D18" s="10">
         <v>16</v>
       </c>
-      <c r="E18" s="38"/>
+      <c r="E18" s="43"/>
       <c r="F18" s="10">
         <v>2</v>
       </c>
@@ -3052,7 +3052,7 @@
       <c r="D19" s="10">
         <v>17</v>
       </c>
-      <c r="E19" s="38"/>
+      <c r="E19" s="43"/>
       <c r="F19" s="10">
         <v>2</v>
       </c>
@@ -3070,7 +3070,7 @@
       <c r="D20" s="10">
         <v>18</v>
       </c>
-      <c r="E20" s="39"/>
+      <c r="E20" s="44"/>
       <c r="F20" s="10">
         <v>2</v>
       </c>
@@ -3088,7 +3088,7 @@
       <c r="D21" s="10">
         <v>19</v>
       </c>
-      <c r="E21" s="43">
+      <c r="E21" s="42">
         <v>10028</v>
       </c>
       <c r="F21" s="10">
@@ -3108,7 +3108,7 @@
       <c r="D22" s="10">
         <v>20</v>
       </c>
-      <c r="E22" s="38"/>
+      <c r="E22" s="43"/>
       <c r="F22" s="10">
         <v>2</v>
       </c>
@@ -3126,7 +3126,7 @@
       <c r="D23" s="10">
         <v>21</v>
       </c>
-      <c r="E23" s="38"/>
+      <c r="E23" s="43"/>
       <c r="F23" s="10">
         <v>2</v>
       </c>
@@ -3144,7 +3144,7 @@
       <c r="D24" s="10">
         <v>22</v>
       </c>
-      <c r="E24" s="38"/>
+      <c r="E24" s="43"/>
       <c r="F24" s="10">
         <v>2</v>
       </c>
@@ -3162,7 +3162,7 @@
       <c r="D25" s="10">
         <v>23</v>
       </c>
-      <c r="E25" s="38"/>
+      <c r="E25" s="43"/>
       <c r="F25" s="10">
         <v>2</v>
       </c>
@@ -3180,7 +3180,7 @@
       <c r="D26" s="10">
         <v>24</v>
       </c>
-      <c r="E26" s="39"/>
+      <c r="E26" s="44"/>
       <c r="F26" s="10">
         <v>2</v>
       </c>
@@ -3198,7 +3198,7 @@
       <c r="D27" s="10">
         <v>25</v>
       </c>
-      <c r="E27" s="43">
+      <c r="E27" s="42">
         <v>10034</v>
       </c>
       <c r="F27" s="10">
@@ -3218,7 +3218,7 @@
       <c r="D28" s="10">
         <v>26</v>
       </c>
-      <c r="E28" s="38"/>
+      <c r="E28" s="43"/>
       <c r="F28" s="10">
         <v>2</v>
       </c>
@@ -3236,7 +3236,7 @@
       <c r="D29" s="10">
         <v>27</v>
       </c>
-      <c r="E29" s="38"/>
+      <c r="E29" s="43"/>
       <c r="F29" s="10">
         <v>2</v>
       </c>
@@ -3254,7 +3254,7 @@
       <c r="D30" s="10">
         <v>28</v>
       </c>
-      <c r="E30" s="38"/>
+      <c r="E30" s="43"/>
       <c r="F30" s="10">
         <v>2</v>
       </c>
@@ -3272,7 +3272,7 @@
       <c r="D31" s="10">
         <v>29</v>
       </c>
-      <c r="E31" s="38"/>
+      <c r="E31" s="43"/>
       <c r="F31" s="10">
         <v>2</v>
       </c>
@@ -3290,7 +3290,7 @@
       <c r="D32" s="10">
         <v>30</v>
       </c>
-      <c r="E32" s="39"/>
+      <c r="E32" s="44"/>
       <c r="F32" s="10">
         <v>2</v>
       </c>
@@ -3308,7 +3308,7 @@
       <c r="D33" s="10">
         <v>31</v>
       </c>
-      <c r="E33" s="43">
+      <c r="E33" s="42">
         <v>10040</v>
       </c>
       <c r="F33" s="10">
@@ -3328,7 +3328,7 @@
       <c r="D34" s="10">
         <v>32</v>
       </c>
-      <c r="E34" s="38"/>
+      <c r="E34" s="43"/>
       <c r="F34" s="10">
         <v>2</v>
       </c>
@@ -3346,7 +3346,7 @@
       <c r="D35" s="10">
         <v>33</v>
       </c>
-      <c r="E35" s="38"/>
+      <c r="E35" s="43"/>
       <c r="F35" s="10">
         <v>2</v>
       </c>
@@ -3364,7 +3364,7 @@
       <c r="D36" s="10">
         <v>34</v>
       </c>
-      <c r="E36" s="38"/>
+      <c r="E36" s="43"/>
       <c r="F36" s="10">
         <v>2</v>
       </c>
@@ -3382,7 +3382,7 @@
       <c r="D37" s="10">
         <v>35</v>
       </c>
-      <c r="E37" s="38"/>
+      <c r="E37" s="43"/>
       <c r="F37" s="10">
         <v>2</v>
       </c>
@@ -3400,7 +3400,7 @@
       <c r="D38" s="10">
         <v>36</v>
       </c>
-      <c r="E38" s="39"/>
+      <c r="E38" s="44"/>
       <c r="F38" s="10">
         <v>2</v>
       </c>
@@ -3418,7 +3418,7 @@
       <c r="D39" s="10">
         <v>37</v>
       </c>
-      <c r="E39" s="43">
+      <c r="E39" s="42">
         <v>10046</v>
       </c>
       <c r="F39" s="10">
@@ -3438,7 +3438,7 @@
       <c r="D40" s="10">
         <v>38</v>
       </c>
-      <c r="E40" s="38"/>
+      <c r="E40" s="43"/>
       <c r="F40" s="10">
         <v>3</v>
       </c>
@@ -3456,7 +3456,7 @@
       <c r="D41" s="10">
         <v>39</v>
       </c>
-      <c r="E41" s="38"/>
+      <c r="E41" s="43"/>
       <c r="F41" s="10">
         <v>3</v>
       </c>
@@ -3474,7 +3474,7 @@
       <c r="D42" s="10">
         <v>40</v>
       </c>
-      <c r="E42" s="38"/>
+      <c r="E42" s="43"/>
       <c r="F42" s="10">
         <v>3</v>
       </c>
@@ -3492,7 +3492,7 @@
       <c r="D43" s="10">
         <v>41</v>
       </c>
-      <c r="E43" s="38"/>
+      <c r="E43" s="43"/>
       <c r="F43" s="10">
         <v>3</v>
       </c>
@@ -3510,7 +3510,7 @@
       <c r="D44" s="10">
         <v>42</v>
       </c>
-      <c r="E44" s="39"/>
+      <c r="E44" s="44"/>
       <c r="F44" s="10">
         <v>3</v>
       </c>
@@ -3528,7 +3528,7 @@
       <c r="D45" s="10">
         <v>43</v>
       </c>
-      <c r="E45" s="43">
+      <c r="E45" s="42">
         <v>10052</v>
       </c>
       <c r="F45" s="10">
@@ -3548,7 +3548,7 @@
       <c r="D46" s="10">
         <v>44</v>
       </c>
-      <c r="E46" s="38"/>
+      <c r="E46" s="43"/>
       <c r="F46" s="10">
         <v>3</v>
       </c>
@@ -3566,7 +3566,7 @@
       <c r="D47" s="10">
         <v>45</v>
       </c>
-      <c r="E47" s="38"/>
+      <c r="E47" s="43"/>
       <c r="F47" s="10">
         <v>3</v>
       </c>
@@ -3584,7 +3584,7 @@
       <c r="D48" s="10">
         <v>46</v>
       </c>
-      <c r="E48" s="38"/>
+      <c r="E48" s="43"/>
       <c r="F48" s="10">
         <v>3</v>
       </c>
@@ -3602,7 +3602,7 @@
       <c r="D49" s="10">
         <v>47</v>
       </c>
-      <c r="E49" s="39"/>
+      <c r="E49" s="44"/>
       <c r="F49" s="10">
         <v>3</v>
       </c>
@@ -3620,7 +3620,7 @@
       <c r="D50" s="10">
         <v>48</v>
       </c>
-      <c r="E50" s="43">
+      <c r="E50" s="42">
         <v>10053</v>
       </c>
       <c r="F50" s="10">
@@ -3640,7 +3640,7 @@
       <c r="D51" s="10">
         <v>49</v>
       </c>
-      <c r="E51" s="44"/>
+      <c r="E51" s="52"/>
       <c r="F51" s="10">
         <v>3</v>
       </c>
@@ -3658,7 +3658,7 @@
       <c r="D52" s="10">
         <v>50</v>
       </c>
-      <c r="E52" s="44"/>
+      <c r="E52" s="52"/>
       <c r="F52" s="10">
         <v>3</v>
       </c>
@@ -3676,7 +3676,7 @@
       <c r="D53" s="10">
         <v>51</v>
       </c>
-      <c r="E53" s="44"/>
+      <c r="E53" s="52"/>
       <c r="F53" s="10">
         <v>3</v>
       </c>
@@ -3694,7 +3694,7 @@
       <c r="D54" s="10">
         <v>52</v>
       </c>
-      <c r="E54" s="45"/>
+      <c r="E54" s="53"/>
       <c r="F54" s="10">
         <v>3</v>
       </c>
@@ -3712,7 +3712,7 @@
       <c r="D55" s="10">
         <v>53</v>
       </c>
-      <c r="E55" s="43">
+      <c r="E55" s="42">
         <v>10062</v>
       </c>
       <c r="F55" s="10">
@@ -3732,7 +3732,7 @@
       <c r="D56" s="10">
         <v>54</v>
       </c>
-      <c r="E56" s="38"/>
+      <c r="E56" s="43"/>
       <c r="F56" s="10">
         <v>3</v>
       </c>
@@ -3750,7 +3750,7 @@
       <c r="D57" s="10">
         <v>55</v>
       </c>
-      <c r="E57" s="38"/>
+      <c r="E57" s="43"/>
       <c r="F57" s="10">
         <v>3</v>
       </c>
@@ -3768,7 +3768,7 @@
       <c r="D58" s="10">
         <v>56</v>
       </c>
-      <c r="E58" s="38"/>
+      <c r="E58" s="43"/>
       <c r="F58" s="10">
         <v>3</v>
       </c>
@@ -3786,7 +3786,7 @@
       <c r="D59" s="10">
         <v>57</v>
       </c>
-      <c r="E59" s="38"/>
+      <c r="E59" s="43"/>
       <c r="F59" s="10">
         <v>3</v>
       </c>
@@ -3804,7 +3804,7 @@
       <c r="D60" s="10">
         <v>58</v>
       </c>
-      <c r="E60" s="39"/>
+      <c r="E60" s="44"/>
       <c r="F60" s="10">
         <v>3</v>
       </c>
@@ -3882,7 +3882,7 @@
       <c r="D64" s="10">
         <v>62</v>
       </c>
-      <c r="E64" s="40">
+      <c r="E64" s="49">
         <v>10071</v>
       </c>
       <c r="F64" s="10">
@@ -3902,7 +3902,7 @@
       <c r="D65" s="10">
         <v>63</v>
       </c>
-      <c r="E65" s="41"/>
+      <c r="E65" s="50"/>
       <c r="F65" s="10">
         <v>4</v>
       </c>
@@ -3920,7 +3920,7 @@
       <c r="D66" s="10">
         <v>64</v>
       </c>
-      <c r="E66" s="41"/>
+      <c r="E66" s="50"/>
       <c r="F66" s="10">
         <v>4</v>
       </c>
@@ -3938,7 +3938,7 @@
       <c r="D67" s="10">
         <v>65</v>
       </c>
-      <c r="E67" s="41"/>
+      <c r="E67" s="50"/>
       <c r="F67" s="10">
         <v>4</v>
       </c>
@@ -3956,7 +3956,7 @@
       <c r="D68" s="10">
         <v>66</v>
       </c>
-      <c r="E68" s="41"/>
+      <c r="E68" s="50"/>
       <c r="F68" s="10">
         <v>4</v>
       </c>
@@ -3974,7 +3974,7 @@
       <c r="D69" s="10">
         <v>67</v>
       </c>
-      <c r="E69" s="42"/>
+      <c r="E69" s="51"/>
       <c r="F69" s="10">
         <v>4</v>
       </c>
@@ -3992,7 +3992,7 @@
       <c r="D70" s="10">
         <v>68</v>
       </c>
-      <c r="E70" s="40">
+      <c r="E70" s="49">
         <v>10077</v>
       </c>
       <c r="F70" s="10">
@@ -4012,7 +4012,7 @@
       <c r="D71" s="10">
         <v>69</v>
       </c>
-      <c r="E71" s="41"/>
+      <c r="E71" s="50"/>
       <c r="F71" s="10">
         <v>4</v>
       </c>
@@ -4030,7 +4030,7 @@
       <c r="D72" s="10">
         <v>70</v>
       </c>
-      <c r="E72" s="41"/>
+      <c r="E72" s="50"/>
       <c r="F72" s="10">
         <v>4</v>
       </c>
@@ -4048,7 +4048,7 @@
       <c r="D73" s="10">
         <v>71</v>
       </c>
-      <c r="E73" s="41"/>
+      <c r="E73" s="50"/>
       <c r="F73" s="10">
         <v>4</v>
       </c>
@@ -4066,7 +4066,7 @@
       <c r="D74" s="10">
         <v>72</v>
       </c>
-      <c r="E74" s="42"/>
+      <c r="E74" s="51"/>
       <c r="F74" s="10">
         <v>4</v>
       </c>
@@ -4084,7 +4084,7 @@
       <c r="D75" s="10">
         <v>73</v>
       </c>
-      <c r="E75" s="40">
+      <c r="E75" s="49">
         <v>10078</v>
       </c>
       <c r="F75" s="10">
@@ -4104,7 +4104,7 @@
       <c r="D76" s="10">
         <v>74</v>
       </c>
-      <c r="E76" s="41"/>
+      <c r="E76" s="50"/>
       <c r="F76" s="10">
         <v>4</v>
       </c>
@@ -4122,7 +4122,7 @@
       <c r="D77" s="10">
         <v>75</v>
       </c>
-      <c r="E77" s="41"/>
+      <c r="E77" s="50"/>
       <c r="F77" s="10">
         <v>4</v>
       </c>
@@ -4140,7 +4140,7 @@
       <c r="D78" s="10">
         <v>76</v>
       </c>
-      <c r="E78" s="41"/>
+      <c r="E78" s="50"/>
       <c r="F78" s="10">
         <v>4</v>
       </c>
@@ -4158,7 +4158,7 @@
       <c r="D79" s="10">
         <v>77</v>
       </c>
-      <c r="E79" s="42"/>
+      <c r="E79" s="51"/>
       <c r="F79" s="10">
         <v>4</v>
       </c>
@@ -4176,7 +4176,7 @@
       <c r="D80" s="10">
         <v>78</v>
       </c>
-      <c r="E80" s="40">
+      <c r="E80" s="49">
         <v>10087</v>
       </c>
       <c r="F80" s="10">
@@ -4196,7 +4196,7 @@
       <c r="D81" s="10">
         <v>79</v>
       </c>
-      <c r="E81" s="41"/>
+      <c r="E81" s="50"/>
       <c r="F81" s="10">
         <v>4</v>
       </c>
@@ -4214,7 +4214,7 @@
       <c r="D82" s="10">
         <v>80</v>
       </c>
-      <c r="E82" s="41"/>
+      <c r="E82" s="50"/>
       <c r="F82" s="10">
         <v>4</v>
       </c>
@@ -4232,7 +4232,7 @@
       <c r="D83" s="10">
         <v>81</v>
       </c>
-      <c r="E83" s="41"/>
+      <c r="E83" s="50"/>
       <c r="F83" s="10">
         <v>4</v>
       </c>
@@ -4250,7 +4250,7 @@
       <c r="D84" s="10">
         <v>82</v>
       </c>
-      <c r="E84" s="42"/>
+      <c r="E84" s="51"/>
       <c r="F84" s="10">
         <v>4</v>
       </c>
@@ -4328,7 +4328,7 @@
       <c r="D88" s="10">
         <v>86</v>
       </c>
-      <c r="E88" s="43">
+      <c r="E88" s="42">
         <v>10095</v>
       </c>
       <c r="F88" s="10">
@@ -4348,7 +4348,7 @@
       <c r="D89" s="10">
         <v>87</v>
       </c>
-      <c r="E89" s="38"/>
+      <c r="E89" s="43"/>
       <c r="F89" s="10">
         <v>5</v>
       </c>
@@ -4366,7 +4366,7 @@
       <c r="D90" s="10">
         <v>88</v>
       </c>
-      <c r="E90" s="38"/>
+      <c r="E90" s="43"/>
       <c r="F90" s="10">
         <v>5</v>
       </c>
@@ -4384,7 +4384,7 @@
       <c r="D91" s="10">
         <v>89</v>
       </c>
-      <c r="E91" s="38"/>
+      <c r="E91" s="43"/>
       <c r="F91" s="10">
         <v>5</v>
       </c>
@@ -4402,7 +4402,7 @@
       <c r="D92" s="10">
         <v>90</v>
       </c>
-      <c r="E92" s="38"/>
+      <c r="E92" s="43"/>
       <c r="F92" s="10">
         <v>5</v>
       </c>
@@ -4420,7 +4420,7 @@
       <c r="D93" s="10">
         <v>91</v>
       </c>
-      <c r="E93" s="39"/>
+      <c r="E93" s="44"/>
       <c r="F93" s="10">
         <v>5</v>
       </c>
@@ -4438,7 +4438,7 @@
       <c r="D94" s="10">
         <v>92</v>
       </c>
-      <c r="E94" s="43">
+      <c r="E94" s="42">
         <v>10101</v>
       </c>
       <c r="F94" s="10">
@@ -4458,7 +4458,7 @@
       <c r="D95" s="10">
         <v>93</v>
       </c>
-      <c r="E95" s="38"/>
+      <c r="E95" s="43"/>
       <c r="F95" s="10">
         <v>5</v>
       </c>
@@ -4476,7 +4476,7 @@
       <c r="D96" s="10">
         <v>94</v>
       </c>
-      <c r="E96" s="38"/>
+      <c r="E96" s="43"/>
       <c r="F96" s="10">
         <v>5</v>
       </c>
@@ -4494,7 +4494,7 @@
       <c r="D97" s="10">
         <v>95</v>
       </c>
-      <c r="E97" s="38"/>
+      <c r="E97" s="43"/>
       <c r="F97" s="10">
         <v>5</v>
       </c>
@@ -4512,7 +4512,7 @@
       <c r="D98" s="10">
         <v>96</v>
       </c>
-      <c r="E98" s="39"/>
+      <c r="E98" s="44"/>
       <c r="F98" s="10">
         <v>5</v>
       </c>
@@ -4530,7 +4530,7 @@
       <c r="D99" s="10">
         <v>97</v>
       </c>
-      <c r="E99" s="43">
+      <c r="E99" s="42">
         <v>10107</v>
       </c>
       <c r="F99" s="10">
@@ -4550,7 +4550,7 @@
       <c r="D100" s="10">
         <v>98</v>
       </c>
-      <c r="E100" s="38"/>
+      <c r="E100" s="43"/>
       <c r="F100" s="10">
         <v>5</v>
       </c>
@@ -4568,7 +4568,7 @@
       <c r="D101" s="10">
         <v>99</v>
       </c>
-      <c r="E101" s="38"/>
+      <c r="E101" s="43"/>
       <c r="F101" s="10">
         <v>5</v>
       </c>
@@ -4586,7 +4586,7 @@
       <c r="D102" s="10">
         <v>100</v>
       </c>
-      <c r="E102" s="38"/>
+      <c r="E102" s="43"/>
       <c r="F102" s="10">
         <v>5</v>
       </c>
@@ -4604,7 +4604,7 @@
       <c r="D103" s="10">
         <v>101</v>
       </c>
-      <c r="E103" s="38"/>
+      <c r="E103" s="43"/>
       <c r="F103" s="10">
         <v>5</v>
       </c>
@@ -4622,7 +4622,7 @@
       <c r="D104" s="10">
         <v>102</v>
       </c>
-      <c r="E104" s="39"/>
+      <c r="E104" s="44"/>
       <c r="F104" s="10">
         <v>5</v>
       </c>
@@ -4660,7 +4660,7 @@
       <c r="D106" s="10">
         <v>104</v>
       </c>
-      <c r="E106" s="41">
+      <c r="E106" s="50">
         <v>10113</v>
       </c>
       <c r="F106" s="10">
@@ -4680,7 +4680,7 @@
       <c r="D107" s="10">
         <v>105</v>
       </c>
-      <c r="E107" s="41"/>
+      <c r="E107" s="50"/>
       <c r="F107" s="10">
         <v>7</v>
       </c>
@@ -4698,7 +4698,7 @@
       <c r="D108" s="10">
         <v>106</v>
       </c>
-      <c r="E108" s="41"/>
+      <c r="E108" s="50"/>
       <c r="F108" s="10">
         <v>7</v>
       </c>
@@ -4716,7 +4716,7 @@
       <c r="D109" s="10">
         <v>107</v>
       </c>
-      <c r="E109" s="42"/>
+      <c r="E109" s="51"/>
       <c r="F109" s="10">
         <v>7</v>
       </c>
@@ -4734,7 +4734,7 @@
       <c r="D110" s="10">
         <v>108</v>
       </c>
-      <c r="E110" s="40">
+      <c r="E110" s="49">
         <v>10117</v>
       </c>
       <c r="F110" s="10">
@@ -4754,7 +4754,7 @@
       <c r="D111" s="10">
         <v>109</v>
       </c>
-      <c r="E111" s="41"/>
+      <c r="E111" s="50"/>
       <c r="F111" s="10">
         <v>7</v>
       </c>
@@ -4772,7 +4772,7 @@
       <c r="D112" s="10">
         <v>110</v>
       </c>
-      <c r="E112" s="41"/>
+      <c r="E112" s="50"/>
       <c r="F112" s="10">
         <v>7</v>
       </c>
@@ -4790,7 +4790,7 @@
       <c r="D113" s="10">
         <v>111</v>
       </c>
-      <c r="E113" s="42"/>
+      <c r="E113" s="51"/>
       <c r="F113" s="10">
         <v>7</v>
       </c>
@@ -4808,7 +4808,7 @@
       <c r="D114" s="10">
         <v>112</v>
       </c>
-      <c r="E114" s="40">
+      <c r="E114" s="49">
         <v>10121</v>
       </c>
       <c r="F114" s="10">
@@ -4828,7 +4828,7 @@
       <c r="D115" s="10">
         <v>113</v>
       </c>
-      <c r="E115" s="41"/>
+      <c r="E115" s="50"/>
       <c r="F115" s="10">
         <v>7</v>
       </c>
@@ -4846,7 +4846,7 @@
       <c r="D116" s="10">
         <v>114</v>
       </c>
-      <c r="E116" s="41"/>
+      <c r="E116" s="50"/>
       <c r="F116" s="10">
         <v>7</v>
       </c>
@@ -4864,7 +4864,7 @@
       <c r="D117" s="10">
         <v>115</v>
       </c>
-      <c r="E117" s="42"/>
+      <c r="E117" s="51"/>
       <c r="F117" s="10">
         <v>7</v>
       </c>
@@ -4882,7 +4882,7 @@
       <c r="D118" s="10">
         <v>116</v>
       </c>
-      <c r="E118" s="43">
+      <c r="E118" s="42">
         <v>10125</v>
       </c>
       <c r="F118" s="10">
@@ -4902,7 +4902,7 @@
       <c r="D119" s="10">
         <v>117</v>
       </c>
-      <c r="E119" s="38"/>
+      <c r="E119" s="43"/>
       <c r="F119" s="10">
         <v>7</v>
       </c>
@@ -4920,7 +4920,7 @@
       <c r="D120" s="10">
         <v>118</v>
       </c>
-      <c r="E120" s="38"/>
+      <c r="E120" s="43"/>
       <c r="F120" s="10">
         <v>7</v>
       </c>
@@ -4938,7 +4938,7 @@
       <c r="D121" s="10">
         <v>119</v>
       </c>
-      <c r="E121" s="38"/>
+      <c r="E121" s="43"/>
       <c r="F121" s="10">
         <v>7</v>
       </c>
@@ -4956,7 +4956,7 @@
       <c r="D122" s="10">
         <v>120</v>
       </c>
-      <c r="E122" s="38"/>
+      <c r="E122" s="43"/>
       <c r="F122" s="10">
         <v>7</v>
       </c>
@@ -4974,7 +4974,7 @@
       <c r="D123" s="10">
         <v>121</v>
       </c>
-      <c r="E123" s="39"/>
+      <c r="E123" s="44"/>
       <c r="F123" s="10">
         <v>7</v>
       </c>
@@ -4992,7 +4992,7 @@
       <c r="D124" s="10">
         <v>122</v>
       </c>
-      <c r="E124" s="43">
+      <c r="E124" s="42">
         <v>10131</v>
       </c>
       <c r="F124" s="10">
@@ -5012,7 +5012,7 @@
       <c r="D125" s="10">
         <v>123</v>
       </c>
-      <c r="E125" s="38"/>
+      <c r="E125" s="43"/>
       <c r="F125" s="10">
         <v>7</v>
       </c>
@@ -5030,7 +5030,7 @@
       <c r="D126" s="10">
         <v>124</v>
       </c>
-      <c r="E126" s="38"/>
+      <c r="E126" s="43"/>
       <c r="F126" s="10">
         <v>7</v>
       </c>
@@ -5048,7 +5048,7 @@
       <c r="D127" s="10">
         <v>125</v>
       </c>
-      <c r="E127" s="38"/>
+      <c r="E127" s="43"/>
       <c r="F127" s="10">
         <v>7</v>
       </c>
@@ -5066,7 +5066,7 @@
       <c r="D128" s="10">
         <v>126</v>
       </c>
-      <c r="E128" s="38"/>
+      <c r="E128" s="43"/>
       <c r="F128" s="10">
         <v>7</v>
       </c>
@@ -5084,7 +5084,7 @@
       <c r="D129" s="10">
         <v>127</v>
       </c>
-      <c r="E129" s="39"/>
+      <c r="E129" s="44"/>
       <c r="F129" s="10">
         <v>7</v>
       </c>
@@ -5102,7 +5102,7 @@
       <c r="D130" s="10">
         <v>128</v>
       </c>
-      <c r="E130" s="43">
+      <c r="E130" s="42">
         <v>10137</v>
       </c>
       <c r="F130" s="10">
@@ -5122,7 +5122,7 @@
       <c r="D131" s="10">
         <v>129</v>
       </c>
-      <c r="E131" s="38"/>
+      <c r="E131" s="43"/>
       <c r="F131" s="10">
         <v>7</v>
       </c>
@@ -5140,7 +5140,7 @@
       <c r="D132" s="10">
         <v>130</v>
       </c>
-      <c r="E132" s="38"/>
+      <c r="E132" s="43"/>
       <c r="F132" s="10">
         <v>7</v>
       </c>
@@ -5158,7 +5158,7 @@
       <c r="D133" s="10">
         <v>131</v>
       </c>
-      <c r="E133" s="38"/>
+      <c r="E133" s="43"/>
       <c r="F133" s="10">
         <v>7</v>
       </c>
@@ -5176,7 +5176,7 @@
       <c r="D134" s="10">
         <v>132</v>
       </c>
-      <c r="E134" s="38"/>
+      <c r="E134" s="43"/>
       <c r="F134" s="10">
         <v>7</v>
       </c>
@@ -5194,7 +5194,7 @@
       <c r="D135" s="10">
         <v>133</v>
       </c>
-      <c r="E135" s="39"/>
+      <c r="E135" s="44"/>
       <c r="F135" s="10">
         <v>7</v>
       </c>
@@ -5212,7 +5212,7 @@
       <c r="D136" s="10">
         <v>134</v>
       </c>
-      <c r="E136" s="43">
+      <c r="E136" s="42">
         <v>10143</v>
       </c>
       <c r="F136" s="10">
@@ -5232,7 +5232,7 @@
       <c r="D137" s="10">
         <v>135</v>
       </c>
-      <c r="E137" s="38"/>
+      <c r="E137" s="43"/>
       <c r="F137" s="10">
         <v>7</v>
       </c>
@@ -5250,7 +5250,7 @@
       <c r="D138" s="10">
         <v>136</v>
       </c>
-      <c r="E138" s="38"/>
+      <c r="E138" s="43"/>
       <c r="F138" s="10">
         <v>7</v>
       </c>
@@ -5268,7 +5268,7 @@
       <c r="D139" s="10">
         <v>137</v>
       </c>
-      <c r="E139" s="38"/>
+      <c r="E139" s="43"/>
       <c r="F139" s="10">
         <v>7</v>
       </c>
@@ -5286,7 +5286,7 @@
       <c r="D140" s="10">
         <v>138</v>
       </c>
-      <c r="E140" s="39"/>
+      <c r="E140" s="44"/>
       <c r="F140" s="10">
         <v>7</v>
       </c>
@@ -5302,7 +5302,7 @@
       <c r="D141" s="25">
         <v>199</v>
       </c>
-      <c r="E141" s="37">
+      <c r="E141" s="48">
         <v>10144</v>
       </c>
       <c r="F141" s="25">
@@ -5320,7 +5320,7 @@
       <c r="D142" s="25">
         <v>200</v>
       </c>
-      <c r="E142" s="38"/>
+      <c r="E142" s="43"/>
       <c r="F142" s="25">
         <v>7</v>
       </c>
@@ -5336,7 +5336,7 @@
       <c r="D143" s="25">
         <v>201</v>
       </c>
-      <c r="E143" s="38"/>
+      <c r="E143" s="43"/>
       <c r="F143" s="25">
         <v>7</v>
       </c>
@@ -5352,7 +5352,7 @@
       <c r="D144" s="25">
         <v>202</v>
       </c>
-      <c r="E144" s="38"/>
+      <c r="E144" s="43"/>
       <c r="F144" s="25">
         <v>7</v>
       </c>
@@ -5368,7 +5368,7 @@
       <c r="D145" s="25">
         <v>203</v>
       </c>
-      <c r="E145" s="39"/>
+      <c r="E145" s="44"/>
       <c r="F145" s="25">
         <v>7</v>
       </c>
@@ -5426,7 +5426,7 @@
       <c r="D148" s="10">
         <v>141</v>
       </c>
-      <c r="E148" s="43">
+      <c r="E148" s="42">
         <v>10150</v>
       </c>
       <c r="F148" s="10">
@@ -5446,7 +5446,7 @@
       <c r="D149" s="10">
         <v>142</v>
       </c>
-      <c r="E149" s="38"/>
+      <c r="E149" s="43"/>
       <c r="F149" s="10">
         <v>8</v>
       </c>
@@ -5464,7 +5464,7 @@
       <c r="D150" s="10">
         <v>143</v>
       </c>
-      <c r="E150" s="38"/>
+      <c r="E150" s="43"/>
       <c r="F150" s="10">
         <v>8</v>
       </c>
@@ -5482,7 +5482,7 @@
       <c r="D151" s="10">
         <v>144</v>
       </c>
-      <c r="E151" s="38"/>
+      <c r="E151" s="43"/>
       <c r="F151" s="10">
         <v>8</v>
       </c>
@@ -5500,7 +5500,7 @@
       <c r="D152" s="10">
         <v>145</v>
       </c>
-      <c r="E152" s="38"/>
+      <c r="E152" s="43"/>
       <c r="F152" s="10">
         <v>8</v>
       </c>
@@ -5518,7 +5518,7 @@
       <c r="D153" s="10">
         <v>146</v>
       </c>
-      <c r="E153" s="39"/>
+      <c r="E153" s="44"/>
       <c r="F153" s="10">
         <v>8</v>
       </c>
@@ -5536,7 +5536,7 @@
       <c r="D154" s="10">
         <v>147</v>
       </c>
-      <c r="E154" s="43">
+      <c r="E154" s="42">
         <v>10156</v>
       </c>
       <c r="F154" s="10">
@@ -5556,7 +5556,7 @@
       <c r="D155" s="10">
         <v>148</v>
       </c>
-      <c r="E155" s="38"/>
+      <c r="E155" s="43"/>
       <c r="F155" s="10">
         <v>8</v>
       </c>
@@ -5574,7 +5574,7 @@
       <c r="D156" s="10">
         <v>149</v>
       </c>
-      <c r="E156" s="38"/>
+      <c r="E156" s="43"/>
       <c r="F156" s="10">
         <v>8</v>
       </c>
@@ -5592,7 +5592,7 @@
       <c r="D157" s="10">
         <v>150</v>
       </c>
-      <c r="E157" s="38"/>
+      <c r="E157" s="43"/>
       <c r="F157" s="10">
         <v>8</v>
       </c>
@@ -5610,7 +5610,7 @@
       <c r="D158" s="10">
         <v>151</v>
       </c>
-      <c r="E158" s="38"/>
+      <c r="E158" s="43"/>
       <c r="F158" s="10">
         <v>8</v>
       </c>
@@ -5628,7 +5628,7 @@
       <c r="D159" s="10">
         <v>152</v>
       </c>
-      <c r="E159" s="39"/>
+      <c r="E159" s="44"/>
       <c r="F159" s="10">
         <v>8</v>
       </c>
@@ -5644,7 +5644,7 @@
       <c r="D160" s="25">
         <v>204</v>
       </c>
-      <c r="E160" s="37">
+      <c r="E160" s="48">
         <v>10157</v>
       </c>
       <c r="F160" s="25">
@@ -5662,7 +5662,7 @@
       <c r="D161" s="25">
         <v>205</v>
       </c>
-      <c r="E161" s="38"/>
+      <c r="E161" s="43"/>
       <c r="F161" s="25">
         <v>8</v>
       </c>
@@ -5678,7 +5678,7 @@
       <c r="D162" s="25">
         <v>206</v>
       </c>
-      <c r="E162" s="38"/>
+      <c r="E162" s="43"/>
       <c r="F162" s="25">
         <v>8</v>
       </c>
@@ -5694,7 +5694,7 @@
       <c r="D163" s="25">
         <v>207</v>
       </c>
-      <c r="E163" s="38"/>
+      <c r="E163" s="43"/>
       <c r="F163" s="25">
         <v>8</v>
       </c>
@@ -5710,7 +5710,7 @@
       <c r="D164" s="25">
         <v>208</v>
       </c>
-      <c r="E164" s="39"/>
+      <c r="E164" s="44"/>
       <c r="F164" s="25">
         <v>8</v>
       </c>
@@ -5728,7 +5728,7 @@
       <c r="D165" s="10">
         <v>153</v>
       </c>
-      <c r="E165" s="43">
+      <c r="E165" s="42">
         <v>10162</v>
       </c>
       <c r="F165" s="10">
@@ -5748,7 +5748,7 @@
       <c r="D166" s="10">
         <v>154</v>
       </c>
-      <c r="E166" s="38"/>
+      <c r="E166" s="43"/>
       <c r="F166" s="10">
         <v>9</v>
       </c>
@@ -5766,7 +5766,7 @@
       <c r="D167" s="10">
         <v>155</v>
       </c>
-      <c r="E167" s="38"/>
+      <c r="E167" s="43"/>
       <c r="F167" s="10">
         <v>9</v>
       </c>
@@ -5784,7 +5784,7 @@
       <c r="D168" s="10">
         <v>156</v>
       </c>
-      <c r="E168" s="38"/>
+      <c r="E168" s="43"/>
       <c r="F168" s="10">
         <v>9</v>
       </c>
@@ -5802,7 +5802,7 @@
       <c r="D169" s="10">
         <v>157</v>
       </c>
-      <c r="E169" s="38"/>
+      <c r="E169" s="43"/>
       <c r="F169" s="10">
         <v>9</v>
       </c>
@@ -5820,7 +5820,7 @@
       <c r="D170" s="10">
         <v>158</v>
       </c>
-      <c r="E170" s="39"/>
+      <c r="E170" s="44"/>
       <c r="F170" s="10">
         <v>9</v>
       </c>
@@ -5838,7 +5838,7 @@
       <c r="D171" s="10">
         <v>159</v>
       </c>
-      <c r="E171" s="43">
+      <c r="E171" s="42">
         <v>10168</v>
       </c>
       <c r="F171" s="10">
@@ -5858,7 +5858,7 @@
       <c r="D172" s="10">
         <v>160</v>
       </c>
-      <c r="E172" s="38"/>
+      <c r="E172" s="43"/>
       <c r="F172" s="10">
         <v>9</v>
       </c>
@@ -5876,7 +5876,7 @@
       <c r="D173" s="10">
         <v>161</v>
       </c>
-      <c r="E173" s="38"/>
+      <c r="E173" s="43"/>
       <c r="F173" s="10">
         <v>9</v>
       </c>
@@ -5894,7 +5894,7 @@
       <c r="D174" s="10">
         <v>162</v>
       </c>
-      <c r="E174" s="38"/>
+      <c r="E174" s="43"/>
       <c r="F174" s="10">
         <v>9</v>
       </c>
@@ -5912,7 +5912,7 @@
       <c r="D175" s="10">
         <v>163</v>
       </c>
-      <c r="E175" s="38"/>
+      <c r="E175" s="43"/>
       <c r="F175" s="10">
         <v>9</v>
       </c>
@@ -5930,7 +5930,7 @@
       <c r="D176" s="10">
         <v>164</v>
       </c>
-      <c r="E176" s="39"/>
+      <c r="E176" s="44"/>
       <c r="F176" s="10">
         <v>9</v>
       </c>
@@ -5948,7 +5948,7 @@
       <c r="D177" s="10">
         <v>165</v>
       </c>
-      <c r="E177" s="43">
+      <c r="E177" s="42">
         <v>10174</v>
       </c>
       <c r="F177" s="10">
@@ -5968,7 +5968,7 @@
       <c r="D178" s="10">
         <v>166</v>
       </c>
-      <c r="E178" s="38"/>
+      <c r="E178" s="43"/>
       <c r="F178" s="10">
         <v>9</v>
       </c>
@@ -5986,7 +5986,7 @@
       <c r="D179" s="10">
         <v>167</v>
       </c>
-      <c r="E179" s="38"/>
+      <c r="E179" s="43"/>
       <c r="F179" s="10">
         <v>9</v>
       </c>
@@ -6004,7 +6004,7 @@
       <c r="D180" s="10">
         <v>168</v>
       </c>
-      <c r="E180" s="38"/>
+      <c r="E180" s="43"/>
       <c r="F180" s="10">
         <v>9</v>
       </c>
@@ -6022,7 +6022,7 @@
       <c r="D181" s="10">
         <v>169</v>
       </c>
-      <c r="E181" s="38"/>
+      <c r="E181" s="43"/>
       <c r="F181" s="10">
         <v>9</v>
       </c>
@@ -6040,7 +6040,7 @@
       <c r="D182" s="10">
         <v>170</v>
       </c>
-      <c r="E182" s="39"/>
+      <c r="E182" s="44"/>
       <c r="F182" s="10">
         <v>9</v>
       </c>
@@ -6056,7 +6056,7 @@
       <c r="D183" s="25">
         <v>209</v>
       </c>
-      <c r="E183" s="37">
+      <c r="E183" s="48">
         <v>10175</v>
       </c>
       <c r="F183" s="25">
@@ -6074,7 +6074,7 @@
       <c r="D184" s="25">
         <v>210</v>
       </c>
-      <c r="E184" s="38"/>
+      <c r="E184" s="43"/>
       <c r="F184" s="25">
         <v>9</v>
       </c>
@@ -6090,7 +6090,7 @@
       <c r="D185" s="25">
         <v>211</v>
       </c>
-      <c r="E185" s="38"/>
+      <c r="E185" s="43"/>
       <c r="F185" s="25">
         <v>9</v>
       </c>
@@ -6106,7 +6106,7 @@
       <c r="D186" s="25">
         <v>212</v>
       </c>
-      <c r="E186" s="38"/>
+      <c r="E186" s="43"/>
       <c r="F186" s="25">
         <v>9</v>
       </c>
@@ -6122,7 +6122,7 @@
       <c r="D187" s="25">
         <v>213</v>
       </c>
-      <c r="E187" s="39"/>
+      <c r="E187" s="44"/>
       <c r="F187" s="25">
         <v>9</v>
       </c>
@@ -6140,7 +6140,7 @@
       <c r="D188" s="10">
         <v>171</v>
       </c>
-      <c r="E188" s="40">
+      <c r="E188" s="49">
         <v>10180</v>
       </c>
       <c r="F188" s="10">
@@ -6160,7 +6160,7 @@
       <c r="D189" s="10">
         <v>172</v>
       </c>
-      <c r="E189" s="41"/>
+      <c r="E189" s="50"/>
       <c r="F189" s="10">
         <v>10</v>
       </c>
@@ -6178,7 +6178,7 @@
       <c r="D190" s="10">
         <v>173</v>
       </c>
-      <c r="E190" s="41"/>
+      <c r="E190" s="50"/>
       <c r="F190" s="10">
         <v>10</v>
       </c>
@@ -6196,7 +6196,7 @@
       <c r="D191" s="10">
         <v>174</v>
       </c>
-      <c r="E191" s="41"/>
+      <c r="E191" s="50"/>
       <c r="F191" s="10">
         <v>10</v>
       </c>
@@ -6214,7 +6214,7 @@
       <c r="D192" s="10">
         <v>175</v>
       </c>
-      <c r="E192" s="41"/>
+      <c r="E192" s="50"/>
       <c r="F192" s="10">
         <v>10</v>
       </c>
@@ -6232,7 +6232,7 @@
       <c r="D193" s="10">
         <v>176</v>
       </c>
-      <c r="E193" s="42"/>
+      <c r="E193" s="51"/>
       <c r="F193" s="10">
         <v>10</v>
       </c>
@@ -6248,7 +6248,7 @@
       <c r="D194" s="25">
         <v>214</v>
       </c>
-      <c r="E194" s="37">
+      <c r="E194" s="48">
         <v>10179</v>
       </c>
       <c r="F194" s="25">
@@ -6266,7 +6266,7 @@
       <c r="D195" s="25">
         <v>215</v>
       </c>
-      <c r="E195" s="38"/>
+      <c r="E195" s="43"/>
       <c r="F195" s="25">
         <v>10</v>
       </c>
@@ -6282,7 +6282,7 @@
       <c r="D196" s="25">
         <v>216</v>
       </c>
-      <c r="E196" s="38"/>
+      <c r="E196" s="43"/>
       <c r="F196" s="25">
         <v>10</v>
       </c>
@@ -6298,7 +6298,7 @@
       <c r="D197" s="25">
         <v>217</v>
       </c>
-      <c r="E197" s="38"/>
+      <c r="E197" s="43"/>
       <c r="F197" s="25">
         <v>10</v>
       </c>
@@ -6314,7 +6314,7 @@
       <c r="D198" s="25">
         <v>218</v>
       </c>
-      <c r="E198" s="39"/>
+      <c r="E198" s="44"/>
       <c r="F198" s="25">
         <v>10</v>
       </c>
@@ -6332,7 +6332,7 @@
       <c r="D199" s="10">
         <v>177</v>
       </c>
-      <c r="E199" s="43">
+      <c r="E199" s="42">
         <v>10181</v>
       </c>
       <c r="F199" s="10">
@@ -6352,7 +6352,7 @@
       <c r="D200" s="10">
         <v>178</v>
       </c>
-      <c r="E200" s="44"/>
+      <c r="E200" s="52"/>
       <c r="F200" s="10">
         <v>11</v>
       </c>
@@ -6370,7 +6370,7 @@
       <c r="D201" s="10">
         <v>179</v>
       </c>
-      <c r="E201" s="44"/>
+      <c r="E201" s="52"/>
       <c r="F201" s="10">
         <v>11</v>
       </c>
@@ -6388,7 +6388,7 @@
       <c r="D202" s="10">
         <v>180</v>
       </c>
-      <c r="E202" s="44"/>
+      <c r="E202" s="52"/>
       <c r="F202" s="10">
         <v>11</v>
       </c>
@@ -6406,7 +6406,7 @@
       <c r="D203" s="10">
         <v>181</v>
       </c>
-      <c r="E203" s="44"/>
+      <c r="E203" s="52"/>
       <c r="F203" s="10">
         <v>11</v>
       </c>
@@ -6424,7 +6424,7 @@
       <c r="D204" s="10">
         <v>182</v>
       </c>
-      <c r="E204" s="45"/>
+      <c r="E204" s="53"/>
       <c r="F204" s="10">
         <v>11</v>
       </c>
@@ -6442,7 +6442,7 @@
       <c r="D205" s="10">
         <v>183</v>
       </c>
-      <c r="E205" s="43">
+      <c r="E205" s="42">
         <v>10182</v>
       </c>
       <c r="F205" s="10">
@@ -6462,7 +6462,7 @@
       <c r="D206" s="10">
         <v>184</v>
       </c>
-      <c r="E206" s="44"/>
+      <c r="E206" s="52"/>
       <c r="F206" s="10">
         <v>11</v>
       </c>
@@ -6480,7 +6480,7 @@
       <c r="D207" s="10">
         <v>185</v>
       </c>
-      <c r="E207" s="44"/>
+      <c r="E207" s="52"/>
       <c r="F207" s="10">
         <v>11</v>
       </c>
@@ -6498,7 +6498,7 @@
       <c r="D208" s="10">
         <v>186</v>
       </c>
-      <c r="E208" s="44"/>
+      <c r="E208" s="52"/>
       <c r="F208" s="10">
         <v>11</v>
       </c>
@@ -6516,7 +6516,7 @@
       <c r="D209" s="10">
         <v>187</v>
       </c>
-      <c r="E209" s="45"/>
+      <c r="E209" s="53"/>
       <c r="F209" s="10">
         <v>11</v>
       </c>
@@ -6534,7 +6534,7 @@
       <c r="D210" s="10">
         <v>188</v>
       </c>
-      <c r="E210" s="43">
+      <c r="E210" s="42">
         <v>10197</v>
       </c>
       <c r="F210" s="10">
@@ -6554,7 +6554,7 @@
       <c r="D211" s="10">
         <v>189</v>
       </c>
-      <c r="E211" s="38"/>
+      <c r="E211" s="43"/>
       <c r="F211" s="10">
         <v>11</v>
       </c>
@@ -6572,7 +6572,7 @@
       <c r="D212" s="10">
         <v>190</v>
       </c>
-      <c r="E212" s="38"/>
+      <c r="E212" s="43"/>
       <c r="F212" s="10">
         <v>11</v>
       </c>
@@ -6590,7 +6590,7 @@
       <c r="D213" s="10">
         <v>191</v>
       </c>
-      <c r="E213" s="38"/>
+      <c r="E213" s="43"/>
       <c r="F213" s="10">
         <v>11</v>
       </c>
@@ -6608,7 +6608,7 @@
       <c r="D214" s="10">
         <v>192</v>
       </c>
-      <c r="E214" s="39"/>
+      <c r="E214" s="44"/>
       <c r="F214" s="10">
         <v>11</v>
       </c>
@@ -6626,7 +6626,7 @@
       <c r="D215" s="10">
         <v>193</v>
       </c>
-      <c r="E215" s="43">
+      <c r="E215" s="42">
         <v>10202</v>
       </c>
       <c r="F215" s="10">
@@ -6646,7 +6646,7 @@
       <c r="D216" s="10">
         <v>194</v>
       </c>
-      <c r="E216" s="38"/>
+      <c r="E216" s="43"/>
       <c r="F216" s="10">
         <v>11</v>
       </c>
@@ -6664,7 +6664,7 @@
       <c r="D217" s="10">
         <v>195</v>
       </c>
-      <c r="E217" s="38"/>
+      <c r="E217" s="43"/>
       <c r="F217" s="10">
         <v>11</v>
       </c>
@@ -6682,7 +6682,7 @@
       <c r="D218" s="10">
         <v>196</v>
       </c>
-      <c r="E218" s="38"/>
+      <c r="E218" s="43"/>
       <c r="F218" s="10">
         <v>11</v>
       </c>
@@ -6700,7 +6700,7 @@
       <c r="D219" s="10">
         <v>197</v>
       </c>
-      <c r="E219" s="38"/>
+      <c r="E219" s="43"/>
       <c r="F219" s="10">
         <v>11</v>
       </c>
@@ -6718,7 +6718,7 @@
       <c r="D220" s="10">
         <v>198</v>
       </c>
-      <c r="E220" s="39"/>
+      <c r="E220" s="44"/>
       <c r="F220" s="10">
         <v>11</v>
       </c>
@@ -6727,202 +6727,202 @@
       </c>
     </row>
     <row r="221" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B221" s="48" t="s">
+      <c r="B221" s="37" t="s">
         <v>666</v>
       </c>
-      <c r="C221" s="49"/>
-      <c r="D221" s="50">
+      <c r="C221" s="38"/>
+      <c r="D221" s="39">
         <v>219</v>
       </c>
-      <c r="E221" s="51">
+      <c r="E221" s="45">
         <v>10210</v>
       </c>
-      <c r="F221" s="50" t="s">
+      <c r="F221" s="39" t="s">
         <v>690</v>
       </c>
-      <c r="G221" s="50" t="s">
+      <c r="G221" s="39" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="222" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B222" s="48" t="s">
+      <c r="B222" s="37" t="s">
         <v>668</v>
       </c>
-      <c r="C222" s="49"/>
-      <c r="D222" s="50">
+      <c r="C222" s="38"/>
+      <c r="D222" s="39">
         <v>220</v>
       </c>
-      <c r="E222" s="52"/>
-      <c r="F222" s="50" t="s">
+      <c r="E222" s="46"/>
+      <c r="F222" s="39" t="s">
         <v>690</v>
       </c>
-      <c r="G222" s="50" t="s">
+      <c r="G222" s="39" t="s">
         <v>682</v>
       </c>
     </row>
     <row r="223" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B223" s="48" t="s">
+      <c r="B223" s="37" t="s">
         <v>669</v>
       </c>
-      <c r="C223" s="49"/>
-      <c r="D223" s="50">
+      <c r="C223" s="38"/>
+      <c r="D223" s="39">
         <v>221</v>
       </c>
-      <c r="E223" s="52"/>
-      <c r="F223" s="50" t="s">
+      <c r="E223" s="46"/>
+      <c r="F223" s="39" t="s">
         <v>690</v>
       </c>
-      <c r="G223" s="50" t="s">
+      <c r="G223" s="39" t="s">
         <v>683</v>
       </c>
     </row>
     <row r="224" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B224" s="48" t="s">
+      <c r="B224" s="37" t="s">
         <v>670</v>
       </c>
-      <c r="C224" s="49"/>
-      <c r="D224" s="50">
+      <c r="C224" s="38"/>
+      <c r="D224" s="39">
         <v>222</v>
       </c>
-      <c r="E224" s="52"/>
-      <c r="F224" s="50" t="s">
+      <c r="E224" s="46"/>
+      <c r="F224" s="39" t="s">
         <v>690</v>
       </c>
-      <c r="G224" s="50" t="s">
+      <c r="G224" s="39" t="s">
         <v>684</v>
       </c>
     </row>
     <row r="225" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B225" s="48" t="s">
+      <c r="B225" s="37" t="s">
         <v>671</v>
       </c>
-      <c r="C225" s="49"/>
-      <c r="D225" s="50">
+      <c r="C225" s="38"/>
+      <c r="D225" s="39">
         <v>223</v>
       </c>
-      <c r="E225" s="53"/>
-      <c r="F225" s="50" t="s">
+      <c r="E225" s="47"/>
+      <c r="F225" s="39" t="s">
         <v>690</v>
       </c>
-      <c r="G225" s="50" t="s">
+      <c r="G225" s="39" t="s">
         <v>685</v>
       </c>
     </row>
     <row r="226" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B226" s="48" t="s">
+      <c r="B226" s="37" t="s">
         <v>667</v>
       </c>
-      <c r="C226" s="49"/>
-      <c r="D226" s="50">
+      <c r="C226" s="38"/>
+      <c r="D226" s="39">
         <v>224</v>
       </c>
-      <c r="E226" s="51">
+      <c r="E226" s="45">
         <v>10211</v>
       </c>
-      <c r="F226" s="50" t="s">
+      <c r="F226" s="39" t="s">
         <v>690</v>
       </c>
-      <c r="G226" s="50" t="s">
+      <c r="G226" s="39" t="s">
         <v>673</v>
       </c>
     </row>
     <row r="227" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B227" s="48" t="s">
+      <c r="B227" s="37" t="s">
         <v>674</v>
       </c>
-      <c r="C227" s="49"/>
-      <c r="D227" s="50">
+      <c r="C227" s="38"/>
+      <c r="D227" s="39">
         <v>225</v>
       </c>
-      <c r="E227" s="52"/>
-      <c r="F227" s="50" t="s">
+      <c r="E227" s="46"/>
+      <c r="F227" s="39" t="s">
         <v>690</v>
       </c>
-      <c r="G227" s="50" t="s">
+      <c r="G227" s="39" t="s">
         <v>672</v>
       </c>
     </row>
     <row r="228" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B228" s="48" t="s">
+      <c r="B228" s="37" t="s">
         <v>675</v>
       </c>
-      <c r="C228" s="49"/>
-      <c r="D228" s="50">
+      <c r="C228" s="38"/>
+      <c r="D228" s="39">
         <v>226</v>
       </c>
-      <c r="E228" s="52"/>
-      <c r="F228" s="50" t="s">
+      <c r="E228" s="46"/>
+      <c r="F228" s="39" t="s">
         <v>690</v>
       </c>
-      <c r="G228" s="50" t="s">
+      <c r="G228" s="39" t="s">
         <v>678</v>
       </c>
     </row>
     <row r="229" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B229" s="48" t="s">
+      <c r="B229" s="37" t="s">
         <v>676</v>
       </c>
-      <c r="C229" s="49"/>
-      <c r="D229" s="50">
+      <c r="C229" s="38"/>
+      <c r="D229" s="39">
         <v>227</v>
       </c>
-      <c r="E229" s="52"/>
-      <c r="F229" s="50" t="s">
+      <c r="E229" s="46"/>
+      <c r="F229" s="39" t="s">
         <v>690</v>
       </c>
-      <c r="G229" s="50" t="s">
+      <c r="G229" s="39" t="s">
         <v>679</v>
       </c>
     </row>
     <row r="230" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B230" s="48" t="s">
+      <c r="B230" s="37" t="s">
         <v>677</v>
       </c>
-      <c r="C230" s="49"/>
-      <c r="D230" s="50">
+      <c r="C230" s="38"/>
+      <c r="D230" s="39">
         <v>228</v>
       </c>
-      <c r="E230" s="53"/>
-      <c r="F230" s="50" t="s">
+      <c r="E230" s="47"/>
+      <c r="F230" s="39" t="s">
         <v>690</v>
       </c>
-      <c r="G230" s="50" t="s">
+      <c r="G230" s="39" t="s">
         <v>680</v>
       </c>
     </row>
     <row r="231" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B231" s="48" t="s">
+      <c r="B231" s="37" t="s">
         <v>687</v>
       </c>
-      <c r="C231" s="49"/>
-      <c r="D231" s="50">
-        <v>219</v>
-      </c>
-      <c r="E231" s="55">
+      <c r="C231" s="38"/>
+      <c r="D231" s="39">
+        <v>229</v>
+      </c>
+      <c r="E231" s="41">
         <v>10212</v>
       </c>
-      <c r="F231" s="50" t="s">
+      <c r="F231" s="39" t="s">
         <v>690</v>
       </c>
-      <c r="G231" s="50" t="s">
+      <c r="G231" s="39" t="s">
         <v>686</v>
       </c>
     </row>
     <row r="232" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B232" s="48" t="s">
+      <c r="B232" s="37" t="s">
         <v>688</v>
       </c>
-      <c r="C232" s="49"/>
-      <c r="D232" s="50">
-        <v>219</v>
-      </c>
-      <c r="E232" s="55">
+      <c r="C232" s="38"/>
+      <c r="D232" s="39">
+        <v>230</v>
+      </c>
+      <c r="E232" s="41">
         <v>10213</v>
       </c>
-      <c r="F232" s="50" t="s">
+      <c r="F232" s="39" t="s">
         <v>690</v>
       </c>
-      <c r="G232" s="50" t="s">
+      <c r="G232" s="39" t="s">
         <v>689</v>
       </c>
     </row>
@@ -6950,20 +6950,26 @@
     </row>
     <row r="240" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="241" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B241" s="54" t="s">
+      <c r="B241" s="40" t="s">
         <v>665</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E215:E220"/>
-    <mergeCell ref="E221:E225"/>
-    <mergeCell ref="E226:E230"/>
-    <mergeCell ref="E160:E164"/>
-    <mergeCell ref="E188:E193"/>
-    <mergeCell ref="E199:E204"/>
-    <mergeCell ref="E205:E209"/>
-    <mergeCell ref="E210:E214"/>
+    <mergeCell ref="E106:E109"/>
+    <mergeCell ref="E99:E104"/>
+    <mergeCell ref="E33:E38"/>
+    <mergeCell ref="E39:E44"/>
+    <mergeCell ref="E45:E49"/>
+    <mergeCell ref="E50:E54"/>
+    <mergeCell ref="E55:E60"/>
+    <mergeCell ref="E64:E69"/>
+    <mergeCell ref="E70:E74"/>
+    <mergeCell ref="E3:E8"/>
+    <mergeCell ref="E9:E14"/>
+    <mergeCell ref="E15:E20"/>
+    <mergeCell ref="E21:E26"/>
+    <mergeCell ref="E27:E32"/>
     <mergeCell ref="E75:E79"/>
     <mergeCell ref="E80:E84"/>
     <mergeCell ref="E88:E93"/>
@@ -6980,25 +6986,19 @@
     <mergeCell ref="E165:E170"/>
     <mergeCell ref="E171:E176"/>
     <mergeCell ref="E141:E145"/>
+    <mergeCell ref="E215:E220"/>
+    <mergeCell ref="E221:E225"/>
+    <mergeCell ref="E226:E230"/>
+    <mergeCell ref="E160:E164"/>
+    <mergeCell ref="E188:E193"/>
+    <mergeCell ref="E199:E204"/>
+    <mergeCell ref="E205:E209"/>
+    <mergeCell ref="E210:E214"/>
     <mergeCell ref="E183:E187"/>
     <mergeCell ref="E194:E198"/>
-    <mergeCell ref="E3:E8"/>
-    <mergeCell ref="E9:E14"/>
-    <mergeCell ref="E15:E20"/>
-    <mergeCell ref="E21:E26"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="E106:E109"/>
-    <mergeCell ref="E99:E104"/>
-    <mergeCell ref="E33:E38"/>
-    <mergeCell ref="E39:E44"/>
-    <mergeCell ref="E45:E49"/>
-    <mergeCell ref="E50:E54"/>
-    <mergeCell ref="E55:E60"/>
-    <mergeCell ref="E64:E69"/>
-    <mergeCell ref="E70:E74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7082,7 +7082,7 @@
       <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="55" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="6" t="s">
@@ -7105,7 +7105,7 @@
       <c r="C5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="47"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="6" t="s">
         <v>20</v>
       </c>
@@ -7126,7 +7126,7 @@
       <c r="C6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="47"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="6" t="s">
         <v>25</v>
       </c>
@@ -7147,7 +7147,7 @@
       <c r="C7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="47"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="6" t="s">
         <v>30</v>
       </c>
@@ -7168,7 +7168,7 @@
       <c r="C8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="47"/>
+      <c r="D8" s="55"/>
       <c r="E8" s="6" t="s">
         <v>35</v>
       </c>
@@ -7189,7 +7189,7 @@
       <c r="C9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="47" t="s">
+      <c r="D9" s="55" t="s">
         <v>40</v>
       </c>
       <c r="E9" s="6" t="s">
@@ -7212,7 +7212,7 @@
       <c r="C10" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="47"/>
+      <c r="D10" s="55"/>
       <c r="E10" s="6" t="s">
         <v>46</v>
       </c>
@@ -7233,7 +7233,7 @@
       <c r="C11" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="47"/>
+      <c r="D11" s="55"/>
       <c r="E11" s="6" t="s">
         <v>51</v>
       </c>
@@ -7254,7 +7254,7 @@
       <c r="C12" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="47"/>
+      <c r="D12" s="55"/>
       <c r="E12" s="6" t="s">
         <v>55</v>
       </c>
@@ -7275,7 +7275,7 @@
       <c r="C13" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="47"/>
+      <c r="D13" s="55"/>
       <c r="E13" s="6" t="s">
         <v>48</v>
       </c>
@@ -7296,7 +7296,7 @@
       <c r="C14" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="47"/>
+      <c r="D14" s="55"/>
       <c r="E14" s="6" t="s">
         <v>48</v>
       </c>
@@ -7317,7 +7317,7 @@
       <c r="C15" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="47"/>
+      <c r="D15" s="55"/>
       <c r="E15" s="6" t="s">
         <v>48</v>
       </c>
@@ -7338,7 +7338,7 @@
       <c r="C16" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="47" t="s">
+      <c r="D16" s="55" t="s">
         <v>66</v>
       </c>
       <c r="E16" s="6" t="s">
@@ -7361,7 +7361,7 @@
       <c r="C17" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="47"/>
+      <c r="D17" s="55"/>
       <c r="E17" s="6" t="s">
         <v>72</v>
       </c>
@@ -7382,7 +7382,7 @@
       <c r="C18" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="47"/>
+      <c r="D18" s="55"/>
       <c r="E18" s="6" t="s">
         <v>76</v>
       </c>
@@ -7403,7 +7403,7 @@
       <c r="C19" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="47"/>
+      <c r="D19" s="55"/>
       <c r="E19" s="6" t="s">
         <v>80</v>
       </c>
@@ -7424,7 +7424,7 @@
       <c r="C20" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="47"/>
+      <c r="D20" s="55"/>
       <c r="E20" s="6" t="s">
         <v>48</v>
       </c>
@@ -7445,7 +7445,7 @@
       <c r="C21" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="47"/>
+      <c r="D21" s="55"/>
       <c r="E21" s="6" t="s">
         <v>48</v>
       </c>
@@ -7466,7 +7466,7 @@
       <c r="C22" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="47"/>
+      <c r="D22" s="55"/>
       <c r="E22" s="6" t="s">
         <v>48</v>
       </c>
@@ -7487,7 +7487,7 @@
       <c r="C23" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="47" t="s">
+      <c r="D23" s="55" t="s">
         <v>90</v>
       </c>
       <c r="E23" s="6" t="s">
@@ -7510,7 +7510,7 @@
       <c r="C24" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="47"/>
+      <c r="D24" s="55"/>
       <c r="E24" s="6" t="s">
         <v>96</v>
       </c>
@@ -7531,7 +7531,7 @@
       <c r="C25" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="47"/>
+      <c r="D25" s="55"/>
       <c r="E25" s="6" t="s">
         <v>100</v>
       </c>
@@ -7552,7 +7552,7 @@
       <c r="C26" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="47"/>
+      <c r="D26" s="55"/>
       <c r="E26" s="6" t="s">
         <v>48</v>
       </c>
@@ -7573,7 +7573,7 @@
       <c r="C27" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D27" s="46" t="s">
+      <c r="D27" s="54" t="s">
         <v>107</v>
       </c>
       <c r="E27" s="6" t="s">
@@ -7596,7 +7596,7 @@
       <c r="C28" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D28" s="47"/>
+      <c r="D28" s="55"/>
       <c r="E28" s="6" t="s">
         <v>112</v>
       </c>
@@ -7617,7 +7617,7 @@
       <c r="C29" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="D29" s="47"/>
+      <c r="D29" s="55"/>
       <c r="E29" s="6" t="s">
         <v>116</v>
       </c>
@@ -7638,7 +7638,7 @@
       <c r="C30" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D30" s="47"/>
+      <c r="D30" s="55"/>
       <c r="E30" s="6" t="s">
         <v>120</v>
       </c>
@@ -7659,7 +7659,7 @@
       <c r="C31" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D31" s="47"/>
+      <c r="D31" s="55"/>
       <c r="E31" s="6" t="s">
         <v>125</v>
       </c>
@@ -7680,7 +7680,7 @@
       <c r="C32" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="D32" s="47"/>
+      <c r="D32" s="55"/>
       <c r="E32" s="6" t="s">
         <v>130</v>
       </c>
@@ -7701,7 +7701,7 @@
       <c r="C33" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="D33" s="47"/>
+      <c r="D33" s="55"/>
       <c r="E33" s="6" t="s">
         <v>135</v>
       </c>
@@ -7722,7 +7722,7 @@
       <c r="C34" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D34" s="47"/>
+      <c r="D34" s="55"/>
       <c r="E34" s="6" t="s">
         <v>140</v>
       </c>
@@ -7743,7 +7743,7 @@
       <c r="C35" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D35" s="47"/>
+      <c r="D35" s="55"/>
       <c r="E35" s="6" t="s">
         <v>145</v>
       </c>
@@ -7764,7 +7764,7 @@
       <c r="C36" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D36" s="47"/>
+      <c r="D36" s="55"/>
       <c r="E36" s="6" t="s">
         <v>150</v>
       </c>
@@ -7785,7 +7785,7 @@
       <c r="C37" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D37" s="47"/>
+      <c r="D37" s="55"/>
       <c r="E37" s="6" t="s">
         <v>151</v>
       </c>
@@ -7806,7 +7806,7 @@
       <c r="C38" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="D38" s="46" t="s">
+      <c r="D38" s="54" t="s">
         <v>153</v>
       </c>
       <c r="E38" s="6" t="s">
@@ -7829,7 +7829,7 @@
       <c r="C39" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D39" s="47"/>
+      <c r="D39" s="55"/>
       <c r="E39" s="6" t="s">
         <v>159</v>
       </c>
@@ -7850,7 +7850,7 @@
       <c r="C40" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="D40" s="47"/>
+      <c r="D40" s="55"/>
       <c r="E40" s="6" t="s">
         <v>164</v>
       </c>
@@ -7871,7 +7871,7 @@
       <c r="C41" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D41" s="47"/>
+      <c r="D41" s="55"/>
       <c r="E41" s="6" t="s">
         <v>168</v>
       </c>
@@ -7892,7 +7892,7 @@
       <c r="C42" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="D42" s="46" t="s">
+      <c r="D42" s="54" t="s">
         <v>172</v>
       </c>
       <c r="E42" s="6" t="s">
@@ -7915,7 +7915,7 @@
       <c r="C43" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D43" s="47"/>
+      <c r="D43" s="55"/>
       <c r="E43" s="6" t="s">
         <v>178</v>
       </c>
@@ -7936,7 +7936,7 @@
       <c r="C44" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D44" s="47"/>
+      <c r="D44" s="55"/>
       <c r="E44" s="6" t="s">
         <v>182</v>
       </c>
@@ -7957,7 +7957,7 @@
       <c r="C45" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D45" s="47"/>
+      <c r="D45" s="55"/>
       <c r="E45" s="7" t="s">
         <v>186</v>
       </c>

</xml_diff>